<commit_message>
ARCHIVO 14 JUN 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #06  JUNIO 2022/ENTRADAS OBRADOR     J U N I O         2022.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #06  JUNIO 2022/ENTRADAS OBRADOR     J U N I O         2022.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16365" windowHeight="10305" firstSheet="4" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16365" windowHeight="10305" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="CANALES  ENERO  2022   " sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1488" uniqueCount="513">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1520" uniqueCount="514">
   <si>
     <t>FECHA DE PAGO</t>
   </si>
@@ -1582,6 +1582,9 @@
   </si>
   <si>
     <t>20598--4806</t>
+  </si>
+  <si>
+    <t>P-1</t>
   </si>
 </sst>
 </file>
@@ -4329,78 +4332,7 @@
     <xf numFmtId="1" fontId="12" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="31" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="31" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="11" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="11" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="26" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="26" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4434,11 +4366,83 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="11" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="11" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="22" fillId="11" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="22" fillId="11" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="26" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="26" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="31" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="31" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -4468,12 +4472,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="32" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="32" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4509,6 +4507,12 @@
     <xf numFmtId="1" fontId="18" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="4" fontId="32" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="32" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="1" fontId="11" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4527,7 +4531,6 @@
     <xf numFmtId="164" fontId="12" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -4857,18 +4860,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="42.75" thickBot="1" x14ac:dyDescent="0.7">
-      <c r="A1" s="537" t="s">
+      <c r="A1" s="514" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="537"/>
-      <c r="C1" s="537"/>
-      <c r="D1" s="537"/>
-      <c r="E1" s="537"/>
-      <c r="F1" s="537"/>
-      <c r="G1" s="537"/>
-      <c r="H1" s="537"/>
-      <c r="I1" s="537"/>
-      <c r="J1" s="537"/>
+      <c r="B1" s="514"/>
+      <c r="C1" s="514"/>
+      <c r="D1" s="514"/>
+      <c r="E1" s="514"/>
+      <c r="F1" s="514"/>
+      <c r="G1" s="514"/>
+      <c r="H1" s="514"/>
+      <c r="I1" s="514"/>
+      <c r="J1" s="514"/>
       <c r="K1" s="375"/>
       <c r="L1" s="375"/>
       <c r="M1" s="375"/>
@@ -4882,22 +4885,22 @@
       <c r="V1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="W1" s="538" t="s">
+      <c r="W1" s="515" t="s">
         <v>2</v>
       </c>
-      <c r="X1" s="539"/>
+      <c r="X1" s="516"/>
     </row>
     <row r="2" spans="1:24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="537"/>
-      <c r="B2" s="537"/>
-      <c r="C2" s="537"/>
-      <c r="D2" s="537"/>
-      <c r="E2" s="537"/>
-      <c r="F2" s="537"/>
-      <c r="G2" s="537"/>
-      <c r="H2" s="537"/>
-      <c r="I2" s="537"/>
-      <c r="J2" s="537"/>
+      <c r="A2" s="514"/>
+      <c r="B2" s="514"/>
+      <c r="C2" s="514"/>
+      <c r="D2" s="514"/>
+      <c r="E2" s="514"/>
+      <c r="F2" s="514"/>
+      <c r="G2" s="514"/>
+      <c r="H2" s="514"/>
+      <c r="I2" s="514"/>
+      <c r="J2" s="514"/>
       <c r="K2" s="377"/>
       <c r="L2" s="377"/>
       <c r="M2" s="377"/>
@@ -4951,10 +4954,10 @@
       <c r="N3" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="540" t="s">
+      <c r="O3" s="517" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="541"/>
+      <c r="P3" s="518"/>
       <c r="Q3" s="30" t="s">
         <v>16</v>
       </c>
@@ -5498,7 +5501,7 @@
       <c r="B12" s="58" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="542" t="s">
+      <c r="C12" s="519" t="s">
         <v>103</v>
       </c>
       <c r="D12" s="400"/>
@@ -5562,7 +5565,7 @@
       <c r="B13" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="543"/>
+      <c r="C13" s="520"/>
       <c r="D13" s="400"/>
       <c r="E13" s="401"/>
       <c r="F13" s="402">
@@ -7564,13 +7567,13 @@
       <c r="V55" s="160"/>
     </row>
     <row r="56" spans="1:24" s="161" customFormat="1" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="521" t="s">
+      <c r="A56" s="531" t="s">
         <v>41</v>
       </c>
       <c r="B56" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="C56" s="523" t="s">
+      <c r="C56" s="533" t="s">
         <v>110</v>
       </c>
       <c r="D56" s="150"/>
@@ -7610,11 +7613,11 @@
       <c r="V56" s="160"/>
     </row>
     <row r="57" spans="1:24" s="161" customFormat="1" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="522"/>
+      <c r="A57" s="532"/>
       <c r="B57" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="C57" s="524"/>
+      <c r="C57" s="534"/>
       <c r="D57" s="150"/>
       <c r="E57" s="40"/>
       <c r="F57" s="151">
@@ -7650,13 +7653,13 @@
       <c r="V57" s="160"/>
     </row>
     <row r="58" spans="1:24" s="161" customFormat="1" ht="29.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="521" t="s">
+      <c r="A58" s="531" t="s">
         <v>41</v>
       </c>
       <c r="B58" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="C58" s="523" t="s">
+      <c r="C58" s="533" t="s">
         <v>129</v>
       </c>
       <c r="D58" s="150"/>
@@ -7689,7 +7692,7 @@
       <c r="O58" s="527" t="s">
         <v>59</v>
       </c>
-      <c r="P58" s="548">
+      <c r="P58" s="529">
         <v>44606</v>
       </c>
       <c r="Q58" s="128"/>
@@ -7700,11 +7703,11 @@
       <c r="V58" s="160"/>
     </row>
     <row r="59" spans="1:24" s="161" customFormat="1" ht="29.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="522"/>
+      <c r="A59" s="532"/>
       <c r="B59" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="C59" s="524"/>
+      <c r="C59" s="534"/>
       <c r="D59" s="150"/>
       <c r="E59" s="40"/>
       <c r="F59" s="151">
@@ -7731,7 +7734,7 @@
         <v>22440</v>
       </c>
       <c r="O59" s="528"/>
-      <c r="P59" s="549"/>
+      <c r="P59" s="530"/>
       <c r="Q59" s="128"/>
       <c r="R59" s="158"/>
       <c r="S59" s="92"/>
@@ -7740,13 +7743,13 @@
       <c r="V59" s="160"/>
     </row>
     <row r="60" spans="1:24" s="161" customFormat="1" ht="48.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="546" t="s">
+      <c r="A60" s="523" t="s">
         <v>41</v>
       </c>
       <c r="B60" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="C60" s="544" t="s">
+      <c r="C60" s="521" t="s">
         <v>109</v>
       </c>
       <c r="D60" s="163"/>
@@ -7782,7 +7785,7 @@
       <c r="O60" s="527" t="s">
         <v>59</v>
       </c>
-      <c r="P60" s="548">
+      <c r="P60" s="529">
         <v>44594</v>
       </c>
       <c r="Q60" s="164"/>
@@ -7795,11 +7798,11 @@
       <c r="X60"/>
     </row>
     <row r="61" spans="1:24" ht="26.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="547"/>
+      <c r="A61" s="524"/>
       <c r="B61" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="C61" s="545"/>
+      <c r="C61" s="522"/>
       <c r="D61" s="165"/>
       <c r="E61" s="40">
         <f t="shared" si="2"/>
@@ -7829,7 +7832,7 @@
         <v>23623.200000000001</v>
       </c>
       <c r="O61" s="528"/>
-      <c r="P61" s="549"/>
+      <c r="P61" s="530"/>
       <c r="Q61" s="164"/>
       <c r="R61" s="129"/>
       <c r="S61" s="92"/>
@@ -7895,7 +7898,7 @@
       <c r="B63" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="C63" s="515"/>
+      <c r="C63" s="547"/>
       <c r="D63" s="163"/>
       <c r="E63" s="40">
         <f t="shared" si="2"/>
@@ -7903,7 +7906,7 @@
       </c>
       <c r="F63" s="151"/>
       <c r="G63" s="152"/>
-      <c r="H63" s="517"/>
+      <c r="H63" s="549"/>
       <c r="I63" s="151"/>
       <c r="J63" s="45">
         <f t="shared" si="0"/>
@@ -7932,7 +7935,7 @@
       <c r="B64" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="C64" s="516"/>
+      <c r="C64" s="548"/>
       <c r="D64" s="168"/>
       <c r="E64" s="40">
         <f t="shared" si="2"/>
@@ -7940,7 +7943,7 @@
       </c>
       <c r="F64" s="151"/>
       <c r="G64" s="152"/>
-      <c r="H64" s="518"/>
+      <c r="H64" s="550"/>
       <c r="I64" s="151"/>
       <c r="J64" s="45">
         <f t="shared" si="0"/>
@@ -8118,8 +8121,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O68" s="519"/>
-      <c r="P68" s="513"/>
+      <c r="O68" s="539"/>
+      <c r="P68" s="545"/>
       <c r="Q68" s="164"/>
       <c r="R68" s="129"/>
       <c r="S68" s="180"/>
@@ -8153,8 +8156,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O69" s="520"/>
-      <c r="P69" s="514"/>
+      <c r="O69" s="540"/>
+      <c r="P69" s="546"/>
       <c r="Q69" s="164"/>
       <c r="R69" s="129"/>
       <c r="S69" s="180"/>
@@ -8644,8 +8647,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O82" s="519"/>
-      <c r="P82" s="533"/>
+      <c r="O82" s="539"/>
+      <c r="P82" s="541"/>
       <c r="Q82" s="164"/>
       <c r="R82" s="129"/>
       <c r="S82" s="180"/>
@@ -8677,8 +8680,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O83" s="520"/>
-      <c r="P83" s="534"/>
+      <c r="O83" s="540"/>
+      <c r="P83" s="542"/>
       <c r="Q83" s="164"/>
       <c r="R83" s="129"/>
       <c r="S83" s="180"/>
@@ -8710,8 +8713,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O84" s="519"/>
-      <c r="P84" s="533"/>
+      <c r="O84" s="539"/>
+      <c r="P84" s="541"/>
       <c r="Q84" s="164"/>
       <c r="R84" s="158"/>
       <c r="S84" s="180"/>
@@ -8743,8 +8746,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O85" s="520"/>
-      <c r="P85" s="534"/>
+      <c r="O85" s="540"/>
+      <c r="P85" s="542"/>
       <c r="Q85" s="164"/>
       <c r="R85" s="158"/>
       <c r="S85" s="180"/>
@@ -8902,8 +8905,8 @@
         <v>0</v>
       </c>
       <c r="K90" s="100"/>
-      <c r="L90" s="535"/>
-      <c r="M90" s="536"/>
+      <c r="L90" s="543"/>
+      <c r="M90" s="544"/>
       <c r="N90" s="77">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -8935,8 +8938,8 @@
         <v>0</v>
       </c>
       <c r="K91" s="100"/>
-      <c r="L91" s="535"/>
-      <c r="M91" s="536"/>
+      <c r="L91" s="543"/>
+      <c r="M91" s="544"/>
       <c r="N91" s="77">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -9139,8 +9142,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O97" s="519"/>
-      <c r="P97" s="529"/>
+      <c r="O97" s="539"/>
+      <c r="P97" s="535"/>
       <c r="Q97" s="164"/>
       <c r="R97" s="129"/>
       <c r="S97" s="180"/>
@@ -9172,8 +9175,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O98" s="520"/>
-      <c r="P98" s="530"/>
+      <c r="O98" s="540"/>
+      <c r="P98" s="536"/>
       <c r="Q98" s="164"/>
       <c r="R98" s="129"/>
       <c r="S98" s="180"/>
@@ -14565,11 +14568,11 @@
         <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
-      <c r="F262" s="531" t="s">
+      <c r="F262" s="537" t="s">
         <v>26</v>
       </c>
-      <c r="G262" s="531"/>
-      <c r="H262" s="532"/>
+      <c r="G262" s="537"/>
+      <c r="H262" s="538"/>
       <c r="I262" s="317">
         <f>SUM(I4:I261)</f>
         <v>426245.47000000003</v>
@@ -15143,6 +15146,22 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="P68:P69"/>
+    <mergeCell ref="C63:C64"/>
+    <mergeCell ref="H63:H64"/>
+    <mergeCell ref="O68:O69"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="H58:H59"/>
+    <mergeCell ref="O58:O59"/>
+    <mergeCell ref="P97:P98"/>
+    <mergeCell ref="F262:H262"/>
+    <mergeCell ref="O82:O83"/>
+    <mergeCell ref="P82:P83"/>
+    <mergeCell ref="O84:O85"/>
+    <mergeCell ref="P84:P85"/>
+    <mergeCell ref="L90:M91"/>
+    <mergeCell ref="O97:O98"/>
     <mergeCell ref="A1:J2"/>
     <mergeCell ref="W1:X1"/>
     <mergeCell ref="O3:P3"/>
@@ -15156,22 +15175,6 @@
     <mergeCell ref="C56:C57"/>
     <mergeCell ref="H56:H57"/>
     <mergeCell ref="P58:P59"/>
-    <mergeCell ref="P97:P98"/>
-    <mergeCell ref="F262:H262"/>
-    <mergeCell ref="O82:O83"/>
-    <mergeCell ref="P82:P83"/>
-    <mergeCell ref="O84:O85"/>
-    <mergeCell ref="P84:P85"/>
-    <mergeCell ref="L90:M91"/>
-    <mergeCell ref="O97:O98"/>
-    <mergeCell ref="P68:P69"/>
-    <mergeCell ref="C63:C64"/>
-    <mergeCell ref="H63:H64"/>
-    <mergeCell ref="O68:O69"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="C58:C59"/>
-    <mergeCell ref="H58:H59"/>
-    <mergeCell ref="O58:O59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -15215,49 +15218,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="42.75" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A1" s="537" t="s">
+      <c r="A1" s="514" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="537"/>
-      <c r="C1" s="537"/>
-      <c r="D1" s="537"/>
-      <c r="E1" s="537"/>
-      <c r="F1" s="537"/>
-      <c r="G1" s="537"/>
-      <c r="H1" s="537"/>
-      <c r="I1" s="537"/>
-      <c r="J1" s="537"/>
+      <c r="B1" s="514"/>
+      <c r="C1" s="514"/>
+      <c r="D1" s="514"/>
+      <c r="E1" s="514"/>
+      <c r="F1" s="514"/>
+      <c r="G1" s="514"/>
+      <c r="H1" s="514"/>
+      <c r="I1" s="514"/>
+      <c r="J1" s="514"/>
       <c r="K1" s="375"/>
       <c r="L1" s="375"/>
       <c r="M1" s="375"/>
       <c r="N1" s="375"/>
       <c r="O1" s="376"/>
-      <c r="S1" s="556" t="s">
+      <c r="S1" s="557" t="s">
         <v>142</v>
       </c>
-      <c r="T1" s="556"/>
+      <c r="T1" s="557"/>
       <c r="U1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="V1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="W1" s="538" t="s">
+      <c r="W1" s="515" t="s">
         <v>2</v>
       </c>
-      <c r="X1" s="539"/>
+      <c r="X1" s="516"/>
     </row>
     <row r="2" spans="1:24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="537"/>
-      <c r="B2" s="537"/>
-      <c r="C2" s="537"/>
-      <c r="D2" s="537"/>
-      <c r="E2" s="537"/>
-      <c r="F2" s="537"/>
-      <c r="G2" s="537"/>
-      <c r="H2" s="537"/>
-      <c r="I2" s="537"/>
-      <c r="J2" s="537"/>
+      <c r="A2" s="514"/>
+      <c r="B2" s="514"/>
+      <c r="C2" s="514"/>
+      <c r="D2" s="514"/>
+      <c r="E2" s="514"/>
+      <c r="F2" s="514"/>
+      <c r="G2" s="514"/>
+      <c r="H2" s="514"/>
+      <c r="I2" s="514"/>
+      <c r="J2" s="514"/>
       <c r="K2" s="377"/>
       <c r="L2" s="377"/>
       <c r="M2" s="377"/>
@@ -15265,8 +15268,8 @@
       <c r="O2" s="379"/>
       <c r="Q2" s="10"/>
       <c r="R2" s="11"/>
-      <c r="S2" s="557"/>
-      <c r="T2" s="557"/>
+      <c r="S2" s="558"/>
+      <c r="T2" s="558"/>
       <c r="U2" s="14"/>
       <c r="V2" s="15"/>
       <c r="W2" s="16"/>
@@ -15311,10 +15314,10 @@
       <c r="N3" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="540" t="s">
+      <c r="O3" s="517" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="541"/>
+      <c r="P3" s="518"/>
       <c r="Q3" s="30" t="s">
         <v>16</v>
       </c>
@@ -17950,13 +17953,13 @@
       <c r="V54" s="160"/>
     </row>
     <row r="55" spans="1:24" s="161" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="558" t="s">
+      <c r="A55" s="559" t="s">
         <v>41</v>
       </c>
       <c r="B55" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="C55" s="523" t="s">
+      <c r="C55" s="533" t="s">
         <v>160</v>
       </c>
       <c r="D55" s="150"/>
@@ -17967,7 +17970,7 @@
       <c r="G55" s="152">
         <v>44599</v>
       </c>
-      <c r="H55" s="517" t="s">
+      <c r="H55" s="549" t="s">
         <v>161</v>
       </c>
       <c r="I55" s="151">
@@ -17996,11 +17999,11 @@
       <c r="V55" s="160"/>
     </row>
     <row r="56" spans="1:24" s="161" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="559"/>
+      <c r="A56" s="560"/>
       <c r="B56" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="C56" s="524"/>
+      <c r="C56" s="534"/>
       <c r="D56" s="163"/>
       <c r="E56" s="40"/>
       <c r="F56" s="151">
@@ -18009,7 +18012,7 @@
       <c r="G56" s="152">
         <v>44599</v>
       </c>
-      <c r="H56" s="518"/>
+      <c r="H56" s="550"/>
       <c r="I56" s="151">
         <v>194.4</v>
       </c>
@@ -18038,13 +18041,13 @@
       <c r="X56"/>
     </row>
     <row r="57" spans="1:24" ht="26.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="550" t="s">
+      <c r="A57" s="551" t="s">
         <v>41</v>
       </c>
       <c r="B57" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="C57" s="552" t="s">
+      <c r="C57" s="553" t="s">
         <v>162</v>
       </c>
       <c r="D57" s="165"/>
@@ -18055,7 +18058,7 @@
       <c r="G57" s="152">
         <v>44606</v>
       </c>
-      <c r="H57" s="517" t="s">
+      <c r="H57" s="549" t="s">
         <v>163</v>
       </c>
       <c r="I57" s="151">
@@ -18074,10 +18077,10 @@
         <f t="shared" si="1"/>
         <v>35776</v>
       </c>
-      <c r="O57" s="519" t="s">
+      <c r="O57" s="539" t="s">
         <v>59</v>
       </c>
-      <c r="P57" s="513">
+      <c r="P57" s="545">
         <v>44620</v>
       </c>
       <c r="Q57" s="164"/>
@@ -18088,11 +18091,11 @@
       <c r="V57" s="54"/>
     </row>
     <row r="58" spans="1:24" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="551"/>
+      <c r="A58" s="552"/>
       <c r="B58" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="C58" s="553"/>
+      <c r="C58" s="554"/>
       <c r="D58" s="165"/>
       <c r="E58" s="40"/>
       <c r="F58" s="151">
@@ -18101,7 +18104,7 @@
       <c r="G58" s="152">
         <v>44606</v>
       </c>
-      <c r="H58" s="518"/>
+      <c r="H58" s="550"/>
       <c r="I58" s="151">
         <v>627.60209999999995</v>
       </c>
@@ -18118,8 +18121,8 @@
         <f t="shared" si="1"/>
         <v>58366.995299999995</v>
       </c>
-      <c r="O58" s="554"/>
-      <c r="P58" s="555"/>
+      <c r="O58" s="555"/>
+      <c r="P58" s="556"/>
       <c r="Q58" s="164"/>
       <c r="R58" s="129"/>
       <c r="S58" s="92"/>
@@ -18145,7 +18148,7 @@
       <c r="G59" s="152">
         <v>44613</v>
       </c>
-      <c r="H59" s="517" t="s">
+      <c r="H59" s="549" t="s">
         <v>225</v>
       </c>
       <c r="I59" s="151">
@@ -18189,7 +18192,7 @@
       <c r="E60" s="40"/>
       <c r="F60" s="151"/>
       <c r="G60" s="152"/>
-      <c r="H60" s="518"/>
+      <c r="H60" s="550"/>
       <c r="I60" s="151"/>
       <c r="J60" s="45">
         <f t="shared" si="0"/>
@@ -18852,8 +18855,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O79" s="519"/>
-      <c r="P79" s="533"/>
+      <c r="O79" s="539"/>
+      <c r="P79" s="541"/>
       <c r="Q79" s="164"/>
       <c r="R79" s="129"/>
       <c r="S79" s="180"/>
@@ -18882,8 +18885,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O80" s="520"/>
-      <c r="P80" s="534"/>
+      <c r="O80" s="540"/>
+      <c r="P80" s="542"/>
       <c r="Q80" s="164"/>
       <c r="R80" s="129"/>
       <c r="S80" s="180"/>
@@ -18912,8 +18915,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O81" s="519"/>
-      <c r="P81" s="533"/>
+      <c r="O81" s="539"/>
+      <c r="P81" s="541"/>
       <c r="Q81" s="164"/>
       <c r="R81" s="158"/>
       <c r="S81" s="180"/>
@@ -18945,8 +18948,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O82" s="520"/>
-      <c r="P82" s="534"/>
+      <c r="O82" s="540"/>
+      <c r="P82" s="542"/>
       <c r="Q82" s="164"/>
       <c r="R82" s="158"/>
       <c r="S82" s="180"/>
@@ -19104,8 +19107,8 @@
         <v>0</v>
       </c>
       <c r="K87" s="100"/>
-      <c r="L87" s="535"/>
-      <c r="M87" s="536"/>
+      <c r="L87" s="543"/>
+      <c r="M87" s="544"/>
       <c r="N87" s="77">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -19137,8 +19140,8 @@
         <v>0</v>
       </c>
       <c r="K88" s="100"/>
-      <c r="L88" s="535"/>
-      <c r="M88" s="536"/>
+      <c r="L88" s="543"/>
+      <c r="M88" s="544"/>
       <c r="N88" s="77">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -19341,8 +19344,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O94" s="519"/>
-      <c r="P94" s="529"/>
+      <c r="O94" s="539"/>
+      <c r="P94" s="535"/>
       <c r="Q94" s="164"/>
       <c r="R94" s="129"/>
       <c r="S94" s="180"/>
@@ -19374,8 +19377,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O95" s="520"/>
-      <c r="P95" s="530"/>
+      <c r="O95" s="540"/>
+      <c r="P95" s="536"/>
       <c r="Q95" s="164"/>
       <c r="R95" s="129"/>
       <c r="S95" s="180"/>
@@ -24767,11 +24770,11 @@
         <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
-      <c r="F259" s="531" t="s">
+      <c r="F259" s="537" t="s">
         <v>26</v>
       </c>
-      <c r="G259" s="531"/>
-      <c r="H259" s="532"/>
+      <c r="G259" s="537"/>
+      <c r="H259" s="538"/>
       <c r="I259" s="317">
         <f>SUM(I4:I258)</f>
         <v>387207.97210000001</v>
@@ -25345,12 +25348,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="F259:H259"/>
-    <mergeCell ref="O81:O82"/>
-    <mergeCell ref="P81:P82"/>
-    <mergeCell ref="L87:M88"/>
-    <mergeCell ref="O94:O95"/>
-    <mergeCell ref="P94:P95"/>
     <mergeCell ref="O79:O80"/>
     <mergeCell ref="P79:P80"/>
     <mergeCell ref="A1:J2"/>
@@ -25366,6 +25363,12 @@
     <mergeCell ref="C55:C56"/>
     <mergeCell ref="A55:A56"/>
     <mergeCell ref="H55:H56"/>
+    <mergeCell ref="F259:H259"/>
+    <mergeCell ref="O81:O82"/>
+    <mergeCell ref="P81:P82"/>
+    <mergeCell ref="L87:M88"/>
+    <mergeCell ref="O94:O95"/>
+    <mergeCell ref="P94:P95"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -25412,49 +25415,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="42.75" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A1" s="537" t="s">
+      <c r="A1" s="514" t="s">
         <v>189</v>
       </c>
-      <c r="B1" s="537"/>
-      <c r="C1" s="537"/>
-      <c r="D1" s="537"/>
-      <c r="E1" s="537"/>
-      <c r="F1" s="537"/>
-      <c r="G1" s="537"/>
-      <c r="H1" s="537"/>
-      <c r="I1" s="537"/>
-      <c r="J1" s="537"/>
+      <c r="B1" s="514"/>
+      <c r="C1" s="514"/>
+      <c r="D1" s="514"/>
+      <c r="E1" s="514"/>
+      <c r="F1" s="514"/>
+      <c r="G1" s="514"/>
+      <c r="H1" s="514"/>
+      <c r="I1" s="514"/>
+      <c r="J1" s="514"/>
       <c r="K1" s="375"/>
       <c r="L1" s="375"/>
       <c r="M1" s="375"/>
       <c r="N1" s="375"/>
       <c r="O1" s="376"/>
-      <c r="S1" s="556" t="s">
+      <c r="S1" s="557" t="s">
         <v>142</v>
       </c>
-      <c r="T1" s="556"/>
+      <c r="T1" s="557"/>
       <c r="U1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="V1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="W1" s="538" t="s">
+      <c r="W1" s="515" t="s">
         <v>2</v>
       </c>
-      <c r="X1" s="539"/>
+      <c r="X1" s="516"/>
     </row>
     <row r="2" spans="1:24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="537"/>
-      <c r="B2" s="537"/>
-      <c r="C2" s="537"/>
-      <c r="D2" s="537"/>
-      <c r="E2" s="537"/>
-      <c r="F2" s="537"/>
-      <c r="G2" s="537"/>
-      <c r="H2" s="537"/>
-      <c r="I2" s="537"/>
-      <c r="J2" s="537"/>
+      <c r="A2" s="514"/>
+      <c r="B2" s="514"/>
+      <c r="C2" s="514"/>
+      <c r="D2" s="514"/>
+      <c r="E2" s="514"/>
+      <c r="F2" s="514"/>
+      <c r="G2" s="514"/>
+      <c r="H2" s="514"/>
+      <c r="I2" s="514"/>
+      <c r="J2" s="514"/>
       <c r="K2" s="377"/>
       <c r="L2" s="377"/>
       <c r="M2" s="377"/>
@@ -25462,8 +25465,8 @@
       <c r="O2" s="379"/>
       <c r="Q2" s="10"/>
       <c r="R2" s="11"/>
-      <c r="S2" s="557"/>
-      <c r="T2" s="557"/>
+      <c r="S2" s="558"/>
+      <c r="T2" s="558"/>
       <c r="U2" s="14"/>
       <c r="V2" s="15"/>
       <c r="W2" s="16"/>
@@ -25508,10 +25511,10 @@
       <c r="N3" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="540" t="s">
+      <c r="O3" s="517" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="541"/>
+      <c r="P3" s="518"/>
       <c r="Q3" s="30" t="s">
         <v>16</v>
       </c>
@@ -28719,13 +28722,13 @@
       <c r="V54" s="160"/>
     </row>
     <row r="55" spans="1:24" s="161" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="558" t="s">
+      <c r="A55" s="559" t="s">
         <v>41</v>
       </c>
       <c r="B55" s="438" t="s">
         <v>24</v>
       </c>
-      <c r="C55" s="523" t="s">
+      <c r="C55" s="533" t="s">
         <v>229</v>
       </c>
       <c r="D55" s="439"/>
@@ -28736,7 +28739,7 @@
       <c r="G55" s="152">
         <v>44627</v>
       </c>
-      <c r="H55" s="563" t="s">
+      <c r="H55" s="562" t="s">
         <v>230</v>
       </c>
       <c r="I55" s="151">
@@ -28755,10 +28758,10 @@
         <f t="shared" si="1"/>
         <v>18886.399999999998</v>
       </c>
-      <c r="O55" s="519" t="s">
+      <c r="O55" s="539" t="s">
         <v>59</v>
       </c>
-      <c r="P55" s="513">
+      <c r="P55" s="545">
         <v>44645</v>
       </c>
       <c r="Q55" s="128"/>
@@ -28769,11 +28772,11 @@
       <c r="V55" s="160"/>
     </row>
     <row r="56" spans="1:24" s="161" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="562"/>
+      <c r="A56" s="561"/>
       <c r="B56" s="438" t="s">
         <v>24</v>
       </c>
-      <c r="C56" s="524"/>
+      <c r="C56" s="534"/>
       <c r="D56" s="440"/>
       <c r="E56" s="60"/>
       <c r="F56" s="151">
@@ -28782,7 +28785,7 @@
       <c r="G56" s="152">
         <v>44627</v>
       </c>
-      <c r="H56" s="564"/>
+      <c r="H56" s="563"/>
       <c r="I56" s="151">
         <v>967</v>
       </c>
@@ -28799,8 +28802,8 @@
         <f t="shared" si="1"/>
         <v>92832</v>
       </c>
-      <c r="O56" s="520"/>
-      <c r="P56" s="514"/>
+      <c r="O56" s="540"/>
+      <c r="P56" s="546"/>
       <c r="Q56" s="164"/>
       <c r="R56" s="158"/>
       <c r="S56" s="92"/>
@@ -28861,13 +28864,13 @@
       <c r="V57" s="54"/>
     </row>
     <row r="58" spans="1:24" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="546" t="s">
+      <c r="A58" s="523" t="s">
         <v>41</v>
       </c>
       <c r="B58" s="170" t="s">
         <v>24</v>
       </c>
-      <c r="C58" s="560" t="s">
+      <c r="C58" s="572" t="s">
         <v>319</v>
       </c>
       <c r="D58" s="165"/>
@@ -28878,7 +28881,7 @@
       <c r="G58" s="152">
         <v>44648</v>
       </c>
-      <c r="H58" s="571" t="s">
+      <c r="H58" s="570" t="s">
         <v>315</v>
       </c>
       <c r="I58" s="151">
@@ -28900,7 +28903,7 @@
       <c r="O58" s="527" t="s">
         <v>59</v>
       </c>
-      <c r="P58" s="548">
+      <c r="P58" s="529">
         <v>44662</v>
       </c>
       <c r="Q58" s="164"/>
@@ -28911,11 +28914,11 @@
       <c r="V58" s="54"/>
     </row>
     <row r="59" spans="1:24" s="161" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="547"/>
+      <c r="A59" s="524"/>
       <c r="B59" s="170" t="s">
         <v>23</v>
       </c>
-      <c r="C59" s="561"/>
+      <c r="C59" s="573"/>
       <c r="D59" s="163"/>
       <c r="E59" s="60"/>
       <c r="F59" s="151">
@@ -28924,7 +28927,7 @@
       <c r="G59" s="152">
         <v>44648</v>
       </c>
-      <c r="H59" s="572"/>
+      <c r="H59" s="571"/>
       <c r="I59" s="151">
         <v>719</v>
       </c>
@@ -28942,7 +28945,7 @@
         <v>69024</v>
       </c>
       <c r="O59" s="528"/>
-      <c r="P59" s="549"/>
+      <c r="P59" s="530"/>
       <c r="Q59" s="164"/>
       <c r="R59" s="158"/>
       <c r="S59" s="92"/>
@@ -29015,13 +29018,13 @@
       <c r="V61" s="54"/>
     </row>
     <row r="62" spans="1:24" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A62" s="565" t="s">
+      <c r="A62" s="564" t="s">
         <v>106</v>
       </c>
       <c r="B62" s="178" t="s">
         <v>237</v>
       </c>
-      <c r="C62" s="567" t="s">
+      <c r="C62" s="566" t="s">
         <v>238</v>
       </c>
       <c r="D62" s="168"/>
@@ -29032,7 +29035,7 @@
       <c r="G62" s="152">
         <v>44622</v>
       </c>
-      <c r="H62" s="569">
+      <c r="H62" s="568">
         <v>37162</v>
       </c>
       <c r="I62" s="151">
@@ -29051,10 +29054,10 @@
         <f t="shared" si="1"/>
         <v>7782.5999999999995</v>
       </c>
-      <c r="O62" s="519" t="s">
+      <c r="O62" s="539" t="s">
         <v>61</v>
       </c>
-      <c r="P62" s="513">
+      <c r="P62" s="545">
         <v>44643</v>
       </c>
       <c r="Q62" s="164"/>
@@ -29065,11 +29068,11 @@
       <c r="V62" s="54"/>
     </row>
     <row r="63" spans="1:24" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A63" s="566"/>
+      <c r="A63" s="565"/>
       <c r="B63" s="178" t="s">
         <v>239</v>
       </c>
-      <c r="C63" s="568"/>
+      <c r="C63" s="567"/>
       <c r="D63" s="168"/>
       <c r="E63" s="60"/>
       <c r="F63" s="151">
@@ -29078,7 +29081,7 @@
       <c r="G63" s="152">
         <v>44622</v>
       </c>
-      <c r="H63" s="570"/>
+      <c r="H63" s="569"/>
       <c r="I63" s="151">
         <v>204.8</v>
       </c>
@@ -29095,8 +29098,8 @@
         <f t="shared" si="1"/>
         <v>16998.400000000001</v>
       </c>
-      <c r="O63" s="520"/>
-      <c r="P63" s="514"/>
+      <c r="O63" s="540"/>
+      <c r="P63" s="546"/>
       <c r="Q63" s="164"/>
       <c r="R63" s="129"/>
       <c r="S63" s="92"/>
@@ -29575,8 +29578,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O79" s="519"/>
-      <c r="P79" s="533"/>
+      <c r="O79" s="539"/>
+      <c r="P79" s="541"/>
       <c r="Q79" s="164"/>
       <c r="R79" s="129"/>
       <c r="S79" s="180"/>
@@ -29605,8 +29608,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O80" s="520"/>
-      <c r="P80" s="534"/>
+      <c r="O80" s="540"/>
+      <c r="P80" s="542"/>
       <c r="Q80" s="164"/>
       <c r="R80" s="129"/>
       <c r="S80" s="180"/>
@@ -29635,8 +29638,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O81" s="519"/>
-      <c r="P81" s="533"/>
+      <c r="O81" s="539"/>
+      <c r="P81" s="541"/>
       <c r="Q81" s="164"/>
       <c r="R81" s="158"/>
       <c r="S81" s="180"/>
@@ -29668,8 +29671,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O82" s="520"/>
-      <c r="P82" s="534"/>
+      <c r="O82" s="540"/>
+      <c r="P82" s="542"/>
       <c r="Q82" s="164"/>
       <c r="R82" s="158"/>
       <c r="S82" s="180"/>
@@ -29827,8 +29830,8 @@
         <v>0</v>
       </c>
       <c r="K87" s="100"/>
-      <c r="L87" s="535"/>
-      <c r="M87" s="536"/>
+      <c r="L87" s="543"/>
+      <c r="M87" s="544"/>
       <c r="N87" s="48">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -29860,8 +29863,8 @@
         <v>0</v>
       </c>
       <c r="K88" s="100"/>
-      <c r="L88" s="535"/>
-      <c r="M88" s="536"/>
+      <c r="L88" s="543"/>
+      <c r="M88" s="544"/>
       <c r="N88" s="48">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -30064,8 +30067,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O94" s="519"/>
-      <c r="P94" s="529"/>
+      <c r="O94" s="539"/>
+      <c r="P94" s="535"/>
       <c r="Q94" s="164"/>
       <c r="R94" s="129"/>
       <c r="S94" s="180"/>
@@ -30097,8 +30100,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O95" s="520"/>
-      <c r="P95" s="530"/>
+      <c r="O95" s="540"/>
+      <c r="P95" s="536"/>
       <c r="Q95" s="164"/>
       <c r="R95" s="129"/>
       <c r="S95" s="180"/>
@@ -35490,11 +35493,11 @@
         <f t="shared" si="10"/>
         <v>#VALUE!</v>
       </c>
-      <c r="F259" s="531" t="s">
+      <c r="F259" s="537" t="s">
         <v>26</v>
       </c>
-      <c r="G259" s="531"/>
-      <c r="H259" s="532"/>
+      <c r="G259" s="537"/>
+      <c r="H259" s="538"/>
       <c r="I259" s="317">
         <f>SUM(I4:I258)</f>
         <v>517031.52999999991</v>
@@ -36068,6 +36071,17 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="O58:O59"/>
+    <mergeCell ref="P58:P59"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="O94:O95"/>
+    <mergeCell ref="P94:P95"/>
+    <mergeCell ref="F259:H259"/>
+    <mergeCell ref="O79:O80"/>
+    <mergeCell ref="P79:P80"/>
+    <mergeCell ref="O81:O82"/>
+    <mergeCell ref="P81:P82"/>
     <mergeCell ref="A1:J2"/>
     <mergeCell ref="S1:T2"/>
     <mergeCell ref="W1:X1"/>
@@ -36084,17 +36098,6 @@
     <mergeCell ref="O62:O63"/>
     <mergeCell ref="P62:P63"/>
     <mergeCell ref="H58:H59"/>
-    <mergeCell ref="F259:H259"/>
-    <mergeCell ref="O79:O80"/>
-    <mergeCell ref="P79:P80"/>
-    <mergeCell ref="O81:O82"/>
-    <mergeCell ref="P81:P82"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="O58:O59"/>
-    <mergeCell ref="P58:P59"/>
-    <mergeCell ref="C58:C59"/>
-    <mergeCell ref="O94:O95"/>
-    <mergeCell ref="P94:P95"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -36109,7 +36112,7 @@
   <dimension ref="A1:X292"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="8" ySplit="3" topLeftCell="I33" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="8" ySplit="3" topLeftCell="W4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight" activeCell="A37" sqref="A37"/>
@@ -36141,49 +36144,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="42.75" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A1" s="537" t="s">
+      <c r="A1" s="514" t="s">
         <v>288</v>
       </c>
-      <c r="B1" s="537"/>
-      <c r="C1" s="537"/>
-      <c r="D1" s="537"/>
-      <c r="E1" s="537"/>
-      <c r="F1" s="537"/>
-      <c r="G1" s="537"/>
-      <c r="H1" s="537"/>
-      <c r="I1" s="537"/>
-      <c r="J1" s="537"/>
+      <c r="B1" s="514"/>
+      <c r="C1" s="514"/>
+      <c r="D1" s="514"/>
+      <c r="E1" s="514"/>
+      <c r="F1" s="514"/>
+      <c r="G1" s="514"/>
+      <c r="H1" s="514"/>
+      <c r="I1" s="514"/>
+      <c r="J1" s="514"/>
       <c r="K1" s="375"/>
       <c r="L1" s="375"/>
       <c r="M1" s="375"/>
       <c r="N1" s="375"/>
       <c r="O1" s="376"/>
-      <c r="S1" s="556" t="s">
+      <c r="S1" s="557" t="s">
         <v>142</v>
       </c>
-      <c r="T1" s="556"/>
+      <c r="T1" s="557"/>
       <c r="U1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="V1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="W1" s="538" t="s">
+      <c r="W1" s="515" t="s">
         <v>2</v>
       </c>
-      <c r="X1" s="539"/>
+      <c r="X1" s="516"/>
     </row>
     <row r="2" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="537"/>
-      <c r="B2" s="537"/>
-      <c r="C2" s="537"/>
-      <c r="D2" s="537"/>
-      <c r="E2" s="537"/>
-      <c r="F2" s="537"/>
-      <c r="G2" s="537"/>
-      <c r="H2" s="537"/>
-      <c r="I2" s="537"/>
-      <c r="J2" s="537"/>
+      <c r="A2" s="514"/>
+      <c r="B2" s="514"/>
+      <c r="C2" s="514"/>
+      <c r="D2" s="514"/>
+      <c r="E2" s="514"/>
+      <c r="F2" s="514"/>
+      <c r="G2" s="514"/>
+      <c r="H2" s="514"/>
+      <c r="I2" s="514"/>
+      <c r="J2" s="514"/>
       <c r="K2" s="377"/>
       <c r="L2" s="377"/>
       <c r="M2" s="377"/>
@@ -36191,8 +36194,8 @@
       <c r="O2" s="379"/>
       <c r="Q2" s="10"/>
       <c r="R2" s="11"/>
-      <c r="S2" s="557"/>
-      <c r="T2" s="557"/>
+      <c r="S2" s="558"/>
+      <c r="T2" s="558"/>
       <c r="U2" s="14"/>
       <c r="V2" s="15"/>
       <c r="W2" s="16"/>
@@ -36237,10 +36240,10 @@
       <c r="N3" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="540" t="s">
+      <c r="O3" s="517" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="541"/>
+      <c r="P3" s="518"/>
       <c r="Q3" s="30" t="s">
         <v>16</v>
       </c>
@@ -39622,13 +39625,13 @@
       <c r="V63" s="54"/>
     </row>
     <row r="64" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="558" t="s">
+      <c r="A64" s="559" t="s">
         <v>111</v>
       </c>
       <c r="B64" s="178" t="s">
         <v>464</v>
       </c>
-      <c r="C64" s="567" t="s">
+      <c r="C64" s="566" t="s">
         <v>465</v>
       </c>
       <c r="D64" s="171"/>
@@ -39639,7 +39642,7 @@
       <c r="G64" s="504">
         <v>44681</v>
       </c>
-      <c r="H64" s="573">
+      <c r="H64" s="574">
         <v>132899</v>
       </c>
       <c r="I64" s="505">
@@ -39658,10 +39661,10 @@
         <f t="shared" si="1"/>
         <v>19360</v>
       </c>
-      <c r="O64" s="575" t="s">
+      <c r="O64" s="576" t="s">
         <v>59</v>
       </c>
-      <c r="P64" s="577">
+      <c r="P64" s="578">
         <v>44708</v>
       </c>
       <c r="Q64" s="167"/>
@@ -39672,11 +39675,11 @@
       <c r="V64" s="54"/>
     </row>
     <row r="65" spans="1:22" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="562"/>
+      <c r="A65" s="561"/>
       <c r="B65" s="178" t="s">
         <v>240</v>
       </c>
-      <c r="C65" s="568"/>
+      <c r="C65" s="567"/>
       <c r="D65" s="171"/>
       <c r="E65" s="60"/>
       <c r="F65" s="151">
@@ -39685,7 +39688,7 @@
       <c r="G65" s="504">
         <v>44681</v>
       </c>
-      <c r="H65" s="574"/>
+      <c r="H65" s="575"/>
       <c r="I65" s="505">
         <v>508</v>
       </c>
@@ -39702,8 +39705,8 @@
         <f t="shared" si="1"/>
         <v>32512</v>
       </c>
-      <c r="O65" s="576"/>
-      <c r="P65" s="578"/>
+      <c r="O65" s="577"/>
+      <c r="P65" s="579"/>
       <c r="Q65" s="167"/>
       <c r="R65" s="129"/>
       <c r="S65" s="180"/>
@@ -40122,8 +40125,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O79" s="519"/>
-      <c r="P79" s="533"/>
+      <c r="O79" s="539"/>
+      <c r="P79" s="541"/>
       <c r="Q79" s="164"/>
       <c r="R79" s="129"/>
       <c r="S79" s="180"/>
@@ -40152,8 +40155,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O80" s="520"/>
-      <c r="P80" s="534"/>
+      <c r="O80" s="540"/>
+      <c r="P80" s="542"/>
       <c r="Q80" s="164"/>
       <c r="R80" s="129"/>
       <c r="S80" s="180"/>
@@ -40182,8 +40185,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O81" s="519"/>
-      <c r="P81" s="533"/>
+      <c r="O81" s="539"/>
+      <c r="P81" s="541"/>
       <c r="Q81" s="164"/>
       <c r="R81" s="158"/>
       <c r="S81" s="180"/>
@@ -40215,8 +40218,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O82" s="520"/>
-      <c r="P82" s="534"/>
+      <c r="O82" s="540"/>
+      <c r="P82" s="542"/>
       <c r="Q82" s="164"/>
       <c r="R82" s="158"/>
       <c r="S82" s="180"/>
@@ -40374,8 +40377,8 @@
         <v>0</v>
       </c>
       <c r="K87" s="100"/>
-      <c r="L87" s="535"/>
-      <c r="M87" s="536"/>
+      <c r="L87" s="543"/>
+      <c r="M87" s="544"/>
       <c r="N87" s="48">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -40407,8 +40410,8 @@
         <v>0</v>
       </c>
       <c r="K88" s="100"/>
-      <c r="L88" s="535"/>
-      <c r="M88" s="536"/>
+      <c r="L88" s="543"/>
+      <c r="M88" s="544"/>
       <c r="N88" s="48">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -40611,8 +40614,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O94" s="519"/>
-      <c r="P94" s="529"/>
+      <c r="O94" s="539"/>
+      <c r="P94" s="535"/>
       <c r="Q94" s="164"/>
       <c r="R94" s="129"/>
       <c r="S94" s="180"/>
@@ -40644,8 +40647,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O95" s="520"/>
-      <c r="P95" s="530"/>
+      <c r="O95" s="540"/>
+      <c r="P95" s="536"/>
       <c r="Q95" s="164"/>
       <c r="R95" s="129"/>
       <c r="S95" s="180"/>
@@ -46037,11 +46040,11 @@
         <f t="shared" si="11"/>
         <v>#VALUE!</v>
       </c>
-      <c r="F259" s="531" t="s">
+      <c r="F259" s="537" t="s">
         <v>26</v>
       </c>
-      <c r="G259" s="531"/>
-      <c r="H259" s="532"/>
+      <c r="G259" s="537"/>
+      <c r="H259" s="538"/>
       <c r="I259" s="317">
         <f>SUM(I4:I258)</f>
         <v>491966.85000000003</v>
@@ -46615,12 +46618,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="F259:H259"/>
-    <mergeCell ref="O81:O82"/>
-    <mergeCell ref="P81:P82"/>
-    <mergeCell ref="L87:M88"/>
-    <mergeCell ref="O94:O95"/>
-    <mergeCell ref="P94:P95"/>
     <mergeCell ref="W1:X1"/>
     <mergeCell ref="O3:P3"/>
     <mergeCell ref="O79:O80"/>
@@ -46632,6 +46629,12 @@
     <mergeCell ref="H64:H65"/>
     <mergeCell ref="O64:O65"/>
     <mergeCell ref="P64:P65"/>
+    <mergeCell ref="F259:H259"/>
+    <mergeCell ref="O81:O82"/>
+    <mergeCell ref="P81:P82"/>
+    <mergeCell ref="L87:M88"/>
+    <mergeCell ref="O94:O95"/>
+    <mergeCell ref="P94:P95"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -46646,10 +46649,10 @@
   <dimension ref="A1:X292"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="8" ySplit="3" topLeftCell="M24" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="8" ySplit="3" topLeftCell="V24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="O33" sqref="O33"/>
+      <selection pane="bottomRight" activeCell="X36" sqref="X36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -46678,49 +46681,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="42.75" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A1" s="537" t="s">
+      <c r="A1" s="514" t="s">
         <v>402</v>
       </c>
-      <c r="B1" s="537"/>
-      <c r="C1" s="537"/>
-      <c r="D1" s="537"/>
-      <c r="E1" s="537"/>
-      <c r="F1" s="537"/>
-      <c r="G1" s="537"/>
-      <c r="H1" s="537"/>
-      <c r="I1" s="537"/>
-      <c r="J1" s="537"/>
+      <c r="B1" s="514"/>
+      <c r="C1" s="514"/>
+      <c r="D1" s="514"/>
+      <c r="E1" s="514"/>
+      <c r="F1" s="514"/>
+      <c r="G1" s="514"/>
+      <c r="H1" s="514"/>
+      <c r="I1" s="514"/>
+      <c r="J1" s="514"/>
       <c r="K1" s="375"/>
       <c r="L1" s="375"/>
       <c r="M1" s="375"/>
       <c r="N1" s="375"/>
       <c r="O1" s="376"/>
-      <c r="S1" s="556" t="s">
+      <c r="S1" s="557" t="s">
         <v>142</v>
       </c>
-      <c r="T1" s="556"/>
+      <c r="T1" s="557"/>
       <c r="U1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="V1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="W1" s="538" t="s">
+      <c r="W1" s="515" t="s">
         <v>2</v>
       </c>
-      <c r="X1" s="539"/>
+      <c r="X1" s="516"/>
     </row>
     <row r="2" spans="1:24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="537"/>
-      <c r="B2" s="537"/>
-      <c r="C2" s="537"/>
-      <c r="D2" s="537"/>
-      <c r="E2" s="537"/>
-      <c r="F2" s="537"/>
-      <c r="G2" s="537"/>
-      <c r="H2" s="537"/>
-      <c r="I2" s="537"/>
-      <c r="J2" s="537"/>
+      <c r="A2" s="514"/>
+      <c r="B2" s="514"/>
+      <c r="C2" s="514"/>
+      <c r="D2" s="514"/>
+      <c r="E2" s="514"/>
+      <c r="F2" s="514"/>
+      <c r="G2" s="514"/>
+      <c r="H2" s="514"/>
+      <c r="I2" s="514"/>
+      <c r="J2" s="514"/>
       <c r="K2" s="377"/>
       <c r="L2" s="377"/>
       <c r="M2" s="377"/>
@@ -46728,8 +46731,8 @@
       <c r="O2" s="379"/>
       <c r="Q2" s="10"/>
       <c r="R2" s="11"/>
-      <c r="S2" s="557"/>
-      <c r="T2" s="557"/>
+      <c r="S2" s="558"/>
+      <c r="T2" s="558"/>
       <c r="U2" s="14"/>
       <c r="V2" s="15"/>
       <c r="W2" s="16"/>
@@ -46774,10 +46777,10 @@
       <c r="N3" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="540" t="s">
+      <c r="O3" s="517" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="541"/>
+      <c r="P3" s="518"/>
       <c r="Q3" s="30" t="s">
         <v>16</v>
       </c>
@@ -46861,8 +46864,12 @@
       </c>
       <c r="U4" s="53"/>
       <c r="V4" s="54"/>
-      <c r="W4" s="55"/>
-      <c r="X4" s="56"/>
+      <c r="W4" s="55" t="s">
+        <v>513</v>
+      </c>
+      <c r="X4" s="56">
+        <v>4176</v>
+      </c>
     </row>
     <row r="5" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="57" t="s">
@@ -46926,8 +46933,12 @@
       </c>
       <c r="U5" s="53"/>
       <c r="V5" s="54"/>
-      <c r="W5" s="68"/>
-      <c r="X5" s="69"/>
+      <c r="W5" s="68" t="s">
+        <v>513</v>
+      </c>
+      <c r="X5" s="69">
+        <v>4176</v>
+      </c>
     </row>
     <row r="6" spans="1:24" ht="30.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="57" t="s">
@@ -46991,8 +47002,12 @@
       </c>
       <c r="U6" s="53"/>
       <c r="V6" s="54"/>
-      <c r="W6" s="53"/>
-      <c r="X6" s="70"/>
+      <c r="W6" s="53" t="s">
+        <v>513</v>
+      </c>
+      <c r="X6" s="70">
+        <v>4176</v>
+      </c>
     </row>
     <row r="7" spans="1:24" ht="28.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="57" t="s">
@@ -47056,8 +47071,12 @@
       </c>
       <c r="U7" s="53"/>
       <c r="V7" s="54"/>
-      <c r="W7" s="53"/>
-      <c r="X7" s="70"/>
+      <c r="W7" s="53" t="s">
+        <v>513</v>
+      </c>
+      <c r="X7" s="70">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:24" ht="27.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="57" t="s">
@@ -47121,8 +47140,12 @@
       </c>
       <c r="U8" s="53"/>
       <c r="V8" s="54"/>
-      <c r="W8" s="53"/>
-      <c r="X8" s="70"/>
+      <c r="W8" s="53" t="s">
+        <v>513</v>
+      </c>
+      <c r="X8" s="70">
+        <v>4176</v>
+      </c>
     </row>
     <row r="9" spans="1:24" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="71" t="s">
@@ -47186,8 +47209,12 @@
       </c>
       <c r="U9" s="53"/>
       <c r="V9" s="54"/>
-      <c r="W9" s="53"/>
-      <c r="X9" s="70"/>
+      <c r="W9" s="53" t="s">
+        <v>513</v>
+      </c>
+      <c r="X9" s="70">
+        <v>4176</v>
+      </c>
     </row>
     <row r="10" spans="1:24" ht="24.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="71" t="s">
@@ -47251,8 +47278,12 @@
       </c>
       <c r="U10" s="53"/>
       <c r="V10" s="54"/>
-      <c r="W10" s="53"/>
-      <c r="X10" s="70"/>
+      <c r="W10" s="53" t="s">
+        <v>513</v>
+      </c>
+      <c r="X10" s="70">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:24" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="71" t="s">
@@ -47316,8 +47347,12 @@
       </c>
       <c r="U11" s="53"/>
       <c r="V11" s="54"/>
-      <c r="W11" s="53"/>
-      <c r="X11" s="70"/>
+      <c r="W11" s="53" t="s">
+        <v>513</v>
+      </c>
+      <c r="X11" s="70">
+        <v>4176</v>
+      </c>
     </row>
     <row r="12" spans="1:24" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="71" t="s">
@@ -47381,8 +47416,12 @@
       </c>
       <c r="U12" s="53"/>
       <c r="V12" s="54"/>
-      <c r="W12" s="53"/>
-      <c r="X12" s="70"/>
+      <c r="W12" s="53" t="s">
+        <v>513</v>
+      </c>
+      <c r="X12" s="70">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:24" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="71" t="s">
@@ -47446,8 +47485,12 @@
       </c>
       <c r="U13" s="53"/>
       <c r="V13" s="54"/>
-      <c r="W13" s="53"/>
-      <c r="X13" s="70"/>
+      <c r="W13" s="53" t="s">
+        <v>513</v>
+      </c>
+      <c r="X13" s="70">
+        <v>4176</v>
+      </c>
     </row>
     <row r="14" spans="1:24" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="71" t="s">
@@ -47511,8 +47554,12 @@
       </c>
       <c r="U14" s="53"/>
       <c r="V14" s="54"/>
-      <c r="W14" s="53"/>
-      <c r="X14" s="70"/>
+      <c r="W14" s="53" t="s">
+        <v>513</v>
+      </c>
+      <c r="X14" s="70">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:24" ht="33" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="73" t="s">
@@ -47576,8 +47623,12 @@
       </c>
       <c r="U15" s="53"/>
       <c r="V15" s="54"/>
-      <c r="W15" s="53"/>
-      <c r="X15" s="70"/>
+      <c r="W15" s="53" t="s">
+        <v>513</v>
+      </c>
+      <c r="X15" s="70">
+        <v>4176</v>
+      </c>
     </row>
     <row r="16" spans="1:24" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="71" t="s">
@@ -47641,8 +47692,12 @@
       </c>
       <c r="U16" s="53"/>
       <c r="V16" s="54"/>
-      <c r="W16" s="53"/>
-      <c r="X16" s="70"/>
+      <c r="W16" s="53" t="s">
+        <v>513</v>
+      </c>
+      <c r="X16" s="70">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:24" ht="28.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="75" t="s">
@@ -47706,8 +47761,12 @@
       </c>
       <c r="U17" s="53"/>
       <c r="V17" s="54"/>
-      <c r="W17" s="53"/>
-      <c r="X17" s="70"/>
+      <c r="W17" s="53" t="s">
+        <v>513</v>
+      </c>
+      <c r="X17" s="70">
+        <v>4176</v>
+      </c>
     </row>
     <row r="18" spans="1:24" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="81" t="s">
@@ -47771,8 +47830,12 @@
       </c>
       <c r="U18" s="53"/>
       <c r="V18" s="54"/>
-      <c r="W18" s="53"/>
-      <c r="X18" s="70"/>
+      <c r="W18" s="53" t="s">
+        <v>513</v>
+      </c>
+      <c r="X18" s="70">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="1:24" ht="48.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="78" t="s">
@@ -47837,8 +47900,12 @@
       </c>
       <c r="U19" s="53"/>
       <c r="V19" s="54"/>
-      <c r="W19" s="53"/>
-      <c r="X19" s="70"/>
+      <c r="W19" s="53" t="s">
+        <v>513</v>
+      </c>
+      <c r="X19" s="70">
+        <v>4176</v>
+      </c>
     </row>
     <row r="20" spans="1:24" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="80" t="s">
@@ -47902,8 +47969,12 @@
       </c>
       <c r="U20" s="53"/>
       <c r="V20" s="54"/>
-      <c r="W20" s="53"/>
-      <c r="X20" s="70"/>
+      <c r="W20" s="53" t="s">
+        <v>513</v>
+      </c>
+      <c r="X20" s="70">
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="1:24" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="78" t="s">
@@ -47967,8 +48038,12 @@
       </c>
       <c r="U21" s="53"/>
       <c r="V21" s="54"/>
-      <c r="W21" s="53"/>
-      <c r="X21" s="70"/>
+      <c r="W21" s="53" t="s">
+        <v>513</v>
+      </c>
+      <c r="X21" s="70">
+        <v>4176</v>
+      </c>
     </row>
     <row r="22" spans="1:24" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="81" t="s">
@@ -48032,8 +48107,12 @@
       </c>
       <c r="U22" s="53"/>
       <c r="V22" s="54"/>
-      <c r="W22" s="53"/>
-      <c r="X22" s="70"/>
+      <c r="W22" s="53" t="s">
+        <v>513</v>
+      </c>
+      <c r="X22" s="70">
+        <v>0</v>
+      </c>
     </row>
     <row r="23" spans="1:24" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="82" t="s">
@@ -48097,8 +48176,12 @@
       </c>
       <c r="U23" s="53"/>
       <c r="V23" s="54"/>
-      <c r="W23" s="53"/>
-      <c r="X23" s="70"/>
+      <c r="W23" s="53" t="s">
+        <v>513</v>
+      </c>
+      <c r="X23" s="70">
+        <v>4176</v>
+      </c>
     </row>
     <row r="24" spans="1:24" ht="28.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="83" t="s">
@@ -48162,8 +48245,12 @@
       </c>
       <c r="U24" s="53"/>
       <c r="V24" s="54"/>
-      <c r="W24" s="53"/>
-      <c r="X24" s="70"/>
+      <c r="W24" s="53" t="s">
+        <v>513</v>
+      </c>
+      <c r="X24" s="70">
+        <v>0</v>
+      </c>
     </row>
     <row r="25" spans="1:24" ht="48.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="71" t="s">
@@ -48228,8 +48315,12 @@
       </c>
       <c r="U25" s="53"/>
       <c r="V25" s="54"/>
-      <c r="W25" s="53"/>
-      <c r="X25" s="70"/>
+      <c r="W25" s="53" t="s">
+        <v>513</v>
+      </c>
+      <c r="X25" s="70">
+        <v>4176</v>
+      </c>
     </row>
     <row r="26" spans="1:24" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="82" t="s">
@@ -48293,8 +48384,12 @@
       </c>
       <c r="U26" s="53"/>
       <c r="V26" s="54"/>
-      <c r="W26" s="53"/>
-      <c r="X26" s="70"/>
+      <c r="W26" s="53" t="s">
+        <v>513</v>
+      </c>
+      <c r="X26" s="70">
+        <v>0</v>
+      </c>
     </row>
     <row r="27" spans="1:24" ht="48.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="82" t="s">
@@ -48359,8 +48454,12 @@
       </c>
       <c r="U27" s="53"/>
       <c r="V27" s="54"/>
-      <c r="W27" s="53"/>
-      <c r="X27" s="70"/>
+      <c r="W27" s="53" t="s">
+        <v>513</v>
+      </c>
+      <c r="X27" s="70">
+        <v>4176</v>
+      </c>
     </row>
     <row r="28" spans="1:24" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="82" t="s">
@@ -48424,8 +48523,12 @@
       </c>
       <c r="U28" s="53"/>
       <c r="V28" s="54"/>
-      <c r="W28" s="53"/>
-      <c r="X28" s="70"/>
+      <c r="W28" s="53" t="s">
+        <v>513</v>
+      </c>
+      <c r="X28" s="70">
+        <v>0</v>
+      </c>
     </row>
     <row r="29" spans="1:24" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="57" t="s">
@@ -48489,8 +48592,12 @@
       </c>
       <c r="U29" s="53"/>
       <c r="V29" s="54"/>
-      <c r="W29" s="53"/>
-      <c r="X29" s="70"/>
+      <c r="W29" s="53" t="s">
+        <v>513</v>
+      </c>
+      <c r="X29" s="70">
+        <v>4176</v>
+      </c>
     </row>
     <row r="30" spans="1:24" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="57" t="s">
@@ -48554,8 +48661,12 @@
       </c>
       <c r="U30" s="53"/>
       <c r="V30" s="54"/>
-      <c r="W30" s="53"/>
-      <c r="X30" s="70"/>
+      <c r="W30" s="53" t="s">
+        <v>513</v>
+      </c>
+      <c r="X30" s="70">
+        <v>0</v>
+      </c>
     </row>
     <row r="31" spans="1:24" ht="30.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="71" t="s">
@@ -48619,8 +48730,12 @@
       </c>
       <c r="U31" s="53"/>
       <c r="V31" s="54"/>
-      <c r="W31" s="53"/>
-      <c r="X31" s="70"/>
+      <c r="W31" s="53" t="s">
+        <v>513</v>
+      </c>
+      <c r="X31" s="70">
+        <v>4176</v>
+      </c>
     </row>
     <row r="32" spans="1:24" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="71" t="s">
@@ -48684,8 +48799,12 @@
       </c>
       <c r="U32" s="53"/>
       <c r="V32" s="54"/>
-      <c r="W32" s="53"/>
-      <c r="X32" s="70"/>
+      <c r="W32" s="53" t="s">
+        <v>513</v>
+      </c>
+      <c r="X32" s="70">
+        <v>0</v>
+      </c>
     </row>
     <row r="33" spans="1:24" ht="20.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="83" t="s">
@@ -48741,8 +48860,12 @@
       </c>
       <c r="U33" s="53"/>
       <c r="V33" s="54"/>
-      <c r="W33" s="53"/>
-      <c r="X33" s="70"/>
+      <c r="W33" s="53" t="s">
+        <v>513</v>
+      </c>
+      <c r="X33" s="70">
+        <v>4176</v>
+      </c>
     </row>
     <row r="34" spans="1:24" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="82" t="s">
@@ -48798,11 +48921,15 @@
       </c>
       <c r="U34" s="53"/>
       <c r="V34" s="54"/>
-      <c r="W34" s="53"/>
-      <c r="X34" s="70"/>
+      <c r="W34" s="53" t="s">
+        <v>513</v>
+      </c>
+      <c r="X34" s="70">
+        <v>0</v>
+      </c>
     </row>
     <row r="35" spans="1:24" ht="26.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="579" t="s">
+      <c r="A35" s="513" t="s">
         <v>477</v>
       </c>
       <c r="B35" s="93" t="s">
@@ -48849,8 +48976,12 @@
       </c>
       <c r="U35" s="53"/>
       <c r="V35" s="54"/>
-      <c r="W35" s="53"/>
-      <c r="X35" s="70"/>
+      <c r="W35" s="53" t="s">
+        <v>220</v>
+      </c>
+      <c r="X35" s="70">
+        <v>4176</v>
+      </c>
     </row>
     <row r="36" spans="1:24" ht="20.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="57"/>
@@ -48885,7 +49016,10 @@
       <c r="U36" s="53"/>
       <c r="V36" s="54"/>
       <c r="W36" s="53"/>
-      <c r="X36" s="70"/>
+      <c r="X36" s="70">
+        <f>SUM(X4:X35)</f>
+        <v>75168</v>
+      </c>
     </row>
     <row r="37" spans="1:24" ht="20.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="71"/>
@@ -50531,8 +50665,8 @@
         <v>0</v>
       </c>
       <c r="K87" s="100"/>
-      <c r="L87" s="535"/>
-      <c r="M87" s="536"/>
+      <c r="L87" s="543"/>
+      <c r="M87" s="544"/>
       <c r="N87" s="48">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -50564,8 +50698,8 @@
         <v>0</v>
       </c>
       <c r="K88" s="100"/>
-      <c r="L88" s="535"/>
-      <c r="M88" s="536"/>
+      <c r="L88" s="543"/>
+      <c r="M88" s="544"/>
       <c r="N88" s="48">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -50768,8 +50902,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O94" s="519"/>
-      <c r="P94" s="529"/>
+      <c r="O94" s="539"/>
+      <c r="P94" s="535"/>
       <c r="Q94" s="164"/>
       <c r="R94" s="129"/>
       <c r="S94" s="180"/>
@@ -50801,8 +50935,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O95" s="520"/>
-      <c r="P95" s="530"/>
+      <c r="O95" s="540"/>
+      <c r="P95" s="536"/>
       <c r="Q95" s="164"/>
       <c r="R95" s="129"/>
       <c r="S95" s="180"/>
@@ -56194,11 +56328,11 @@
         <f t="shared" si="12"/>
         <v>#VALUE!</v>
       </c>
-      <c r="F259" s="531" t="s">
+      <c r="F259" s="537" t="s">
         <v>26</v>
       </c>
-      <c r="G259" s="531"/>
-      <c r="H259" s="532"/>
+      <c r="G259" s="537"/>
+      <c r="H259" s="538"/>
       <c r="I259" s="317">
         <f>SUM(I4:I258)</f>
         <v>476389.92</v>
@@ -56826,49 +56960,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="42.75" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A1" s="537" t="s">
+      <c r="A1" s="514" t="s">
         <v>482</v>
       </c>
-      <c r="B1" s="537"/>
-      <c r="C1" s="537"/>
-      <c r="D1" s="537"/>
-      <c r="E1" s="537"/>
-      <c r="F1" s="537"/>
-      <c r="G1" s="537"/>
-      <c r="H1" s="537"/>
-      <c r="I1" s="537"/>
-      <c r="J1" s="537"/>
+      <c r="B1" s="514"/>
+      <c r="C1" s="514"/>
+      <c r="D1" s="514"/>
+      <c r="E1" s="514"/>
+      <c r="F1" s="514"/>
+      <c r="G1" s="514"/>
+      <c r="H1" s="514"/>
+      <c r="I1" s="514"/>
+      <c r="J1" s="514"/>
       <c r="K1" s="375"/>
       <c r="L1" s="375"/>
       <c r="M1" s="375"/>
       <c r="N1" s="375"/>
       <c r="O1" s="376"/>
-      <c r="S1" s="556" t="s">
+      <c r="S1" s="557" t="s">
         <v>142</v>
       </c>
-      <c r="T1" s="556"/>
+      <c r="T1" s="557"/>
       <c r="U1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="V1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="W1" s="538" t="s">
+      <c r="W1" s="515" t="s">
         <v>2</v>
       </c>
-      <c r="X1" s="539"/>
+      <c r="X1" s="516"/>
     </row>
     <row r="2" spans="1:24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="537"/>
-      <c r="B2" s="537"/>
-      <c r="C2" s="537"/>
-      <c r="D2" s="537"/>
-      <c r="E2" s="537"/>
-      <c r="F2" s="537"/>
-      <c r="G2" s="537"/>
-      <c r="H2" s="537"/>
-      <c r="I2" s="537"/>
-      <c r="J2" s="537"/>
+      <c r="A2" s="514"/>
+      <c r="B2" s="514"/>
+      <c r="C2" s="514"/>
+      <c r="D2" s="514"/>
+      <c r="E2" s="514"/>
+      <c r="F2" s="514"/>
+      <c r="G2" s="514"/>
+      <c r="H2" s="514"/>
+      <c r="I2" s="514"/>
+      <c r="J2" s="514"/>
       <c r="K2" s="377"/>
       <c r="L2" s="377"/>
       <c r="M2" s="377"/>
@@ -56876,8 +57010,8 @@
       <c r="O2" s="379"/>
       <c r="Q2" s="10"/>
       <c r="R2" s="11"/>
-      <c r="S2" s="557"/>
-      <c r="T2" s="557"/>
+      <c r="S2" s="558"/>
+      <c r="T2" s="558"/>
       <c r="U2" s="14"/>
       <c r="V2" s="15"/>
       <c r="W2" s="16"/>
@@ -56922,10 +57056,10 @@
       <c r="N3" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="540" t="s">
+      <c r="O3" s="517" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="541"/>
+      <c r="P3" s="518"/>
       <c r="Q3" s="30" t="s">
         <v>16</v>
       </c>
@@ -59932,8 +60066,8 @@
         <v>0</v>
       </c>
       <c r="K87" s="100"/>
-      <c r="L87" s="535"/>
-      <c r="M87" s="536"/>
+      <c r="L87" s="543"/>
+      <c r="M87" s="544"/>
       <c r="N87" s="48">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -59965,8 +60099,8 @@
         <v>0</v>
       </c>
       <c r="K88" s="100"/>
-      <c r="L88" s="535"/>
-      <c r="M88" s="536"/>
+      <c r="L88" s="543"/>
+      <c r="M88" s="544"/>
       <c r="N88" s="48">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -60169,8 +60303,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O94" s="519"/>
-      <c r="P94" s="529"/>
+      <c r="O94" s="539"/>
+      <c r="P94" s="535"/>
       <c r="Q94" s="164"/>
       <c r="R94" s="129"/>
       <c r="S94" s="180"/>
@@ -60202,8 +60336,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O95" s="520"/>
-      <c r="P95" s="530"/>
+      <c r="O95" s="540"/>
+      <c r="P95" s="536"/>
       <c r="Q95" s="164"/>
       <c r="R95" s="129"/>
       <c r="S95" s="180"/>
@@ -65595,11 +65729,11 @@
         <f t="shared" si="11"/>
         <v>#VALUE!</v>
       </c>
-      <c r="F259" s="531" t="s">
+      <c r="F259" s="537" t="s">
         <v>26</v>
       </c>
-      <c r="G259" s="531"/>
-      <c r="H259" s="532"/>
+      <c r="G259" s="537"/>
+      <c r="H259" s="538"/>
       <c r="I259" s="317">
         <f>SUM(I4:I258)</f>
         <v>138270</v>

</xml_diff>

<commit_message>
CIERRE  28 JUN 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #06  JUNIO 2022/ENTRADAS OBRADOR     J U N I O         2022.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #06  JUNIO 2022/ENTRADAS OBRADOR     J U N I O         2022.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16365" windowHeight="10305" firstSheet="4" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16365" windowHeight="10305" firstSheet="4" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="CANALES  ENERO  2022   " sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1536" uniqueCount="522">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1548" uniqueCount="529">
   <si>
     <t>FECHA DE PAGO</t>
   </si>
@@ -1554,15 +1554,6 @@
     <t>20558--11028--NC-524</t>
   </si>
   <si>
-    <t>20602--</t>
-  </si>
-  <si>
-    <t>20637--</t>
-  </si>
-  <si>
-    <t>20645--</t>
-  </si>
-  <si>
     <t>20575--11033-NC-523</t>
   </si>
   <si>
@@ -1570,9 +1561,6 @@
   </si>
   <si>
     <t>20592--11043</t>
-  </si>
-  <si>
-    <t>20663--</t>
   </si>
   <si>
     <t>20678--</t>
@@ -1609,6 +1597,39 @@
   </si>
   <si>
     <t>20645--4814</t>
+  </si>
+  <si>
+    <t>20663--6862</t>
+  </si>
+  <si>
+    <t>20700--</t>
+  </si>
+  <si>
+    <t>20717--</t>
+  </si>
+  <si>
+    <t>20735--</t>
+  </si>
+  <si>
+    <t>20743--</t>
+  </si>
+  <si>
+    <t>20645--11075</t>
+  </si>
+  <si>
+    <t>20637--4812</t>
+  </si>
+  <si>
+    <t>20637--11072</t>
+  </si>
+  <si>
+    <t>20602--11050--nc-526</t>
+  </si>
+  <si>
+    <t>38366--</t>
+  </si>
+  <si>
+    <t>20602--11052</t>
   </si>
 </sst>
 </file>
@@ -4357,6 +4378,78 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="31" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="31" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="11" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="11" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="26" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="26" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4390,83 +4483,11 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="11" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="11" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="22" fillId="11" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="22" fillId="11" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="26" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="26" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="31" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="31" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -4496,6 +4517,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="32" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="32" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4529,12 +4556,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="18" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="32" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="32" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="11" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4884,18 +4905,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="42.75" thickBot="1" x14ac:dyDescent="0.7">
-      <c r="A1" s="514" t="s">
+      <c r="A1" s="538" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="514"/>
-      <c r="C1" s="514"/>
-      <c r="D1" s="514"/>
-      <c r="E1" s="514"/>
-      <c r="F1" s="514"/>
-      <c r="G1" s="514"/>
-      <c r="H1" s="514"/>
-      <c r="I1" s="514"/>
-      <c r="J1" s="514"/>
+      <c r="B1" s="538"/>
+      <c r="C1" s="538"/>
+      <c r="D1" s="538"/>
+      <c r="E1" s="538"/>
+      <c r="F1" s="538"/>
+      <c r="G1" s="538"/>
+      <c r="H1" s="538"/>
+      <c r="I1" s="538"/>
+      <c r="J1" s="538"/>
       <c r="K1" s="375"/>
       <c r="L1" s="375"/>
       <c r="M1" s="375"/>
@@ -4909,22 +4930,22 @@
       <c r="V1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="W1" s="515" t="s">
+      <c r="W1" s="539" t="s">
         <v>2</v>
       </c>
-      <c r="X1" s="516"/>
+      <c r="X1" s="540"/>
     </row>
     <row r="2" spans="1:24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="514"/>
-      <c r="B2" s="514"/>
-      <c r="C2" s="514"/>
-      <c r="D2" s="514"/>
-      <c r="E2" s="514"/>
-      <c r="F2" s="514"/>
-      <c r="G2" s="514"/>
-      <c r="H2" s="514"/>
-      <c r="I2" s="514"/>
-      <c r="J2" s="514"/>
+      <c r="A2" s="538"/>
+      <c r="B2" s="538"/>
+      <c r="C2" s="538"/>
+      <c r="D2" s="538"/>
+      <c r="E2" s="538"/>
+      <c r="F2" s="538"/>
+      <c r="G2" s="538"/>
+      <c r="H2" s="538"/>
+      <c r="I2" s="538"/>
+      <c r="J2" s="538"/>
       <c r="K2" s="377"/>
       <c r="L2" s="377"/>
       <c r="M2" s="377"/>
@@ -4978,10 +4999,10 @@
       <c r="N3" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="517" t="s">
+      <c r="O3" s="541" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="518"/>
+      <c r="P3" s="542"/>
       <c r="Q3" s="30" t="s">
         <v>16</v>
       </c>
@@ -5525,7 +5546,7 @@
       <c r="B12" s="58" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="519" t="s">
+      <c r="C12" s="543" t="s">
         <v>103</v>
       </c>
       <c r="D12" s="400"/>
@@ -5589,7 +5610,7 @@
       <c r="B13" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="520"/>
+      <c r="C13" s="544"/>
       <c r="D13" s="400"/>
       <c r="E13" s="401"/>
       <c r="F13" s="402">
@@ -7591,13 +7612,13 @@
       <c r="V55" s="160"/>
     </row>
     <row r="56" spans="1:24" s="161" customFormat="1" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="531" t="s">
+      <c r="A56" s="522" t="s">
         <v>41</v>
       </c>
       <c r="B56" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="C56" s="533" t="s">
+      <c r="C56" s="524" t="s">
         <v>110</v>
       </c>
       <c r="D56" s="150"/>
@@ -7608,7 +7629,7 @@
       <c r="G56" s="152">
         <v>44571</v>
       </c>
-      <c r="H56" s="525">
+      <c r="H56" s="526">
         <v>782</v>
       </c>
       <c r="I56" s="151">
@@ -7637,11 +7658,11 @@
       <c r="V56" s="160"/>
     </row>
     <row r="57" spans="1:24" s="161" customFormat="1" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="532"/>
+      <c r="A57" s="523"/>
       <c r="B57" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="C57" s="534"/>
+      <c r="C57" s="525"/>
       <c r="D57" s="150"/>
       <c r="E57" s="40"/>
       <c r="F57" s="151">
@@ -7650,7 +7671,7 @@
       <c r="G57" s="152">
         <v>44571</v>
       </c>
-      <c r="H57" s="526"/>
+      <c r="H57" s="527"/>
       <c r="I57" s="151">
         <v>319</v>
       </c>
@@ -7677,13 +7698,13 @@
       <c r="V57" s="160"/>
     </row>
     <row r="58" spans="1:24" s="161" customFormat="1" ht="29.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="531" t="s">
+      <c r="A58" s="522" t="s">
         <v>41</v>
       </c>
       <c r="B58" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="C58" s="533" t="s">
+      <c r="C58" s="524" t="s">
         <v>129</v>
       </c>
       <c r="D58" s="150"/>
@@ -7694,7 +7715,7 @@
       <c r="G58" s="152">
         <v>44578</v>
       </c>
-      <c r="H58" s="525">
+      <c r="H58" s="526">
         <v>810</v>
       </c>
       <c r="I58" s="151">
@@ -7713,10 +7734,10 @@
         <f t="shared" si="1"/>
         <v>75875.8</v>
       </c>
-      <c r="O58" s="527" t="s">
+      <c r="O58" s="528" t="s">
         <v>59</v>
       </c>
-      <c r="P58" s="529">
+      <c r="P58" s="549">
         <v>44606</v>
       </c>
       <c r="Q58" s="128"/>
@@ -7727,11 +7748,11 @@
       <c r="V58" s="160"/>
     </row>
     <row r="59" spans="1:24" s="161" customFormat="1" ht="29.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="532"/>
+      <c r="A59" s="523"/>
       <c r="B59" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="C59" s="534"/>
+      <c r="C59" s="525"/>
       <c r="D59" s="150"/>
       <c r="E59" s="40"/>
       <c r="F59" s="151">
@@ -7740,7 +7761,7 @@
       <c r="G59" s="152">
         <v>44578</v>
       </c>
-      <c r="H59" s="526"/>
+      <c r="H59" s="527"/>
       <c r="I59" s="151">
         <v>220</v>
       </c>
@@ -7757,8 +7778,8 @@
         <f t="shared" si="1"/>
         <v>22440</v>
       </c>
-      <c r="O59" s="528"/>
-      <c r="P59" s="530"/>
+      <c r="O59" s="529"/>
+      <c r="P59" s="550"/>
       <c r="Q59" s="128"/>
       <c r="R59" s="158"/>
       <c r="S59" s="92"/>
@@ -7767,13 +7788,13 @@
       <c r="V59" s="160"/>
     </row>
     <row r="60" spans="1:24" s="161" customFormat="1" ht="48.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="523" t="s">
+      <c r="A60" s="547" t="s">
         <v>41</v>
       </c>
       <c r="B60" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="C60" s="521" t="s">
+      <c r="C60" s="545" t="s">
         <v>109</v>
       </c>
       <c r="D60" s="163"/>
@@ -7787,7 +7808,7 @@
       <c r="G60" s="152">
         <v>44585</v>
       </c>
-      <c r="H60" s="525">
+      <c r="H60" s="526">
         <v>800</v>
       </c>
       <c r="I60" s="151">
@@ -7806,10 +7827,10 @@
         <f t="shared" si="1"/>
         <v>151187.4</v>
       </c>
-      <c r="O60" s="527" t="s">
+      <c r="O60" s="528" t="s">
         <v>59</v>
       </c>
-      <c r="P60" s="529">
+      <c r="P60" s="549">
         <v>44594</v>
       </c>
       <c r="Q60" s="164"/>
@@ -7822,11 +7843,11 @@
       <c r="X60"/>
     </row>
     <row r="61" spans="1:24" ht="26.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="524"/>
+      <c r="A61" s="548"/>
       <c r="B61" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="C61" s="522"/>
+      <c r="C61" s="546"/>
       <c r="D61" s="165"/>
       <c r="E61" s="40">
         <f t="shared" si="2"/>
@@ -7838,7 +7859,7 @@
       <c r="G61" s="152">
         <v>44585</v>
       </c>
-      <c r="H61" s="526"/>
+      <c r="H61" s="527"/>
       <c r="I61" s="151">
         <v>231.6</v>
       </c>
@@ -7855,8 +7876,8 @@
         <f t="shared" si="1"/>
         <v>23623.200000000001</v>
       </c>
-      <c r="O61" s="528"/>
-      <c r="P61" s="530"/>
+      <c r="O61" s="529"/>
+      <c r="P61" s="550"/>
       <c r="Q61" s="164"/>
       <c r="R61" s="129"/>
       <c r="S61" s="92"/>
@@ -7922,7 +7943,7 @@
       <c r="B63" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="C63" s="547"/>
+      <c r="C63" s="516"/>
       <c r="D63" s="163"/>
       <c r="E63" s="40">
         <f t="shared" si="2"/>
@@ -7930,7 +7951,7 @@
       </c>
       <c r="F63" s="151"/>
       <c r="G63" s="152"/>
-      <c r="H63" s="549"/>
+      <c r="H63" s="518"/>
       <c r="I63" s="151"/>
       <c r="J63" s="45">
         <f t="shared" si="0"/>
@@ -7959,7 +7980,7 @@
       <c r="B64" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="C64" s="548"/>
+      <c r="C64" s="517"/>
       <c r="D64" s="168"/>
       <c r="E64" s="40">
         <f t="shared" si="2"/>
@@ -7967,7 +7988,7 @@
       </c>
       <c r="F64" s="151"/>
       <c r="G64" s="152"/>
-      <c r="H64" s="550"/>
+      <c r="H64" s="519"/>
       <c r="I64" s="151"/>
       <c r="J64" s="45">
         <f t="shared" si="0"/>
@@ -8145,8 +8166,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O68" s="539"/>
-      <c r="P68" s="545"/>
+      <c r="O68" s="520"/>
+      <c r="P68" s="514"/>
       <c r="Q68" s="164"/>
       <c r="R68" s="129"/>
       <c r="S68" s="180"/>
@@ -8180,8 +8201,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O69" s="540"/>
-      <c r="P69" s="546"/>
+      <c r="O69" s="521"/>
+      <c r="P69" s="515"/>
       <c r="Q69" s="164"/>
       <c r="R69" s="129"/>
       <c r="S69" s="180"/>
@@ -8671,8 +8692,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O82" s="539"/>
-      <c r="P82" s="541"/>
+      <c r="O82" s="520"/>
+      <c r="P82" s="534"/>
       <c r="Q82" s="164"/>
       <c r="R82" s="129"/>
       <c r="S82" s="180"/>
@@ -8704,8 +8725,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O83" s="540"/>
-      <c r="P83" s="542"/>
+      <c r="O83" s="521"/>
+      <c r="P83" s="535"/>
       <c r="Q83" s="164"/>
       <c r="R83" s="129"/>
       <c r="S83" s="180"/>
@@ -8737,8 +8758,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O84" s="539"/>
-      <c r="P84" s="541"/>
+      <c r="O84" s="520"/>
+      <c r="P84" s="534"/>
       <c r="Q84" s="164"/>
       <c r="R84" s="158"/>
       <c r="S84" s="180"/>
@@ -8770,8 +8791,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O85" s="540"/>
-      <c r="P85" s="542"/>
+      <c r="O85" s="521"/>
+      <c r="P85" s="535"/>
       <c r="Q85" s="164"/>
       <c r="R85" s="158"/>
       <c r="S85" s="180"/>
@@ -8929,8 +8950,8 @@
         <v>0</v>
       </c>
       <c r="K90" s="100"/>
-      <c r="L90" s="543"/>
-      <c r="M90" s="544"/>
+      <c r="L90" s="536"/>
+      <c r="M90" s="537"/>
       <c r="N90" s="77">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -8962,8 +8983,8 @@
         <v>0</v>
       </c>
       <c r="K91" s="100"/>
-      <c r="L91" s="543"/>
-      <c r="M91" s="544"/>
+      <c r="L91" s="536"/>
+      <c r="M91" s="537"/>
       <c r="N91" s="77">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -9166,8 +9187,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O97" s="539"/>
-      <c r="P97" s="535"/>
+      <c r="O97" s="520"/>
+      <c r="P97" s="530"/>
       <c r="Q97" s="164"/>
       <c r="R97" s="129"/>
       <c r="S97" s="180"/>
@@ -9199,8 +9220,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O98" s="540"/>
-      <c r="P98" s="536"/>
+      <c r="O98" s="521"/>
+      <c r="P98" s="531"/>
       <c r="Q98" s="164"/>
       <c r="R98" s="129"/>
       <c r="S98" s="180"/>
@@ -14592,11 +14613,11 @@
         <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
-      <c r="F262" s="537" t="s">
+      <c r="F262" s="532" t="s">
         <v>26</v>
       </c>
-      <c r="G262" s="537"/>
-      <c r="H262" s="538"/>
+      <c r="G262" s="532"/>
+      <c r="H262" s="533"/>
       <c r="I262" s="317">
         <f>SUM(I4:I261)</f>
         <v>426245.47000000003</v>
@@ -15170,22 +15191,6 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="P68:P69"/>
-    <mergeCell ref="C63:C64"/>
-    <mergeCell ref="H63:H64"/>
-    <mergeCell ref="O68:O69"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="C58:C59"/>
-    <mergeCell ref="H58:H59"/>
-    <mergeCell ref="O58:O59"/>
-    <mergeCell ref="P97:P98"/>
-    <mergeCell ref="F262:H262"/>
-    <mergeCell ref="O82:O83"/>
-    <mergeCell ref="P82:P83"/>
-    <mergeCell ref="O84:O85"/>
-    <mergeCell ref="P84:P85"/>
-    <mergeCell ref="L90:M91"/>
-    <mergeCell ref="O97:O98"/>
     <mergeCell ref="A1:J2"/>
     <mergeCell ref="W1:X1"/>
     <mergeCell ref="O3:P3"/>
@@ -15199,6 +15204,22 @@
     <mergeCell ref="C56:C57"/>
     <mergeCell ref="H56:H57"/>
     <mergeCell ref="P58:P59"/>
+    <mergeCell ref="P97:P98"/>
+    <mergeCell ref="F262:H262"/>
+    <mergeCell ref="O82:O83"/>
+    <mergeCell ref="P82:P83"/>
+    <mergeCell ref="O84:O85"/>
+    <mergeCell ref="P84:P85"/>
+    <mergeCell ref="L90:M91"/>
+    <mergeCell ref="O97:O98"/>
+    <mergeCell ref="P68:P69"/>
+    <mergeCell ref="C63:C64"/>
+    <mergeCell ref="H63:H64"/>
+    <mergeCell ref="O68:O69"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="H58:H59"/>
+    <mergeCell ref="O58:O59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -15242,18 +15263,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="42.75" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A1" s="514" t="s">
+      <c r="A1" s="538" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="514"/>
-      <c r="C1" s="514"/>
-      <c r="D1" s="514"/>
-      <c r="E1" s="514"/>
-      <c r="F1" s="514"/>
-      <c r="G1" s="514"/>
-      <c r="H1" s="514"/>
-      <c r="I1" s="514"/>
-      <c r="J1" s="514"/>
+      <c r="B1" s="538"/>
+      <c r="C1" s="538"/>
+      <c r="D1" s="538"/>
+      <c r="E1" s="538"/>
+      <c r="F1" s="538"/>
+      <c r="G1" s="538"/>
+      <c r="H1" s="538"/>
+      <c r="I1" s="538"/>
+      <c r="J1" s="538"/>
       <c r="K1" s="375"/>
       <c r="L1" s="375"/>
       <c r="M1" s="375"/>
@@ -15269,22 +15290,22 @@
       <c r="V1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="W1" s="515" t="s">
+      <c r="W1" s="539" t="s">
         <v>2</v>
       </c>
-      <c r="X1" s="516"/>
+      <c r="X1" s="540"/>
     </row>
     <row r="2" spans="1:24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="514"/>
-      <c r="B2" s="514"/>
-      <c r="C2" s="514"/>
-      <c r="D2" s="514"/>
-      <c r="E2" s="514"/>
-      <c r="F2" s="514"/>
-      <c r="G2" s="514"/>
-      <c r="H2" s="514"/>
-      <c r="I2" s="514"/>
-      <c r="J2" s="514"/>
+      <c r="A2" s="538"/>
+      <c r="B2" s="538"/>
+      <c r="C2" s="538"/>
+      <c r="D2" s="538"/>
+      <c r="E2" s="538"/>
+      <c r="F2" s="538"/>
+      <c r="G2" s="538"/>
+      <c r="H2" s="538"/>
+      <c r="I2" s="538"/>
+      <c r="J2" s="538"/>
       <c r="K2" s="377"/>
       <c r="L2" s="377"/>
       <c r="M2" s="377"/>
@@ -15338,10 +15359,10 @@
       <c r="N3" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="517" t="s">
+      <c r="O3" s="541" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="518"/>
+      <c r="P3" s="542"/>
       <c r="Q3" s="30" t="s">
         <v>16</v>
       </c>
@@ -17983,7 +18004,7 @@
       <c r="B55" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="C55" s="533" t="s">
+      <c r="C55" s="524" t="s">
         <v>160</v>
       </c>
       <c r="D55" s="150"/>
@@ -17994,7 +18015,7 @@
       <c r="G55" s="152">
         <v>44599</v>
       </c>
-      <c r="H55" s="549" t="s">
+      <c r="H55" s="518" t="s">
         <v>161</v>
       </c>
       <c r="I55" s="151">
@@ -18027,7 +18048,7 @@
       <c r="B56" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="C56" s="534"/>
+      <c r="C56" s="525"/>
       <c r="D56" s="163"/>
       <c r="E56" s="40"/>
       <c r="F56" s="151">
@@ -18036,7 +18057,7 @@
       <c r="G56" s="152">
         <v>44599</v>
       </c>
-      <c r="H56" s="550"/>
+      <c r="H56" s="519"/>
       <c r="I56" s="151">
         <v>194.4</v>
       </c>
@@ -18082,7 +18103,7 @@
       <c r="G57" s="152">
         <v>44606</v>
       </c>
-      <c r="H57" s="549" t="s">
+      <c r="H57" s="518" t="s">
         <v>163</v>
       </c>
       <c r="I57" s="151">
@@ -18101,10 +18122,10 @@
         <f t="shared" si="1"/>
         <v>35776</v>
       </c>
-      <c r="O57" s="539" t="s">
+      <c r="O57" s="520" t="s">
         <v>59</v>
       </c>
-      <c r="P57" s="545">
+      <c r="P57" s="514">
         <v>44620</v>
       </c>
       <c r="Q57" s="164"/>
@@ -18128,7 +18149,7 @@
       <c r="G58" s="152">
         <v>44606</v>
       </c>
-      <c r="H58" s="550"/>
+      <c r="H58" s="519"/>
       <c r="I58" s="151">
         <v>627.60209999999995</v>
       </c>
@@ -18172,7 +18193,7 @@
       <c r="G59" s="152">
         <v>44613</v>
       </c>
-      <c r="H59" s="549" t="s">
+      <c r="H59" s="518" t="s">
         <v>225</v>
       </c>
       <c r="I59" s="151">
@@ -18216,7 +18237,7 @@
       <c r="E60" s="40"/>
       <c r="F60" s="151"/>
       <c r="G60" s="152"/>
-      <c r="H60" s="550"/>
+      <c r="H60" s="519"/>
       <c r="I60" s="151"/>
       <c r="J60" s="45">
         <f t="shared" si="0"/>
@@ -18879,8 +18900,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O79" s="539"/>
-      <c r="P79" s="541"/>
+      <c r="O79" s="520"/>
+      <c r="P79" s="534"/>
       <c r="Q79" s="164"/>
       <c r="R79" s="129"/>
       <c r="S79" s="180"/>
@@ -18909,8 +18930,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O80" s="540"/>
-      <c r="P80" s="542"/>
+      <c r="O80" s="521"/>
+      <c r="P80" s="535"/>
       <c r="Q80" s="164"/>
       <c r="R80" s="129"/>
       <c r="S80" s="180"/>
@@ -18939,8 +18960,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O81" s="539"/>
-      <c r="P81" s="541"/>
+      <c r="O81" s="520"/>
+      <c r="P81" s="534"/>
       <c r="Q81" s="164"/>
       <c r="R81" s="158"/>
       <c r="S81" s="180"/>
@@ -18972,8 +18993,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O82" s="540"/>
-      <c r="P82" s="542"/>
+      <c r="O82" s="521"/>
+      <c r="P82" s="535"/>
       <c r="Q82" s="164"/>
       <c r="R82" s="158"/>
       <c r="S82" s="180"/>
@@ -19131,8 +19152,8 @@
         <v>0</v>
       </c>
       <c r="K87" s="100"/>
-      <c r="L87" s="543"/>
-      <c r="M87" s="544"/>
+      <c r="L87" s="536"/>
+      <c r="M87" s="537"/>
       <c r="N87" s="77">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -19164,8 +19185,8 @@
         <v>0</v>
       </c>
       <c r="K88" s="100"/>
-      <c r="L88" s="543"/>
-      <c r="M88" s="544"/>
+      <c r="L88" s="536"/>
+      <c r="M88" s="537"/>
       <c r="N88" s="77">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -19368,8 +19389,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O94" s="539"/>
-      <c r="P94" s="535"/>
+      <c r="O94" s="520"/>
+      <c r="P94" s="530"/>
       <c r="Q94" s="164"/>
       <c r="R94" s="129"/>
       <c r="S94" s="180"/>
@@ -19401,8 +19422,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O95" s="540"/>
-      <c r="P95" s="536"/>
+      <c r="O95" s="521"/>
+      <c r="P95" s="531"/>
       <c r="Q95" s="164"/>
       <c r="R95" s="129"/>
       <c r="S95" s="180"/>
@@ -24794,11 +24815,11 @@
         <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
-      <c r="F259" s="537" t="s">
+      <c r="F259" s="532" t="s">
         <v>26</v>
       </c>
-      <c r="G259" s="537"/>
-      <c r="H259" s="538"/>
+      <c r="G259" s="532"/>
+      <c r="H259" s="533"/>
       <c r="I259" s="317">
         <f>SUM(I4:I258)</f>
         <v>387207.97210000001</v>
@@ -25372,6 +25393,12 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="F259:H259"/>
+    <mergeCell ref="O81:O82"/>
+    <mergeCell ref="P81:P82"/>
+    <mergeCell ref="L87:M88"/>
+    <mergeCell ref="O94:O95"/>
+    <mergeCell ref="P94:P95"/>
     <mergeCell ref="O79:O80"/>
     <mergeCell ref="P79:P80"/>
     <mergeCell ref="A1:J2"/>
@@ -25387,12 +25414,6 @@
     <mergeCell ref="C55:C56"/>
     <mergeCell ref="A55:A56"/>
     <mergeCell ref="H55:H56"/>
-    <mergeCell ref="F259:H259"/>
-    <mergeCell ref="O81:O82"/>
-    <mergeCell ref="P81:P82"/>
-    <mergeCell ref="L87:M88"/>
-    <mergeCell ref="O94:O95"/>
-    <mergeCell ref="P94:P95"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -25439,18 +25460,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="42.75" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A1" s="514" t="s">
+      <c r="A1" s="538" t="s">
         <v>189</v>
       </c>
-      <c r="B1" s="514"/>
-      <c r="C1" s="514"/>
-      <c r="D1" s="514"/>
-      <c r="E1" s="514"/>
-      <c r="F1" s="514"/>
-      <c r="G1" s="514"/>
-      <c r="H1" s="514"/>
-      <c r="I1" s="514"/>
-      <c r="J1" s="514"/>
+      <c r="B1" s="538"/>
+      <c r="C1" s="538"/>
+      <c r="D1" s="538"/>
+      <c r="E1" s="538"/>
+      <c r="F1" s="538"/>
+      <c r="G1" s="538"/>
+      <c r="H1" s="538"/>
+      <c r="I1" s="538"/>
+      <c r="J1" s="538"/>
       <c r="K1" s="375"/>
       <c r="L1" s="375"/>
       <c r="M1" s="375"/>
@@ -25466,22 +25487,22 @@
       <c r="V1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="W1" s="515" t="s">
+      <c r="W1" s="539" t="s">
         <v>2</v>
       </c>
-      <c r="X1" s="516"/>
+      <c r="X1" s="540"/>
     </row>
     <row r="2" spans="1:24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="514"/>
-      <c r="B2" s="514"/>
-      <c r="C2" s="514"/>
-      <c r="D2" s="514"/>
-      <c r="E2" s="514"/>
-      <c r="F2" s="514"/>
-      <c r="G2" s="514"/>
-      <c r="H2" s="514"/>
-      <c r="I2" s="514"/>
-      <c r="J2" s="514"/>
+      <c r="A2" s="538"/>
+      <c r="B2" s="538"/>
+      <c r="C2" s="538"/>
+      <c r="D2" s="538"/>
+      <c r="E2" s="538"/>
+      <c r="F2" s="538"/>
+      <c r="G2" s="538"/>
+      <c r="H2" s="538"/>
+      <c r="I2" s="538"/>
+      <c r="J2" s="538"/>
       <c r="K2" s="377"/>
       <c r="L2" s="377"/>
       <c r="M2" s="377"/>
@@ -25535,10 +25556,10 @@
       <c r="N3" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="517" t="s">
+      <c r="O3" s="541" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="518"/>
+      <c r="P3" s="542"/>
       <c r="Q3" s="30" t="s">
         <v>16</v>
       </c>
@@ -28752,7 +28773,7 @@
       <c r="B55" s="438" t="s">
         <v>24</v>
       </c>
-      <c r="C55" s="533" t="s">
+      <c r="C55" s="524" t="s">
         <v>229</v>
       </c>
       <c r="D55" s="439"/>
@@ -28763,7 +28784,7 @@
       <c r="G55" s="152">
         <v>44627</v>
       </c>
-      <c r="H55" s="562" t="s">
+      <c r="H55" s="564" t="s">
         <v>230</v>
       </c>
       <c r="I55" s="151">
@@ -28782,10 +28803,10 @@
         <f t="shared" si="1"/>
         <v>18886.399999999998</v>
       </c>
-      <c r="O55" s="539" t="s">
+      <c r="O55" s="520" t="s">
         <v>59</v>
       </c>
-      <c r="P55" s="545">
+      <c r="P55" s="514">
         <v>44645</v>
       </c>
       <c r="Q55" s="128"/>
@@ -28796,11 +28817,11 @@
       <c r="V55" s="160"/>
     </row>
     <row r="56" spans="1:24" s="161" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="561"/>
+      <c r="A56" s="563"/>
       <c r="B56" s="438" t="s">
         <v>24</v>
       </c>
-      <c r="C56" s="534"/>
+      <c r="C56" s="525"/>
       <c r="D56" s="440"/>
       <c r="E56" s="60"/>
       <c r="F56" s="151">
@@ -28809,7 +28830,7 @@
       <c r="G56" s="152">
         <v>44627</v>
       </c>
-      <c r="H56" s="563"/>
+      <c r="H56" s="565"/>
       <c r="I56" s="151">
         <v>967</v>
       </c>
@@ -28826,8 +28847,8 @@
         <f t="shared" si="1"/>
         <v>92832</v>
       </c>
-      <c r="O56" s="540"/>
-      <c r="P56" s="546"/>
+      <c r="O56" s="521"/>
+      <c r="P56" s="515"/>
       <c r="Q56" s="164"/>
       <c r="R56" s="158"/>
       <c r="S56" s="92"/>
@@ -28888,13 +28909,13 @@
       <c r="V57" s="54"/>
     </row>
     <row r="58" spans="1:24" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="523" t="s">
+      <c r="A58" s="547" t="s">
         <v>41</v>
       </c>
       <c r="B58" s="170" t="s">
         <v>24</v>
       </c>
-      <c r="C58" s="572" t="s">
+      <c r="C58" s="561" t="s">
         <v>319</v>
       </c>
       <c r="D58" s="165"/>
@@ -28905,7 +28926,7 @@
       <c r="G58" s="152">
         <v>44648</v>
       </c>
-      <c r="H58" s="570" t="s">
+      <c r="H58" s="572" t="s">
         <v>315</v>
       </c>
       <c r="I58" s="151">
@@ -28924,10 +28945,10 @@
         <f t="shared" si="1"/>
         <v>35255.600000000006</v>
       </c>
-      <c r="O58" s="527" t="s">
+      <c r="O58" s="528" t="s">
         <v>59</v>
       </c>
-      <c r="P58" s="529">
+      <c r="P58" s="549">
         <v>44662</v>
       </c>
       <c r="Q58" s="164"/>
@@ -28938,11 +28959,11 @@
       <c r="V58" s="54"/>
     </row>
     <row r="59" spans="1:24" s="161" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="524"/>
+      <c r="A59" s="548"/>
       <c r="B59" s="170" t="s">
         <v>23</v>
       </c>
-      <c r="C59" s="573"/>
+      <c r="C59" s="562"/>
       <c r="D59" s="163"/>
       <c r="E59" s="60"/>
       <c r="F59" s="151">
@@ -28951,7 +28972,7 @@
       <c r="G59" s="152">
         <v>44648</v>
       </c>
-      <c r="H59" s="571"/>
+      <c r="H59" s="573"/>
       <c r="I59" s="151">
         <v>719</v>
       </c>
@@ -28968,8 +28989,8 @@
         <f t="shared" si="1"/>
         <v>69024</v>
       </c>
-      <c r="O59" s="528"/>
-      <c r="P59" s="530"/>
+      <c r="O59" s="529"/>
+      <c r="P59" s="550"/>
       <c r="Q59" s="164"/>
       <c r="R59" s="158"/>
       <c r="S59" s="92"/>
@@ -29042,13 +29063,13 @@
       <c r="V61" s="54"/>
     </row>
     <row r="62" spans="1:24" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A62" s="564" t="s">
+      <c r="A62" s="566" t="s">
         <v>106</v>
       </c>
       <c r="B62" s="178" t="s">
         <v>237</v>
       </c>
-      <c r="C62" s="566" t="s">
+      <c r="C62" s="568" t="s">
         <v>238</v>
       </c>
       <c r="D62" s="168"/>
@@ -29059,7 +29080,7 @@
       <c r="G62" s="152">
         <v>44622</v>
       </c>
-      <c r="H62" s="568">
+      <c r="H62" s="570">
         <v>37162</v>
       </c>
       <c r="I62" s="151">
@@ -29078,10 +29099,10 @@
         <f t="shared" si="1"/>
         <v>7782.5999999999995</v>
       </c>
-      <c r="O62" s="539" t="s">
+      <c r="O62" s="520" t="s">
         <v>61</v>
       </c>
-      <c r="P62" s="545">
+      <c r="P62" s="514">
         <v>44643</v>
       </c>
       <c r="Q62" s="164"/>
@@ -29092,11 +29113,11 @@
       <c r="V62" s="54"/>
     </row>
     <row r="63" spans="1:24" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A63" s="565"/>
+      <c r="A63" s="567"/>
       <c r="B63" s="178" t="s">
         <v>239</v>
       </c>
-      <c r="C63" s="567"/>
+      <c r="C63" s="569"/>
       <c r="D63" s="168"/>
       <c r="E63" s="60"/>
       <c r="F63" s="151">
@@ -29105,7 +29126,7 @@
       <c r="G63" s="152">
         <v>44622</v>
       </c>
-      <c r="H63" s="569"/>
+      <c r="H63" s="571"/>
       <c r="I63" s="151">
         <v>204.8</v>
       </c>
@@ -29122,8 +29143,8 @@
         <f t="shared" si="1"/>
         <v>16998.400000000001</v>
       </c>
-      <c r="O63" s="540"/>
-      <c r="P63" s="546"/>
+      <c r="O63" s="521"/>
+      <c r="P63" s="515"/>
       <c r="Q63" s="164"/>
       <c r="R63" s="129"/>
       <c r="S63" s="92"/>
@@ -29602,8 +29623,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O79" s="539"/>
-      <c r="P79" s="541"/>
+      <c r="O79" s="520"/>
+      <c r="P79" s="534"/>
       <c r="Q79" s="164"/>
       <c r="R79" s="129"/>
       <c r="S79" s="180"/>
@@ -29632,8 +29653,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O80" s="540"/>
-      <c r="P80" s="542"/>
+      <c r="O80" s="521"/>
+      <c r="P80" s="535"/>
       <c r="Q80" s="164"/>
       <c r="R80" s="129"/>
       <c r="S80" s="180"/>
@@ -29662,8 +29683,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O81" s="539"/>
-      <c r="P81" s="541"/>
+      <c r="O81" s="520"/>
+      <c r="P81" s="534"/>
       <c r="Q81" s="164"/>
       <c r="R81" s="158"/>
       <c r="S81" s="180"/>
@@ -29695,8 +29716,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O82" s="540"/>
-      <c r="P82" s="542"/>
+      <c r="O82" s="521"/>
+      <c r="P82" s="535"/>
       <c r="Q82" s="164"/>
       <c r="R82" s="158"/>
       <c r="S82" s="180"/>
@@ -29854,8 +29875,8 @@
         <v>0</v>
       </c>
       <c r="K87" s="100"/>
-      <c r="L87" s="543"/>
-      <c r="M87" s="544"/>
+      <c r="L87" s="536"/>
+      <c r="M87" s="537"/>
       <c r="N87" s="48">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -29887,8 +29908,8 @@
         <v>0</v>
       </c>
       <c r="K88" s="100"/>
-      <c r="L88" s="543"/>
-      <c r="M88" s="544"/>
+      <c r="L88" s="536"/>
+      <c r="M88" s="537"/>
       <c r="N88" s="48">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -30091,8 +30112,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O94" s="539"/>
-      <c r="P94" s="535"/>
+      <c r="O94" s="520"/>
+      <c r="P94" s="530"/>
       <c r="Q94" s="164"/>
       <c r="R94" s="129"/>
       <c r="S94" s="180"/>
@@ -30124,8 +30145,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O95" s="540"/>
-      <c r="P95" s="536"/>
+      <c r="O95" s="521"/>
+      <c r="P95" s="531"/>
       <c r="Q95" s="164"/>
       <c r="R95" s="129"/>
       <c r="S95" s="180"/>
@@ -35517,11 +35538,11 @@
         <f t="shared" si="10"/>
         <v>#VALUE!</v>
       </c>
-      <c r="F259" s="537" t="s">
+      <c r="F259" s="532" t="s">
         <v>26</v>
       </c>
-      <c r="G259" s="537"/>
-      <c r="H259" s="538"/>
+      <c r="G259" s="532"/>
+      <c r="H259" s="533"/>
       <c r="I259" s="317">
         <f>SUM(I4:I258)</f>
         <v>517031.52999999991</v>
@@ -36095,17 +36116,6 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="O58:O59"/>
-    <mergeCell ref="P58:P59"/>
-    <mergeCell ref="C58:C59"/>
-    <mergeCell ref="O94:O95"/>
-    <mergeCell ref="P94:P95"/>
-    <mergeCell ref="F259:H259"/>
-    <mergeCell ref="O79:O80"/>
-    <mergeCell ref="P79:P80"/>
-    <mergeCell ref="O81:O82"/>
-    <mergeCell ref="P81:P82"/>
     <mergeCell ref="A1:J2"/>
     <mergeCell ref="S1:T2"/>
     <mergeCell ref="W1:X1"/>
@@ -36122,6 +36132,17 @@
     <mergeCell ref="O62:O63"/>
     <mergeCell ref="P62:P63"/>
     <mergeCell ref="H58:H59"/>
+    <mergeCell ref="F259:H259"/>
+    <mergeCell ref="O79:O80"/>
+    <mergeCell ref="P79:P80"/>
+    <mergeCell ref="O81:O82"/>
+    <mergeCell ref="P81:P82"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="O58:O59"/>
+    <mergeCell ref="P58:P59"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="O94:O95"/>
+    <mergeCell ref="P94:P95"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -36168,18 +36189,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="42.75" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A1" s="514" t="s">
+      <c r="A1" s="538" t="s">
         <v>288</v>
       </c>
-      <c r="B1" s="514"/>
-      <c r="C1" s="514"/>
-      <c r="D1" s="514"/>
-      <c r="E1" s="514"/>
-      <c r="F1" s="514"/>
-      <c r="G1" s="514"/>
-      <c r="H1" s="514"/>
-      <c r="I1" s="514"/>
-      <c r="J1" s="514"/>
+      <c r="B1" s="538"/>
+      <c r="C1" s="538"/>
+      <c r="D1" s="538"/>
+      <c r="E1" s="538"/>
+      <c r="F1" s="538"/>
+      <c r="G1" s="538"/>
+      <c r="H1" s="538"/>
+      <c r="I1" s="538"/>
+      <c r="J1" s="538"/>
       <c r="K1" s="375"/>
       <c r="L1" s="375"/>
       <c r="M1" s="375"/>
@@ -36195,22 +36216,22 @@
       <c r="V1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="W1" s="515" t="s">
+      <c r="W1" s="539" t="s">
         <v>2</v>
       </c>
-      <c r="X1" s="516"/>
+      <c r="X1" s="540"/>
     </row>
     <row r="2" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="514"/>
-      <c r="B2" s="514"/>
-      <c r="C2" s="514"/>
-      <c r="D2" s="514"/>
-      <c r="E2" s="514"/>
-      <c r="F2" s="514"/>
-      <c r="G2" s="514"/>
-      <c r="H2" s="514"/>
-      <c r="I2" s="514"/>
-      <c r="J2" s="514"/>
+      <c r="A2" s="538"/>
+      <c r="B2" s="538"/>
+      <c r="C2" s="538"/>
+      <c r="D2" s="538"/>
+      <c r="E2" s="538"/>
+      <c r="F2" s="538"/>
+      <c r="G2" s="538"/>
+      <c r="H2" s="538"/>
+      <c r="I2" s="538"/>
+      <c r="J2" s="538"/>
       <c r="K2" s="377"/>
       <c r="L2" s="377"/>
       <c r="M2" s="377"/>
@@ -36264,10 +36285,10 @@
       <c r="N3" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="517" t="s">
+      <c r="O3" s="541" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="518"/>
+      <c r="P3" s="542"/>
       <c r="Q3" s="30" t="s">
         <v>16</v>
       </c>
@@ -39655,7 +39676,7 @@
       <c r="B64" s="178" t="s">
         <v>464</v>
       </c>
-      <c r="C64" s="566" t="s">
+      <c r="C64" s="568" t="s">
         <v>465</v>
       </c>
       <c r="D64" s="171"/>
@@ -39699,11 +39720,11 @@
       <c r="V64" s="54"/>
     </row>
     <row r="65" spans="1:22" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="561"/>
+      <c r="A65" s="563"/>
       <c r="B65" s="178" t="s">
         <v>240</v>
       </c>
-      <c r="C65" s="567"/>
+      <c r="C65" s="569"/>
       <c r="D65" s="171"/>
       <c r="E65" s="60"/>
       <c r="F65" s="151">
@@ -40149,8 +40170,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O79" s="539"/>
-      <c r="P79" s="541"/>
+      <c r="O79" s="520"/>
+      <c r="P79" s="534"/>
       <c r="Q79" s="164"/>
       <c r="R79" s="129"/>
       <c r="S79" s="180"/>
@@ -40179,8 +40200,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O80" s="540"/>
-      <c r="P80" s="542"/>
+      <c r="O80" s="521"/>
+      <c r="P80" s="535"/>
       <c r="Q80" s="164"/>
       <c r="R80" s="129"/>
       <c r="S80" s="180"/>
@@ -40209,8 +40230,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O81" s="539"/>
-      <c r="P81" s="541"/>
+      <c r="O81" s="520"/>
+      <c r="P81" s="534"/>
       <c r="Q81" s="164"/>
       <c r="R81" s="158"/>
       <c r="S81" s="180"/>
@@ -40242,8 +40263,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O82" s="540"/>
-      <c r="P82" s="542"/>
+      <c r="O82" s="521"/>
+      <c r="P82" s="535"/>
       <c r="Q82" s="164"/>
       <c r="R82" s="158"/>
       <c r="S82" s="180"/>
@@ -40401,8 +40422,8 @@
         <v>0</v>
       </c>
       <c r="K87" s="100"/>
-      <c r="L87" s="543"/>
-      <c r="M87" s="544"/>
+      <c r="L87" s="536"/>
+      <c r="M87" s="537"/>
       <c r="N87" s="48">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -40434,8 +40455,8 @@
         <v>0</v>
       </c>
       <c r="K88" s="100"/>
-      <c r="L88" s="543"/>
-      <c r="M88" s="544"/>
+      <c r="L88" s="536"/>
+      <c r="M88" s="537"/>
       <c r="N88" s="48">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -40638,8 +40659,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O94" s="539"/>
-      <c r="P94" s="535"/>
+      <c r="O94" s="520"/>
+      <c r="P94" s="530"/>
       <c r="Q94" s="164"/>
       <c r="R94" s="129"/>
       <c r="S94" s="180"/>
@@ -40671,8 +40692,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O95" s="540"/>
-      <c r="P95" s="536"/>
+      <c r="O95" s="521"/>
+      <c r="P95" s="531"/>
       <c r="Q95" s="164"/>
       <c r="R95" s="129"/>
       <c r="S95" s="180"/>
@@ -46064,11 +46085,11 @@
         <f t="shared" si="11"/>
         <v>#VALUE!</v>
       </c>
-      <c r="F259" s="537" t="s">
+      <c r="F259" s="532" t="s">
         <v>26</v>
       </c>
-      <c r="G259" s="537"/>
-      <c r="H259" s="538"/>
+      <c r="G259" s="532"/>
+      <c r="H259" s="533"/>
       <c r="I259" s="317">
         <f>SUM(I4:I258)</f>
         <v>491966.85000000003</v>
@@ -46642,6 +46663,12 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="F259:H259"/>
+    <mergeCell ref="O81:O82"/>
+    <mergeCell ref="P81:P82"/>
+    <mergeCell ref="L87:M88"/>
+    <mergeCell ref="O94:O95"/>
+    <mergeCell ref="P94:P95"/>
     <mergeCell ref="W1:X1"/>
     <mergeCell ref="O3:P3"/>
     <mergeCell ref="O79:O80"/>
@@ -46653,12 +46680,6 @@
     <mergeCell ref="H64:H65"/>
     <mergeCell ref="O64:O65"/>
     <mergeCell ref="P64:P65"/>
-    <mergeCell ref="F259:H259"/>
-    <mergeCell ref="O81:O82"/>
-    <mergeCell ref="P81:P82"/>
-    <mergeCell ref="L87:M88"/>
-    <mergeCell ref="O94:O95"/>
-    <mergeCell ref="P94:P95"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -46672,11 +46693,11 @@
   </sheetPr>
   <dimension ref="A1:X292"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="8" ySplit="3" topLeftCell="V24" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="8" ySplit="3" topLeftCell="I25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="X36" sqref="X36"/>
+      <selection pane="bottomRight" activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -46705,18 +46726,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="42.75" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A1" s="514" t="s">
+      <c r="A1" s="538" t="s">
         <v>402</v>
       </c>
-      <c r="B1" s="514"/>
-      <c r="C1" s="514"/>
-      <c r="D1" s="514"/>
-      <c r="E1" s="514"/>
-      <c r="F1" s="514"/>
-      <c r="G1" s="514"/>
-      <c r="H1" s="514"/>
-      <c r="I1" s="514"/>
-      <c r="J1" s="514"/>
+      <c r="B1" s="538"/>
+      <c r="C1" s="538"/>
+      <c r="D1" s="538"/>
+      <c r="E1" s="538"/>
+      <c r="F1" s="538"/>
+      <c r="G1" s="538"/>
+      <c r="H1" s="538"/>
+      <c r="I1" s="538"/>
+      <c r="J1" s="538"/>
       <c r="K1" s="375"/>
       <c r="L1" s="375"/>
       <c r="M1" s="375"/>
@@ -46732,22 +46753,22 @@
       <c r="V1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="W1" s="515" t="s">
+      <c r="W1" s="539" t="s">
         <v>2</v>
       </c>
-      <c r="X1" s="516"/>
+      <c r="X1" s="540"/>
     </row>
     <row r="2" spans="1:24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="514"/>
-      <c r="B2" s="514"/>
-      <c r="C2" s="514"/>
-      <c r="D2" s="514"/>
-      <c r="E2" s="514"/>
-      <c r="F2" s="514"/>
-      <c r="G2" s="514"/>
-      <c r="H2" s="514"/>
-      <c r="I2" s="514"/>
-      <c r="J2" s="514"/>
+      <c r="A2" s="538"/>
+      <c r="B2" s="538"/>
+      <c r="C2" s="538"/>
+      <c r="D2" s="538"/>
+      <c r="E2" s="538"/>
+      <c r="F2" s="538"/>
+      <c r="G2" s="538"/>
+      <c r="H2" s="538"/>
+      <c r="I2" s="538"/>
+      <c r="J2" s="538"/>
       <c r="K2" s="377"/>
       <c r="L2" s="377"/>
       <c r="M2" s="377"/>
@@ -46801,10 +46822,10 @@
       <c r="N3" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="517" t="s">
+      <c r="O3" s="541" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="518"/>
+      <c r="P3" s="542"/>
       <c r="Q3" s="30" t="s">
         <v>16</v>
       </c>
@@ -46889,7 +46910,7 @@
       <c r="U4" s="53"/>
       <c r="V4" s="54"/>
       <c r="W4" s="55" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="X4" s="56">
         <v>4176</v>
@@ -46958,7 +46979,7 @@
       <c r="U5" s="53"/>
       <c r="V5" s="54"/>
       <c r="W5" s="68" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="X5" s="69">
         <v>4176</v>
@@ -47027,7 +47048,7 @@
       <c r="U6" s="53"/>
       <c r="V6" s="54"/>
       <c r="W6" s="53" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="X6" s="70">
         <v>4176</v>
@@ -47096,7 +47117,7 @@
       <c r="U7" s="53"/>
       <c r="V7" s="54"/>
       <c r="W7" s="53" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="X7" s="70">
         <v>0</v>
@@ -47165,7 +47186,7 @@
       <c r="U8" s="53"/>
       <c r="V8" s="54"/>
       <c r="W8" s="53" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="X8" s="70">
         <v>4176</v>
@@ -47234,7 +47255,7 @@
       <c r="U9" s="53"/>
       <c r="V9" s="54"/>
       <c r="W9" s="53" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="X9" s="70">
         <v>4176</v>
@@ -47303,7 +47324,7 @@
       <c r="U10" s="53"/>
       <c r="V10" s="54"/>
       <c r="W10" s="53" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="X10" s="70">
         <v>0</v>
@@ -47372,7 +47393,7 @@
       <c r="U11" s="53"/>
       <c r="V11" s="54"/>
       <c r="W11" s="53" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="X11" s="70">
         <v>4176</v>
@@ -47441,7 +47462,7 @@
       <c r="U12" s="53"/>
       <c r="V12" s="54"/>
       <c r="W12" s="53" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="X12" s="70">
         <v>0</v>
@@ -47510,7 +47531,7 @@
       <c r="U13" s="53"/>
       <c r="V13" s="54"/>
       <c r="W13" s="53" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="X13" s="70">
         <v>4176</v>
@@ -47579,7 +47600,7 @@
       <c r="U14" s="53"/>
       <c r="V14" s="54"/>
       <c r="W14" s="53" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="X14" s="70">
         <v>0</v>
@@ -47648,7 +47669,7 @@
       <c r="U15" s="53"/>
       <c r="V15" s="54"/>
       <c r="W15" s="53" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="X15" s="70">
         <v>4176</v>
@@ -47717,7 +47738,7 @@
       <c r="U16" s="53"/>
       <c r="V16" s="54"/>
       <c r="W16" s="53" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="X16" s="70">
         <v>0</v>
@@ -47786,7 +47807,7 @@
       <c r="U17" s="53"/>
       <c r="V17" s="54"/>
       <c r="W17" s="53" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="X17" s="70">
         <v>4176</v>
@@ -47855,7 +47876,7 @@
       <c r="U18" s="53"/>
       <c r="V18" s="54"/>
       <c r="W18" s="53" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="X18" s="70">
         <v>0</v>
@@ -47925,7 +47946,7 @@
       <c r="U19" s="53"/>
       <c r="V19" s="54"/>
       <c r="W19" s="53" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="X19" s="70">
         <v>4176</v>
@@ -47994,7 +48015,7 @@
       <c r="U20" s="53"/>
       <c r="V20" s="54"/>
       <c r="W20" s="53" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="X20" s="70">
         <v>0</v>
@@ -48063,7 +48084,7 @@
       <c r="U21" s="53"/>
       <c r="V21" s="54"/>
       <c r="W21" s="53" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="X21" s="70">
         <v>4176</v>
@@ -48132,7 +48153,7 @@
       <c r="U22" s="53"/>
       <c r="V22" s="54"/>
       <c r="W22" s="53" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="X22" s="70">
         <v>0</v>
@@ -48201,7 +48222,7 @@
       <c r="U23" s="53"/>
       <c r="V23" s="54"/>
       <c r="W23" s="53" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="X23" s="70">
         <v>4176</v>
@@ -48270,7 +48291,7 @@
       <c r="U24" s="53"/>
       <c r="V24" s="54"/>
       <c r="W24" s="53" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="X24" s="70">
         <v>0</v>
@@ -48340,7 +48361,7 @@
       <c r="U25" s="53"/>
       <c r="V25" s="54"/>
       <c r="W25" s="53" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="X25" s="70">
         <v>4176</v>
@@ -48409,7 +48430,7 @@
       <c r="U26" s="53"/>
       <c r="V26" s="54"/>
       <c r="W26" s="53" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="X26" s="70">
         <v>0</v>
@@ -48439,7 +48460,7 @@
         <v>44705</v>
       </c>
       <c r="H27" s="446" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="I27" s="411">
         <f>21470-429.4</f>
@@ -48459,7 +48480,7 @@
         <v>778502.2</v>
       </c>
       <c r="O27" s="417" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="P27" s="418">
         <v>44719</v>
@@ -48479,7 +48500,7 @@
       <c r="U27" s="53"/>
       <c r="V27" s="54"/>
       <c r="W27" s="53" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="X27" s="70">
         <v>4176</v>
@@ -48548,7 +48569,7 @@
       <c r="U28" s="53"/>
       <c r="V28" s="54"/>
       <c r="W28" s="53" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="X28" s="70">
         <v>0</v>
@@ -48578,7 +48599,7 @@
         <v>44707</v>
       </c>
       <c r="H29" s="446" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="I29" s="411">
         <v>22070</v>
@@ -48617,7 +48638,7 @@
       <c r="U29" s="53"/>
       <c r="V29" s="54"/>
       <c r="W29" s="53" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="X29" s="70">
         <v>4176</v>
@@ -48686,7 +48707,7 @@
       <c r="U30" s="53"/>
       <c r="V30" s="54"/>
       <c r="W30" s="53" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="X30" s="70">
         <v>0</v>
@@ -48755,7 +48776,7 @@
       <c r="U31" s="53"/>
       <c r="V31" s="54"/>
       <c r="W31" s="53" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="X31" s="70">
         <v>4176</v>
@@ -48785,7 +48806,7 @@
         <v>44708</v>
       </c>
       <c r="H32" s="446" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="I32" s="411">
         <v>5930</v>
@@ -48824,13 +48845,13 @@
       <c r="U32" s="53"/>
       <c r="V32" s="54"/>
       <c r="W32" s="53" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="X32" s="70">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:24" ht="20.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:24" ht="48.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="83" t="s">
         <v>460</v>
       </c>
@@ -48850,14 +48871,15 @@
         <v>44710</v>
       </c>
       <c r="H33" s="446" t="s">
-        <v>503</v>
+        <v>526</v>
       </c>
       <c r="I33" s="411">
-        <v>21360</v>
+        <f>21360-322.02</f>
+        <v>21037.98</v>
       </c>
       <c r="J33" s="45">
         <f t="shared" si="0"/>
-        <v>359</v>
+        <v>36.979999999999563</v>
       </c>
       <c r="K33" s="76">
         <v>38.5</v>
@@ -48866,10 +48888,14 @@
       <c r="M33" s="99"/>
       <c r="N33" s="48">
         <f t="shared" si="1"/>
-        <v>822360</v>
-      </c>
-      <c r="O33" s="417"/>
-      <c r="P33" s="418"/>
+        <v>809962.23</v>
+      </c>
+      <c r="O33" s="417" t="s">
+        <v>61</v>
+      </c>
+      <c r="P33" s="418">
+        <v>44725</v>
+      </c>
       <c r="Q33" s="419">
         <v>26793</v>
       </c>
@@ -48885,13 +48911,13 @@
       <c r="U33" s="53"/>
       <c r="V33" s="54"/>
       <c r="W33" s="53" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="X33" s="70">
         <v>4176</v>
       </c>
     </row>
-    <row r="34" spans="1:24" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:24" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="82" t="s">
         <v>50</v>
       </c>
@@ -48911,7 +48937,7 @@
         <v>44710</v>
       </c>
       <c r="H34" s="446" t="s">
-        <v>503</v>
+        <v>528</v>
       </c>
       <c r="I34" s="411">
         <v>5355</v>
@@ -48921,16 +48947,20 @@
         <v>5355</v>
       </c>
       <c r="K34" s="76">
-        <v>50</v>
+        <v>38.5</v>
       </c>
       <c r="L34" s="99"/>
       <c r="M34" s="99"/>
       <c r="N34" s="48">
         <f t="shared" si="1"/>
-        <v>267750</v>
-      </c>
-      <c r="O34" s="417"/>
-      <c r="P34" s="418"/>
+        <v>206167.5</v>
+      </c>
+      <c r="O34" s="417" t="s">
+        <v>61</v>
+      </c>
+      <c r="P34" s="418">
+        <v>44725</v>
+      </c>
       <c r="Q34" s="419">
         <v>0</v>
       </c>
@@ -48946,7 +48976,7 @@
       <c r="U34" s="53"/>
       <c r="V34" s="54"/>
       <c r="W34" s="53" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="X34" s="70">
         <v>0</v>
@@ -48971,7 +49001,9 @@
       <c r="G35" s="62">
         <v>44712</v>
       </c>
-      <c r="H35" s="446"/>
+      <c r="H35" s="446" t="s">
+        <v>527</v>
+      </c>
       <c r="I35" s="411">
         <v>23032</v>
       </c>
@@ -48988,8 +49020,12 @@
         <f t="shared" si="1"/>
         <v>1213786.4000000001</v>
       </c>
-      <c r="O35" s="417"/>
-      <c r="P35" s="418"/>
+      <c r="O35" s="417" t="s">
+        <v>61</v>
+      </c>
+      <c r="P35" s="418">
+        <v>44726</v>
+      </c>
       <c r="Q35" s="419"/>
       <c r="R35" s="420"/>
       <c r="S35" s="91">
@@ -50689,8 +50725,8 @@
         <v>0</v>
       </c>
       <c r="K87" s="100"/>
-      <c r="L87" s="543"/>
-      <c r="M87" s="544"/>
+      <c r="L87" s="536"/>
+      <c r="M87" s="537"/>
       <c r="N87" s="48">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -50722,8 +50758,8 @@
         <v>0</v>
       </c>
       <c r="K88" s="100"/>
-      <c r="L88" s="543"/>
-      <c r="M88" s="544"/>
+      <c r="L88" s="536"/>
+      <c r="M88" s="537"/>
       <c r="N88" s="48">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -50926,8 +50962,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O94" s="539"/>
-      <c r="P94" s="535"/>
+      <c r="O94" s="520"/>
+      <c r="P94" s="530"/>
       <c r="Q94" s="164"/>
       <c r="R94" s="129"/>
       <c r="S94" s="180"/>
@@ -50959,8 +50995,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O95" s="540"/>
-      <c r="P95" s="536"/>
+      <c r="O95" s="521"/>
+      <c r="P95" s="531"/>
       <c r="Q95" s="164"/>
       <c r="R95" s="129"/>
       <c r="S95" s="180"/>
@@ -56352,14 +56388,14 @@
         <f t="shared" si="12"/>
         <v>#VALUE!</v>
       </c>
-      <c r="F259" s="537" t="s">
+      <c r="F259" s="532" t="s">
         <v>26</v>
       </c>
-      <c r="G259" s="537"/>
-      <c r="H259" s="538"/>
+      <c r="G259" s="532"/>
+      <c r="H259" s="533"/>
       <c r="I259" s="317">
         <f>SUM(I4:I258)</f>
-        <v>476389.92</v>
+        <v>476067.89999999997</v>
       </c>
       <c r="J259" s="318"/>
       <c r="K259" s="314"/>
@@ -56458,7 +56494,7 @@
       <c r="M263" s="336"/>
       <c r="N263" s="337">
         <f>SUM(N4:N262)</f>
-        <v>17769781.285</v>
+        <v>17695801.015000001</v>
       </c>
       <c r="O263" s="338"/>
       <c r="Q263" s="339">
@@ -56518,7 +56554,7 @@
       <c r="M266" s="352"/>
       <c r="N266" s="353">
         <f>V263+S263+Q263+N263+L263</f>
-        <v>18422968.285</v>
+        <v>18348988.015000001</v>
       </c>
       <c r="O266" s="354"/>
       <c r="R266" s="324"/>
@@ -56951,11 +56987,11 @@
   </sheetPr>
   <dimension ref="A1:X292"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="10" ySplit="3" topLeftCell="K43" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="10" ySplit="3" topLeftCell="K16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomRight" activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -56984,18 +57020,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="42.75" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A1" s="514" t="s">
+      <c r="A1" s="538" t="s">
         <v>482</v>
       </c>
-      <c r="B1" s="514"/>
-      <c r="C1" s="514"/>
-      <c r="D1" s="514"/>
-      <c r="E1" s="514"/>
-      <c r="F1" s="514"/>
-      <c r="G1" s="514"/>
-      <c r="H1" s="514"/>
-      <c r="I1" s="514"/>
-      <c r="J1" s="514"/>
+      <c r="B1" s="538"/>
+      <c r="C1" s="538"/>
+      <c r="D1" s="538"/>
+      <c r="E1" s="538"/>
+      <c r="F1" s="538"/>
+      <c r="G1" s="538"/>
+      <c r="H1" s="538"/>
+      <c r="I1" s="538"/>
+      <c r="J1" s="538"/>
       <c r="K1" s="375"/>
       <c r="L1" s="375"/>
       <c r="M1" s="375"/>
@@ -57011,22 +57047,22 @@
       <c r="V1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="W1" s="515" t="s">
+      <c r="W1" s="539" t="s">
         <v>2</v>
       </c>
-      <c r="X1" s="516"/>
+      <c r="X1" s="540"/>
     </row>
     <row r="2" spans="1:24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="514"/>
-      <c r="B2" s="514"/>
-      <c r="C2" s="514"/>
-      <c r="D2" s="514"/>
-      <c r="E2" s="514"/>
-      <c r="F2" s="514"/>
-      <c r="G2" s="514"/>
-      <c r="H2" s="514"/>
-      <c r="I2" s="514"/>
-      <c r="J2" s="514"/>
+      <c r="A2" s="538"/>
+      <c r="B2" s="538"/>
+      <c r="C2" s="538"/>
+      <c r="D2" s="538"/>
+      <c r="E2" s="538"/>
+      <c r="F2" s="538"/>
+      <c r="G2" s="538"/>
+      <c r="H2" s="538"/>
+      <c r="I2" s="538"/>
+      <c r="J2" s="538"/>
       <c r="K2" s="377"/>
       <c r="L2" s="377"/>
       <c r="M2" s="377"/>
@@ -57080,10 +57116,10 @@
       <c r="N3" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="517" t="s">
+      <c r="O3" s="541" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="518"/>
+      <c r="P3" s="542"/>
       <c r="Q3" s="30" t="s">
         <v>16</v>
       </c>
@@ -57125,7 +57161,7 @@
         <v>44714</v>
       </c>
       <c r="H4" s="512" t="s">
-        <v>504</v>
+        <v>525</v>
       </c>
       <c r="I4" s="409">
         <v>20470</v>
@@ -57143,8 +57179,12 @@
         <f t="shared" ref="N4:N114" si="1">K4*I4</f>
         <v>798330</v>
       </c>
-      <c r="O4" s="509"/>
-      <c r="P4" s="394"/>
+      <c r="O4" s="509" t="s">
+        <v>61</v>
+      </c>
+      <c r="P4" s="394">
+        <v>44728</v>
+      </c>
       <c r="Q4" s="49">
         <v>26893</v>
       </c>
@@ -57178,7 +57218,7 @@
         <v>44714</v>
       </c>
       <c r="H5" s="410" t="s">
-        <v>504</v>
+        <v>524</v>
       </c>
       <c r="I5" s="411">
         <v>5460</v>
@@ -57196,8 +57236,12 @@
         <f t="shared" si="1"/>
         <v>212940</v>
       </c>
-      <c r="O5" s="395"/>
-      <c r="P5" s="396"/>
+      <c r="O5" s="395" t="s">
+        <v>61</v>
+      </c>
+      <c r="P5" s="396">
+        <v>44728</v>
+      </c>
       <c r="Q5" s="66">
         <v>0</v>
       </c>
@@ -57231,7 +57275,7 @@
         <v>44715</v>
       </c>
       <c r="H6" s="410" t="s">
-        <v>505</v>
+        <v>523</v>
       </c>
       <c r="I6" s="411">
         <v>23890</v>
@@ -57249,8 +57293,12 @@
         <f t="shared" si="1"/>
         <v>931710</v>
       </c>
-      <c r="O6" s="395"/>
-      <c r="P6" s="396"/>
+      <c r="O6" s="395" t="s">
+        <v>61</v>
+      </c>
+      <c r="P6" s="396">
+        <v>44729</v>
+      </c>
       <c r="Q6" s="66">
         <v>26793</v>
       </c>
@@ -57288,7 +57336,7 @@
         <v>44715</v>
       </c>
       <c r="H7" s="410" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="I7" s="411">
         <v>5600</v>
@@ -57349,7 +57397,7 @@
         <v>44718</v>
       </c>
       <c r="H8" s="410" t="s">
-        <v>509</v>
+        <v>518</v>
       </c>
       <c r="I8" s="411">
         <v>22540</v>
@@ -57367,8 +57415,12 @@
         <f t="shared" si="1"/>
         <v>901600</v>
       </c>
-      <c r="O8" s="89"/>
-      <c r="P8" s="90"/>
+      <c r="O8" s="89" t="s">
+        <v>61</v>
+      </c>
+      <c r="P8" s="90">
+        <v>44732</v>
+      </c>
       <c r="Q8" s="66">
         <v>27221</v>
       </c>
@@ -57406,7 +57458,7 @@
         <v>44718</v>
       </c>
       <c r="H9" s="410" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="I9" s="411">
         <v>5465</v>
@@ -57467,7 +57519,7 @@
         <v>44720</v>
       </c>
       <c r="H10" s="410" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="I10" s="411">
         <v>22580</v>
@@ -57524,7 +57576,7 @@
         <v>44720</v>
       </c>
       <c r="H11" s="410" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="I11" s="411">
         <v>5390</v>
@@ -57581,7 +57633,7 @@
         <v>44722</v>
       </c>
       <c r="H12" s="410" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="I12" s="411">
         <v>21240</v>
@@ -57611,7 +57663,7 @@
         <v>28000</v>
       </c>
       <c r="T12" s="52" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="U12" s="53"/>
       <c r="V12" s="54"/>
@@ -57638,7 +57690,7 @@
         <v>44722</v>
       </c>
       <c r="H13" s="410" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="I13" s="411">
         <v>5635</v>
@@ -57668,7 +57720,7 @@
         <v>0</v>
       </c>
       <c r="T13" s="52" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="U13" s="53"/>
       <c r="V13" s="54"/>
@@ -57694,7 +57746,9 @@
       <c r="G14" s="62">
         <v>44724</v>
       </c>
-      <c r="H14" s="410"/>
+      <c r="H14" s="410" t="s">
+        <v>519</v>
+      </c>
       <c r="I14" s="411">
         <v>23940</v>
       </c>
@@ -57713,13 +57767,17 @@
       </c>
       <c r="O14" s="397"/>
       <c r="P14" s="398"/>
-      <c r="Q14" s="66"/>
-      <c r="R14" s="67"/>
+      <c r="Q14" s="66">
+        <v>20587</v>
+      </c>
+      <c r="R14" s="67">
+        <v>44729</v>
+      </c>
       <c r="S14" s="51">
         <v>28000</v>
       </c>
       <c r="T14" s="52" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="U14" s="53"/>
       <c r="V14" s="54"/>
@@ -57728,7 +57786,7 @@
     </row>
     <row r="15" spans="1:24" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="73" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="B15" s="58" t="s">
         <v>72</v>
@@ -57745,7 +57803,9 @@
       <c r="G15" s="62">
         <v>44726</v>
       </c>
-      <c r="H15" s="410"/>
+      <c r="H15" s="410" t="s">
+        <v>520</v>
+      </c>
       <c r="I15" s="411">
         <v>24190</v>
       </c>
@@ -57764,13 +57824,17 @@
       </c>
       <c r="O15" s="397"/>
       <c r="P15" s="398"/>
-      <c r="Q15" s="66"/>
-      <c r="R15" s="67"/>
+      <c r="Q15" s="66">
+        <v>21550</v>
+      </c>
+      <c r="R15" s="67">
+        <v>44729</v>
+      </c>
       <c r="S15" s="51">
         <v>28000</v>
       </c>
       <c r="T15" s="92" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="U15" s="53"/>
       <c r="V15" s="54"/>
@@ -57796,7 +57860,9 @@
       <c r="G16" s="62">
         <v>44728</v>
       </c>
-      <c r="H16" s="410"/>
+      <c r="H16" s="410" t="s">
+        <v>521</v>
+      </c>
       <c r="I16" s="411">
         <v>24660</v>
       </c>
@@ -57815,13 +57881,17 @@
       </c>
       <c r="O16" s="397"/>
       <c r="P16" s="398"/>
-      <c r="Q16" s="66"/>
-      <c r="R16" s="67"/>
+      <c r="Q16" s="66">
+        <v>21550</v>
+      </c>
+      <c r="R16" s="67">
+        <v>44729</v>
+      </c>
       <c r="S16" s="51">
         <v>28000</v>
       </c>
       <c r="T16" s="92" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="U16" s="53"/>
       <c r="V16" s="54"/>
@@ -57847,7 +57917,9 @@
       <c r="G17" s="62">
         <v>44729</v>
       </c>
-      <c r="H17" s="410"/>
+      <c r="H17" s="410" t="s">
+        <v>522</v>
+      </c>
       <c r="I17" s="411">
         <v>25270</v>
       </c>
@@ -57866,13 +57938,17 @@
       </c>
       <c r="O17" s="397"/>
       <c r="P17" s="398"/>
-      <c r="Q17" s="66"/>
-      <c r="R17" s="67"/>
+      <c r="Q17" s="66">
+        <v>21550</v>
+      </c>
+      <c r="R17" s="67">
+        <v>44729</v>
+      </c>
       <c r="S17" s="51">
         <v>28000</v>
       </c>
       <c r="T17" s="92" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="U17" s="53"/>
       <c r="V17" s="54"/>
@@ -57914,7 +57990,7 @@
       <c r="W18" s="53"/>
       <c r="X18" s="70"/>
     </row>
-    <row r="19" spans="1:24" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="78"/>
       <c r="B19" s="58"/>
       <c r="C19" s="59"/>
@@ -60170,8 +60246,8 @@
         <v>0</v>
       </c>
       <c r="K87" s="100"/>
-      <c r="L87" s="543"/>
-      <c r="M87" s="544"/>
+      <c r="L87" s="536"/>
+      <c r="M87" s="537"/>
       <c r="N87" s="48">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -60203,8 +60279,8 @@
         <v>0</v>
       </c>
       <c r="K88" s="100"/>
-      <c r="L88" s="543"/>
-      <c r="M88" s="544"/>
+      <c r="L88" s="536"/>
+      <c r="M88" s="537"/>
       <c r="N88" s="48">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -60407,8 +60483,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O94" s="539"/>
-      <c r="P94" s="535"/>
+      <c r="O94" s="520"/>
+      <c r="P94" s="530"/>
       <c r="Q94" s="164"/>
       <c r="R94" s="129"/>
       <c r="S94" s="180"/>
@@ -60440,8 +60516,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O95" s="540"/>
-      <c r="P95" s="536"/>
+      <c r="O95" s="521"/>
+      <c r="P95" s="531"/>
       <c r="Q95" s="164"/>
       <c r="R95" s="129"/>
       <c r="S95" s="180"/>
@@ -65833,11 +65909,11 @@
         <f t="shared" si="11"/>
         <v>#VALUE!</v>
       </c>
-      <c r="F259" s="537" t="s">
+      <c r="F259" s="532" t="s">
         <v>26</v>
       </c>
-      <c r="G259" s="537"/>
-      <c r="H259" s="538"/>
+      <c r="G259" s="532"/>
+      <c r="H259" s="533"/>
       <c r="I259" s="317">
         <f>SUM(I4:I258)</f>
         <v>236330</v>
@@ -65944,7 +66020,7 @@
       <c r="O263" s="338"/>
       <c r="Q263" s="339">
         <f>SUM(Q4:Q262)</f>
-        <v>134921</v>
+        <v>220158</v>
       </c>
       <c r="R263" s="8"/>
       <c r="S263" s="340">
@@ -65999,7 +66075,7 @@
       <c r="M266" s="352"/>
       <c r="N266" s="353">
         <f>V263+S263+Q263+N263+L263</f>
-        <v>9751053.5</v>
+        <v>9836290.5</v>
       </c>
       <c r="O266" s="354"/>
       <c r="R266" s="324"/>

</xml_diff>

<commit_message>
CIERRE 5 JULIO 2022
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #06  JUNIO 2022/ENTRADAS OBRADOR     J U N I O         2022.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #06  JUNIO 2022/ENTRADAS OBRADOR     J U N I O         2022.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ROUSS\Documents\GitHub\TRABAJO\01 DOCUEMENTOS\CENTRAL  ARCHIVO   2 0 2 2\CENTRAL #06  JUNIO 2022\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rouss\Documents\GitHub\TRABAJO\01 DOCUEMENTOS\CENTRAL  ARCHIVO   2 0 2 2\CENTRAL #06  JUNIO 2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAD04606-F30D-4EF0-AFB7-99F97A0D2C33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16365" windowHeight="10305" firstSheet="3" activeTab="5"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CANALES  ENERO  2022   " sheetId="1" r:id="rId1"/>
@@ -20,17 +21,25 @@
     <sheet name="   CANALES   DE  JUNIO   2022  " sheetId="6" r:id="rId6"/>
     <sheet name="Hoja1" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1674" uniqueCount="561">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1683" uniqueCount="566">
   <si>
     <t>FECHA DE PAGO</t>
   </si>
@@ -1727,11 +1736,26 @@
   <si>
     <t>D-4414</t>
   </si>
+  <si>
+    <t>0076 A1</t>
+  </si>
+  <si>
+    <t>0104 A1</t>
+  </si>
+  <si>
+    <t>0120 A1</t>
+  </si>
+  <si>
+    <t>0131 A1</t>
+  </si>
+  <si>
+    <t>0157 A1</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="[$-C0A]d\-mmm\-yy;@"/>
@@ -4540,6 +4564,98 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="68" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="54" fillId="0" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="54" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="31" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="31" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="11" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="11" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="26" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="26" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4573,83 +4689,11 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="11" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="11" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="22" fillId="11" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="22" fillId="11" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="26" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="26" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="31" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="31" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -4679,6 +4723,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="32" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="32" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4714,12 +4764,6 @@
     <xf numFmtId="1" fontId="18" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="32" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="32" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="11" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4738,38 +4782,18 @@
     <xf numFmtId="164" fontId="12" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="68" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="68" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="54" fillId="0" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="54" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="54" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -5060,7 +5084,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Hoja1">
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -5099,18 +5123,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="42.75" thickBot="1" x14ac:dyDescent="0.7">
-      <c r="A1" s="514" t="s">
+      <c r="A1" s="546" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="514"/>
-      <c r="C1" s="514"/>
-      <c r="D1" s="514"/>
-      <c r="E1" s="514"/>
-      <c r="F1" s="514"/>
-      <c r="G1" s="514"/>
-      <c r="H1" s="514"/>
-      <c r="I1" s="514"/>
-      <c r="J1" s="514"/>
+      <c r="B1" s="546"/>
+      <c r="C1" s="546"/>
+      <c r="D1" s="546"/>
+      <c r="E1" s="546"/>
+      <c r="F1" s="546"/>
+      <c r="G1" s="546"/>
+      <c r="H1" s="546"/>
+      <c r="I1" s="546"/>
+      <c r="J1" s="546"/>
       <c r="K1" s="375"/>
       <c r="L1" s="375"/>
       <c r="M1" s="375"/>
@@ -5124,22 +5148,22 @@
       <c r="V1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="W1" s="515" t="s">
+      <c r="W1" s="547" t="s">
         <v>2</v>
       </c>
-      <c r="X1" s="516"/>
+      <c r="X1" s="548"/>
     </row>
     <row r="2" spans="1:24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="514"/>
-      <c r="B2" s="514"/>
-      <c r="C2" s="514"/>
-      <c r="D2" s="514"/>
-      <c r="E2" s="514"/>
-      <c r="F2" s="514"/>
-      <c r="G2" s="514"/>
-      <c r="H2" s="514"/>
-      <c r="I2" s="514"/>
-      <c r="J2" s="514"/>
+      <c r="A2" s="546"/>
+      <c r="B2" s="546"/>
+      <c r="C2" s="546"/>
+      <c r="D2" s="546"/>
+      <c r="E2" s="546"/>
+      <c r="F2" s="546"/>
+      <c r="G2" s="546"/>
+      <c r="H2" s="546"/>
+      <c r="I2" s="546"/>
+      <c r="J2" s="546"/>
       <c r="K2" s="377"/>
       <c r="L2" s="377"/>
       <c r="M2" s="377"/>
@@ -5193,10 +5217,10 @@
       <c r="N3" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="517" t="s">
+      <c r="O3" s="549" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="518"/>
+      <c r="P3" s="550"/>
       <c r="Q3" s="30" t="s">
         <v>16</v>
       </c>
@@ -5740,7 +5764,7 @@
       <c r="B12" s="58" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="519" t="s">
+      <c r="C12" s="551" t="s">
         <v>103</v>
       </c>
       <c r="D12" s="400"/>
@@ -5804,7 +5828,7 @@
       <c r="B13" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="520"/>
+      <c r="C13" s="552"/>
       <c r="D13" s="400"/>
       <c r="E13" s="401"/>
       <c r="F13" s="402">
@@ -7806,13 +7830,13 @@
       <c r="V55" s="160"/>
     </row>
     <row r="56" spans="1:24" s="161" customFormat="1" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="531" t="s">
+      <c r="A56" s="530" t="s">
         <v>41</v>
       </c>
       <c r="B56" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="C56" s="533" t="s">
+      <c r="C56" s="532" t="s">
         <v>110</v>
       </c>
       <c r="D56" s="150"/>
@@ -7823,7 +7847,7 @@
       <c r="G56" s="152">
         <v>44571</v>
       </c>
-      <c r="H56" s="525">
+      <c r="H56" s="534">
         <v>782</v>
       </c>
       <c r="I56" s="151">
@@ -7852,11 +7876,11 @@
       <c r="V56" s="160"/>
     </row>
     <row r="57" spans="1:24" s="161" customFormat="1" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="532"/>
+      <c r="A57" s="531"/>
       <c r="B57" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="C57" s="534"/>
+      <c r="C57" s="533"/>
       <c r="D57" s="150"/>
       <c r="E57" s="40"/>
       <c r="F57" s="151">
@@ -7865,7 +7889,7 @@
       <c r="G57" s="152">
         <v>44571</v>
       </c>
-      <c r="H57" s="526"/>
+      <c r="H57" s="535"/>
       <c r="I57" s="151">
         <v>319</v>
       </c>
@@ -7892,13 +7916,13 @@
       <c r="V57" s="160"/>
     </row>
     <row r="58" spans="1:24" s="161" customFormat="1" ht="29.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="531" t="s">
+      <c r="A58" s="530" t="s">
         <v>41</v>
       </c>
       <c r="B58" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="C58" s="533" t="s">
+      <c r="C58" s="532" t="s">
         <v>129</v>
       </c>
       <c r="D58" s="150"/>
@@ -7909,7 +7933,7 @@
       <c r="G58" s="152">
         <v>44578</v>
       </c>
-      <c r="H58" s="525">
+      <c r="H58" s="534">
         <v>810</v>
       </c>
       <c r="I58" s="151">
@@ -7928,10 +7952,10 @@
         <f t="shared" si="1"/>
         <v>75875.8</v>
       </c>
-      <c r="O58" s="527" t="s">
+      <c r="O58" s="536" t="s">
         <v>59</v>
       </c>
-      <c r="P58" s="529">
+      <c r="P58" s="557">
         <v>44606</v>
       </c>
       <c r="Q58" s="128"/>
@@ -7942,11 +7966,11 @@
       <c r="V58" s="160"/>
     </row>
     <row r="59" spans="1:24" s="161" customFormat="1" ht="29.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="532"/>
+      <c r="A59" s="531"/>
       <c r="B59" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="C59" s="534"/>
+      <c r="C59" s="533"/>
       <c r="D59" s="150"/>
       <c r="E59" s="40"/>
       <c r="F59" s="151">
@@ -7955,7 +7979,7 @@
       <c r="G59" s="152">
         <v>44578</v>
       </c>
-      <c r="H59" s="526"/>
+      <c r="H59" s="535"/>
       <c r="I59" s="151">
         <v>220</v>
       </c>
@@ -7972,8 +7996,8 @@
         <f t="shared" si="1"/>
         <v>22440</v>
       </c>
-      <c r="O59" s="528"/>
-      <c r="P59" s="530"/>
+      <c r="O59" s="537"/>
+      <c r="P59" s="558"/>
       <c r="Q59" s="128"/>
       <c r="R59" s="158"/>
       <c r="S59" s="92"/>
@@ -7982,13 +8006,13 @@
       <c r="V59" s="160"/>
     </row>
     <row r="60" spans="1:24" s="161" customFormat="1" ht="48.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="523" t="s">
+      <c r="A60" s="555" t="s">
         <v>41</v>
       </c>
       <c r="B60" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="C60" s="521" t="s">
+      <c r="C60" s="553" t="s">
         <v>109</v>
       </c>
       <c r="D60" s="163"/>
@@ -8002,7 +8026,7 @@
       <c r="G60" s="152">
         <v>44585</v>
       </c>
-      <c r="H60" s="525">
+      <c r="H60" s="534">
         <v>800</v>
       </c>
       <c r="I60" s="151">
@@ -8021,10 +8045,10 @@
         <f t="shared" si="1"/>
         <v>151187.4</v>
       </c>
-      <c r="O60" s="527" t="s">
+      <c r="O60" s="536" t="s">
         <v>59</v>
       </c>
-      <c r="P60" s="529">
+      <c r="P60" s="557">
         <v>44594</v>
       </c>
       <c r="Q60" s="164"/>
@@ -8037,11 +8061,11 @@
       <c r="X60"/>
     </row>
     <row r="61" spans="1:24" ht="26.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="524"/>
+      <c r="A61" s="556"/>
       <c r="B61" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="C61" s="522"/>
+      <c r="C61" s="554"/>
       <c r="D61" s="165"/>
       <c r="E61" s="40">
         <f t="shared" si="2"/>
@@ -8053,7 +8077,7 @@
       <c r="G61" s="152">
         <v>44585</v>
       </c>
-      <c r="H61" s="526"/>
+      <c r="H61" s="535"/>
       <c r="I61" s="151">
         <v>231.6</v>
       </c>
@@ -8070,8 +8094,8 @@
         <f t="shared" si="1"/>
         <v>23623.200000000001</v>
       </c>
-      <c r="O61" s="528"/>
-      <c r="P61" s="530"/>
+      <c r="O61" s="537"/>
+      <c r="P61" s="558"/>
       <c r="Q61" s="164"/>
       <c r="R61" s="129"/>
       <c r="S61" s="92"/>
@@ -8137,7 +8161,7 @@
       <c r="B63" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="C63" s="547"/>
+      <c r="C63" s="524"/>
       <c r="D63" s="163"/>
       <c r="E63" s="40">
         <f t="shared" si="2"/>
@@ -8145,7 +8169,7 @@
       </c>
       <c r="F63" s="151"/>
       <c r="G63" s="152"/>
-      <c r="H63" s="549"/>
+      <c r="H63" s="526"/>
       <c r="I63" s="151"/>
       <c r="J63" s="45">
         <f t="shared" si="0"/>
@@ -8174,7 +8198,7 @@
       <c r="B64" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="C64" s="548"/>
+      <c r="C64" s="525"/>
       <c r="D64" s="168"/>
       <c r="E64" s="40">
         <f t="shared" si="2"/>
@@ -8182,7 +8206,7 @@
       </c>
       <c r="F64" s="151"/>
       <c r="G64" s="152"/>
-      <c r="H64" s="550"/>
+      <c r="H64" s="527"/>
       <c r="I64" s="151"/>
       <c r="J64" s="45">
         <f t="shared" si="0"/>
@@ -8360,8 +8384,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O68" s="539"/>
-      <c r="P68" s="545"/>
+      <c r="O68" s="528"/>
+      <c r="P68" s="522"/>
       <c r="Q68" s="164"/>
       <c r="R68" s="129"/>
       <c r="S68" s="180"/>
@@ -8395,8 +8419,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O69" s="540"/>
-      <c r="P69" s="546"/>
+      <c r="O69" s="529"/>
+      <c r="P69" s="523"/>
       <c r="Q69" s="164"/>
       <c r="R69" s="129"/>
       <c r="S69" s="180"/>
@@ -8886,8 +8910,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O82" s="539"/>
-      <c r="P82" s="541"/>
+      <c r="O82" s="528"/>
+      <c r="P82" s="542"/>
       <c r="Q82" s="164"/>
       <c r="R82" s="129"/>
       <c r="S82" s="180"/>
@@ -8919,8 +8943,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O83" s="540"/>
-      <c r="P83" s="542"/>
+      <c r="O83" s="529"/>
+      <c r="P83" s="543"/>
       <c r="Q83" s="164"/>
       <c r="R83" s="129"/>
       <c r="S83" s="180"/>
@@ -8952,8 +8976,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O84" s="539"/>
-      <c r="P84" s="541"/>
+      <c r="O84" s="528"/>
+      <c r="P84" s="542"/>
       <c r="Q84" s="164"/>
       <c r="R84" s="158"/>
       <c r="S84" s="180"/>
@@ -8985,8 +9009,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O85" s="540"/>
-      <c r="P85" s="542"/>
+      <c r="O85" s="529"/>
+      <c r="P85" s="543"/>
       <c r="Q85" s="164"/>
       <c r="R85" s="158"/>
       <c r="S85" s="180"/>
@@ -9144,8 +9168,8 @@
         <v>0</v>
       </c>
       <c r="K90" s="100"/>
-      <c r="L90" s="543"/>
-      <c r="M90" s="544"/>
+      <c r="L90" s="544"/>
+      <c r="M90" s="545"/>
       <c r="N90" s="77">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -9177,8 +9201,8 @@
         <v>0</v>
       </c>
       <c r="K91" s="100"/>
-      <c r="L91" s="543"/>
-      <c r="M91" s="544"/>
+      <c r="L91" s="544"/>
+      <c r="M91" s="545"/>
       <c r="N91" s="77">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -9381,8 +9405,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O97" s="539"/>
-      <c r="P97" s="535"/>
+      <c r="O97" s="528"/>
+      <c r="P97" s="538"/>
       <c r="Q97" s="164"/>
       <c r="R97" s="129"/>
       <c r="S97" s="180"/>
@@ -9414,8 +9438,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O98" s="540"/>
-      <c r="P98" s="536"/>
+      <c r="O98" s="529"/>
+      <c r="P98" s="539"/>
       <c r="Q98" s="164"/>
       <c r="R98" s="129"/>
       <c r="S98" s="180"/>
@@ -14807,11 +14831,11 @@
         <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
-      <c r="F262" s="537" t="s">
+      <c r="F262" s="540" t="s">
         <v>26</v>
       </c>
-      <c r="G262" s="537"/>
-      <c r="H262" s="538"/>
+      <c r="G262" s="540"/>
+      <c r="H262" s="541"/>
       <c r="I262" s="317">
         <f>SUM(I4:I261)</f>
         <v>426245.47000000003</v>
@@ -15385,22 +15409,6 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="P68:P69"/>
-    <mergeCell ref="C63:C64"/>
-    <mergeCell ref="H63:H64"/>
-    <mergeCell ref="O68:O69"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="C58:C59"/>
-    <mergeCell ref="H58:H59"/>
-    <mergeCell ref="O58:O59"/>
-    <mergeCell ref="P97:P98"/>
-    <mergeCell ref="F262:H262"/>
-    <mergeCell ref="O82:O83"/>
-    <mergeCell ref="P82:P83"/>
-    <mergeCell ref="O84:O85"/>
-    <mergeCell ref="P84:P85"/>
-    <mergeCell ref="L90:M91"/>
-    <mergeCell ref="O97:O98"/>
     <mergeCell ref="A1:J2"/>
     <mergeCell ref="W1:X1"/>
     <mergeCell ref="O3:P3"/>
@@ -15414,6 +15422,22 @@
     <mergeCell ref="C56:C57"/>
     <mergeCell ref="H56:H57"/>
     <mergeCell ref="P58:P59"/>
+    <mergeCell ref="P97:P98"/>
+    <mergeCell ref="F262:H262"/>
+    <mergeCell ref="O82:O83"/>
+    <mergeCell ref="P82:P83"/>
+    <mergeCell ref="O84:O85"/>
+    <mergeCell ref="P84:P85"/>
+    <mergeCell ref="L90:M91"/>
+    <mergeCell ref="O97:O98"/>
+    <mergeCell ref="P68:P69"/>
+    <mergeCell ref="C63:C64"/>
+    <mergeCell ref="H63:H64"/>
+    <mergeCell ref="O68:O69"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="H58:H59"/>
+    <mergeCell ref="O58:O59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -15421,7 +15445,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Hoja2">
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
@@ -15457,49 +15481,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="42.75" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A1" s="514" t="s">
+      <c r="A1" s="546" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="514"/>
-      <c r="C1" s="514"/>
-      <c r="D1" s="514"/>
-      <c r="E1" s="514"/>
-      <c r="F1" s="514"/>
-      <c r="G1" s="514"/>
-      <c r="H1" s="514"/>
-      <c r="I1" s="514"/>
-      <c r="J1" s="514"/>
+      <c r="B1" s="546"/>
+      <c r="C1" s="546"/>
+      <c r="D1" s="546"/>
+      <c r="E1" s="546"/>
+      <c r="F1" s="546"/>
+      <c r="G1" s="546"/>
+      <c r="H1" s="546"/>
+      <c r="I1" s="546"/>
+      <c r="J1" s="546"/>
       <c r="K1" s="375"/>
       <c r="L1" s="375"/>
       <c r="M1" s="375"/>
       <c r="N1" s="375"/>
       <c r="O1" s="376"/>
-      <c r="S1" s="557" t="s">
+      <c r="S1" s="565" t="s">
         <v>142</v>
       </c>
-      <c r="T1" s="557"/>
+      <c r="T1" s="565"/>
       <c r="U1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="V1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="W1" s="515" t="s">
+      <c r="W1" s="547" t="s">
         <v>2</v>
       </c>
-      <c r="X1" s="516"/>
+      <c r="X1" s="548"/>
     </row>
     <row r="2" spans="1:24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="514"/>
-      <c r="B2" s="514"/>
-      <c r="C2" s="514"/>
-      <c r="D2" s="514"/>
-      <c r="E2" s="514"/>
-      <c r="F2" s="514"/>
-      <c r="G2" s="514"/>
-      <c r="H2" s="514"/>
-      <c r="I2" s="514"/>
-      <c r="J2" s="514"/>
+      <c r="A2" s="546"/>
+      <c r="B2" s="546"/>
+      <c r="C2" s="546"/>
+      <c r="D2" s="546"/>
+      <c r="E2" s="546"/>
+      <c r="F2" s="546"/>
+      <c r="G2" s="546"/>
+      <c r="H2" s="546"/>
+      <c r="I2" s="546"/>
+      <c r="J2" s="546"/>
       <c r="K2" s="377"/>
       <c r="L2" s="377"/>
       <c r="M2" s="377"/>
@@ -15507,8 +15531,8 @@
       <c r="O2" s="379"/>
       <c r="Q2" s="10"/>
       <c r="R2" s="11"/>
-      <c r="S2" s="558"/>
-      <c r="T2" s="558"/>
+      <c r="S2" s="566"/>
+      <c r="T2" s="566"/>
       <c r="U2" s="14"/>
       <c r="V2" s="15"/>
       <c r="W2" s="16"/>
@@ -15553,10 +15577,10 @@
       <c r="N3" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="517" t="s">
+      <c r="O3" s="549" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="518"/>
+      <c r="P3" s="550"/>
       <c r="Q3" s="30" t="s">
         <v>16</v>
       </c>
@@ -18192,13 +18216,13 @@
       <c r="V54" s="160"/>
     </row>
     <row r="55" spans="1:24" s="161" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="559" t="s">
+      <c r="A55" s="567" t="s">
         <v>41</v>
       </c>
       <c r="B55" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="C55" s="533" t="s">
+      <c r="C55" s="532" t="s">
         <v>160</v>
       </c>
       <c r="D55" s="150"/>
@@ -18209,7 +18233,7 @@
       <c r="G55" s="152">
         <v>44599</v>
       </c>
-      <c r="H55" s="549" t="s">
+      <c r="H55" s="526" t="s">
         <v>161</v>
       </c>
       <c r="I55" s="151">
@@ -18238,11 +18262,11 @@
       <c r="V55" s="160"/>
     </row>
     <row r="56" spans="1:24" s="161" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="560"/>
+      <c r="A56" s="568"/>
       <c r="B56" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="C56" s="534"/>
+      <c r="C56" s="533"/>
       <c r="D56" s="163"/>
       <c r="E56" s="40"/>
       <c r="F56" s="151">
@@ -18251,7 +18275,7 @@
       <c r="G56" s="152">
         <v>44599</v>
       </c>
-      <c r="H56" s="550"/>
+      <c r="H56" s="527"/>
       <c r="I56" s="151">
         <v>194.4</v>
       </c>
@@ -18280,13 +18304,13 @@
       <c r="X56"/>
     </row>
     <row r="57" spans="1:24" ht="26.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="551" t="s">
+      <c r="A57" s="559" t="s">
         <v>41</v>
       </c>
       <c r="B57" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="C57" s="553" t="s">
+      <c r="C57" s="561" t="s">
         <v>162</v>
       </c>
       <c r="D57" s="165"/>
@@ -18297,7 +18321,7 @@
       <c r="G57" s="152">
         <v>44606</v>
       </c>
-      <c r="H57" s="549" t="s">
+      <c r="H57" s="526" t="s">
         <v>163</v>
       </c>
       <c r="I57" s="151">
@@ -18316,10 +18340,10 @@
         <f t="shared" si="1"/>
         <v>35776</v>
       </c>
-      <c r="O57" s="539" t="s">
+      <c r="O57" s="528" t="s">
         <v>59</v>
       </c>
-      <c r="P57" s="545">
+      <c r="P57" s="522">
         <v>44620</v>
       </c>
       <c r="Q57" s="164"/>
@@ -18330,11 +18354,11 @@
       <c r="V57" s="54"/>
     </row>
     <row r="58" spans="1:24" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="552"/>
+      <c r="A58" s="560"/>
       <c r="B58" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="C58" s="554"/>
+      <c r="C58" s="562"/>
       <c r="D58" s="165"/>
       <c r="E58" s="40"/>
       <c r="F58" s="151">
@@ -18343,7 +18367,7 @@
       <c r="G58" s="152">
         <v>44606</v>
       </c>
-      <c r="H58" s="550"/>
+      <c r="H58" s="527"/>
       <c r="I58" s="151">
         <v>627.60209999999995</v>
       </c>
@@ -18360,8 +18384,8 @@
         <f t="shared" si="1"/>
         <v>58366.995299999995</v>
       </c>
-      <c r="O58" s="555"/>
-      <c r="P58" s="556"/>
+      <c r="O58" s="563"/>
+      <c r="P58" s="564"/>
       <c r="Q58" s="164"/>
       <c r="R58" s="129"/>
       <c r="S58" s="92"/>
@@ -18387,7 +18411,7 @@
       <c r="G59" s="152">
         <v>44613</v>
       </c>
-      <c r="H59" s="549" t="s">
+      <c r="H59" s="526" t="s">
         <v>225</v>
       </c>
       <c r="I59" s="151">
@@ -18431,7 +18455,7 @@
       <c r="E60" s="40"/>
       <c r="F60" s="151"/>
       <c r="G60" s="152"/>
-      <c r="H60" s="550"/>
+      <c r="H60" s="527"/>
       <c r="I60" s="151"/>
       <c r="J60" s="45">
         <f t="shared" si="0"/>
@@ -19094,8 +19118,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O79" s="539"/>
-      <c r="P79" s="541"/>
+      <c r="O79" s="528"/>
+      <c r="P79" s="542"/>
       <c r="Q79" s="164"/>
       <c r="R79" s="129"/>
       <c r="S79" s="180"/>
@@ -19124,8 +19148,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O80" s="540"/>
-      <c r="P80" s="542"/>
+      <c r="O80" s="529"/>
+      <c r="P80" s="543"/>
       <c r="Q80" s="164"/>
       <c r="R80" s="129"/>
       <c r="S80" s="180"/>
@@ -19154,8 +19178,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O81" s="539"/>
-      <c r="P81" s="541"/>
+      <c r="O81" s="528"/>
+      <c r="P81" s="542"/>
       <c r="Q81" s="164"/>
       <c r="R81" s="158"/>
       <c r="S81" s="180"/>
@@ -19187,8 +19211,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O82" s="540"/>
-      <c r="P82" s="542"/>
+      <c r="O82" s="529"/>
+      <c r="P82" s="543"/>
       <c r="Q82" s="164"/>
       <c r="R82" s="158"/>
       <c r="S82" s="180"/>
@@ -19346,8 +19370,8 @@
         <v>0</v>
       </c>
       <c r="K87" s="100"/>
-      <c r="L87" s="543"/>
-      <c r="M87" s="544"/>
+      <c r="L87" s="544"/>
+      <c r="M87" s="545"/>
       <c r="N87" s="77">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -19379,8 +19403,8 @@
         <v>0</v>
       </c>
       <c r="K88" s="100"/>
-      <c r="L88" s="543"/>
-      <c r="M88" s="544"/>
+      <c r="L88" s="544"/>
+      <c r="M88" s="545"/>
       <c r="N88" s="77">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -19583,8 +19607,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O94" s="539"/>
-      <c r="P94" s="535"/>
+      <c r="O94" s="528"/>
+      <c r="P94" s="538"/>
       <c r="Q94" s="164"/>
       <c r="R94" s="129"/>
       <c r="S94" s="180"/>
@@ -19616,8 +19640,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O95" s="540"/>
-      <c r="P95" s="536"/>
+      <c r="O95" s="529"/>
+      <c r="P95" s="539"/>
       <c r="Q95" s="164"/>
       <c r="R95" s="129"/>
       <c r="S95" s="180"/>
@@ -25009,11 +25033,11 @@
         <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
-      <c r="F259" s="537" t="s">
+      <c r="F259" s="540" t="s">
         <v>26</v>
       </c>
-      <c r="G259" s="537"/>
-      <c r="H259" s="538"/>
+      <c r="G259" s="540"/>
+      <c r="H259" s="541"/>
       <c r="I259" s="317">
         <f>SUM(I4:I258)</f>
         <v>387207.97210000001</v>
@@ -25587,6 +25611,12 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="F259:H259"/>
+    <mergeCell ref="O81:O82"/>
+    <mergeCell ref="P81:P82"/>
+    <mergeCell ref="L87:M88"/>
+    <mergeCell ref="O94:O95"/>
+    <mergeCell ref="P94:P95"/>
     <mergeCell ref="O79:O80"/>
     <mergeCell ref="P79:P80"/>
     <mergeCell ref="A1:J2"/>
@@ -25602,12 +25632,6 @@
     <mergeCell ref="C55:C56"/>
     <mergeCell ref="A55:A56"/>
     <mergeCell ref="H55:H56"/>
-    <mergeCell ref="F259:H259"/>
-    <mergeCell ref="O81:O82"/>
-    <mergeCell ref="P81:P82"/>
-    <mergeCell ref="L87:M88"/>
-    <mergeCell ref="O94:O95"/>
-    <mergeCell ref="P94:P95"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -25615,7 +25639,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Hoja3">
     <tabColor rgb="FFFF5050"/>
   </sheetPr>
@@ -25654,49 +25678,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="42.75" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A1" s="514" t="s">
+      <c r="A1" s="546" t="s">
         <v>189</v>
       </c>
-      <c r="B1" s="514"/>
-      <c r="C1" s="514"/>
-      <c r="D1" s="514"/>
-      <c r="E1" s="514"/>
-      <c r="F1" s="514"/>
-      <c r="G1" s="514"/>
-      <c r="H1" s="514"/>
-      <c r="I1" s="514"/>
-      <c r="J1" s="514"/>
+      <c r="B1" s="546"/>
+      <c r="C1" s="546"/>
+      <c r="D1" s="546"/>
+      <c r="E1" s="546"/>
+      <c r="F1" s="546"/>
+      <c r="G1" s="546"/>
+      <c r="H1" s="546"/>
+      <c r="I1" s="546"/>
+      <c r="J1" s="546"/>
       <c r="K1" s="375"/>
       <c r="L1" s="375"/>
       <c r="M1" s="375"/>
       <c r="N1" s="375"/>
       <c r="O1" s="376"/>
-      <c r="S1" s="557" t="s">
+      <c r="S1" s="565" t="s">
         <v>142</v>
       </c>
-      <c r="T1" s="557"/>
+      <c r="T1" s="565"/>
       <c r="U1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="V1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="W1" s="515" t="s">
+      <c r="W1" s="547" t="s">
         <v>2</v>
       </c>
-      <c r="X1" s="516"/>
+      <c r="X1" s="548"/>
     </row>
     <row r="2" spans="1:24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="514"/>
-      <c r="B2" s="514"/>
-      <c r="C2" s="514"/>
-      <c r="D2" s="514"/>
-      <c r="E2" s="514"/>
-      <c r="F2" s="514"/>
-      <c r="G2" s="514"/>
-      <c r="H2" s="514"/>
-      <c r="I2" s="514"/>
-      <c r="J2" s="514"/>
+      <c r="A2" s="546"/>
+      <c r="B2" s="546"/>
+      <c r="C2" s="546"/>
+      <c r="D2" s="546"/>
+      <c r="E2" s="546"/>
+      <c r="F2" s="546"/>
+      <c r="G2" s="546"/>
+      <c r="H2" s="546"/>
+      <c r="I2" s="546"/>
+      <c r="J2" s="546"/>
       <c r="K2" s="377"/>
       <c r="L2" s="377"/>
       <c r="M2" s="377"/>
@@ -25704,8 +25728,8 @@
       <c r="O2" s="379"/>
       <c r="Q2" s="10"/>
       <c r="R2" s="11"/>
-      <c r="S2" s="558"/>
-      <c r="T2" s="558"/>
+      <c r="S2" s="566"/>
+      <c r="T2" s="566"/>
       <c r="U2" s="14"/>
       <c r="V2" s="15"/>
       <c r="W2" s="16"/>
@@ -25750,10 +25774,10 @@
       <c r="N3" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="517" t="s">
+      <c r="O3" s="549" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="518"/>
+      <c r="P3" s="550"/>
       <c r="Q3" s="30" t="s">
         <v>16</v>
       </c>
@@ -28961,13 +28985,13 @@
       <c r="V54" s="160"/>
     </row>
     <row r="55" spans="1:24" s="161" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="559" t="s">
+      <c r="A55" s="567" t="s">
         <v>41</v>
       </c>
       <c r="B55" s="438" t="s">
         <v>24</v>
       </c>
-      <c r="C55" s="533" t="s">
+      <c r="C55" s="532" t="s">
         <v>229</v>
       </c>
       <c r="D55" s="439"/>
@@ -28978,7 +29002,7 @@
       <c r="G55" s="152">
         <v>44627</v>
       </c>
-      <c r="H55" s="562" t="s">
+      <c r="H55" s="572" t="s">
         <v>230</v>
       </c>
       <c r="I55" s="151">
@@ -28997,10 +29021,10 @@
         <f t="shared" si="1"/>
         <v>18886.399999999998</v>
       </c>
-      <c r="O55" s="539" t="s">
+      <c r="O55" s="528" t="s">
         <v>59</v>
       </c>
-      <c r="P55" s="545">
+      <c r="P55" s="522">
         <v>44645</v>
       </c>
       <c r="Q55" s="128"/>
@@ -29011,11 +29035,11 @@
       <c r="V55" s="160"/>
     </row>
     <row r="56" spans="1:24" s="161" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="561"/>
+      <c r="A56" s="571"/>
       <c r="B56" s="438" t="s">
         <v>24</v>
       </c>
-      <c r="C56" s="534"/>
+      <c r="C56" s="533"/>
       <c r="D56" s="440"/>
       <c r="E56" s="60"/>
       <c r="F56" s="151">
@@ -29024,7 +29048,7 @@
       <c r="G56" s="152">
         <v>44627</v>
       </c>
-      <c r="H56" s="563"/>
+      <c r="H56" s="573"/>
       <c r="I56" s="151">
         <v>967</v>
       </c>
@@ -29041,8 +29065,8 @@
         <f t="shared" si="1"/>
         <v>92832</v>
       </c>
-      <c r="O56" s="540"/>
-      <c r="P56" s="546"/>
+      <c r="O56" s="529"/>
+      <c r="P56" s="523"/>
       <c r="Q56" s="164"/>
       <c r="R56" s="158"/>
       <c r="S56" s="92"/>
@@ -29103,13 +29127,13 @@
       <c r="V57" s="54"/>
     </row>
     <row r="58" spans="1:24" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="523" t="s">
+      <c r="A58" s="555" t="s">
         <v>41</v>
       </c>
       <c r="B58" s="170" t="s">
         <v>24</v>
       </c>
-      <c r="C58" s="572" t="s">
+      <c r="C58" s="569" t="s">
         <v>319</v>
       </c>
       <c r="D58" s="165"/>
@@ -29120,7 +29144,7 @@
       <c r="G58" s="152">
         <v>44648</v>
       </c>
-      <c r="H58" s="570" t="s">
+      <c r="H58" s="580" t="s">
         <v>315</v>
       </c>
       <c r="I58" s="151">
@@ -29139,10 +29163,10 @@
         <f t="shared" si="1"/>
         <v>35255.600000000006</v>
       </c>
-      <c r="O58" s="527" t="s">
+      <c r="O58" s="536" t="s">
         <v>59</v>
       </c>
-      <c r="P58" s="529">
+      <c r="P58" s="557">
         <v>44662</v>
       </c>
       <c r="Q58" s="164"/>
@@ -29153,11 +29177,11 @@
       <c r="V58" s="54"/>
     </row>
     <row r="59" spans="1:24" s="161" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="524"/>
+      <c r="A59" s="556"/>
       <c r="B59" s="170" t="s">
         <v>23</v>
       </c>
-      <c r="C59" s="573"/>
+      <c r="C59" s="570"/>
       <c r="D59" s="163"/>
       <c r="E59" s="60"/>
       <c r="F59" s="151">
@@ -29166,7 +29190,7 @@
       <c r="G59" s="152">
         <v>44648</v>
       </c>
-      <c r="H59" s="571"/>
+      <c r="H59" s="581"/>
       <c r="I59" s="151">
         <v>719</v>
       </c>
@@ -29183,8 +29207,8 @@
         <f t="shared" si="1"/>
         <v>69024</v>
       </c>
-      <c r="O59" s="528"/>
-      <c r="P59" s="530"/>
+      <c r="O59" s="537"/>
+      <c r="P59" s="558"/>
       <c r="Q59" s="164"/>
       <c r="R59" s="158"/>
       <c r="S59" s="92"/>
@@ -29257,13 +29281,13 @@
       <c r="V61" s="54"/>
     </row>
     <row r="62" spans="1:24" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A62" s="564" t="s">
+      <c r="A62" s="574" t="s">
         <v>106</v>
       </c>
       <c r="B62" s="178" t="s">
         <v>237</v>
       </c>
-      <c r="C62" s="566" t="s">
+      <c r="C62" s="576" t="s">
         <v>238</v>
       </c>
       <c r="D62" s="168"/>
@@ -29274,7 +29298,7 @@
       <c r="G62" s="152">
         <v>44622</v>
       </c>
-      <c r="H62" s="568">
+      <c r="H62" s="578">
         <v>37162</v>
       </c>
       <c r="I62" s="151">
@@ -29293,10 +29317,10 @@
         <f t="shared" si="1"/>
         <v>7782.5999999999995</v>
       </c>
-      <c r="O62" s="539" t="s">
+      <c r="O62" s="528" t="s">
         <v>61</v>
       </c>
-      <c r="P62" s="545">
+      <c r="P62" s="522">
         <v>44643</v>
       </c>
       <c r="Q62" s="164"/>
@@ -29307,11 +29331,11 @@
       <c r="V62" s="54"/>
     </row>
     <row r="63" spans="1:24" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A63" s="565"/>
+      <c r="A63" s="575"/>
       <c r="B63" s="178" t="s">
         <v>239</v>
       </c>
-      <c r="C63" s="567"/>
+      <c r="C63" s="577"/>
       <c r="D63" s="168"/>
       <c r="E63" s="60"/>
       <c r="F63" s="151">
@@ -29320,7 +29344,7 @@
       <c r="G63" s="152">
         <v>44622</v>
       </c>
-      <c r="H63" s="569"/>
+      <c r="H63" s="579"/>
       <c r="I63" s="151">
         <v>204.8</v>
       </c>
@@ -29337,8 +29361,8 @@
         <f t="shared" si="1"/>
         <v>16998.400000000001</v>
       </c>
-      <c r="O63" s="540"/>
-      <c r="P63" s="546"/>
+      <c r="O63" s="529"/>
+      <c r="P63" s="523"/>
       <c r="Q63" s="164"/>
       <c r="R63" s="129"/>
       <c r="S63" s="92"/>
@@ -29817,8 +29841,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O79" s="539"/>
-      <c r="P79" s="541"/>
+      <c r="O79" s="528"/>
+      <c r="P79" s="542"/>
       <c r="Q79" s="164"/>
       <c r="R79" s="129"/>
       <c r="S79" s="180"/>
@@ -29847,8 +29871,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O80" s="540"/>
-      <c r="P80" s="542"/>
+      <c r="O80" s="529"/>
+      <c r="P80" s="543"/>
       <c r="Q80" s="164"/>
       <c r="R80" s="129"/>
       <c r="S80" s="180"/>
@@ -29877,8 +29901,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O81" s="539"/>
-      <c r="P81" s="541"/>
+      <c r="O81" s="528"/>
+      <c r="P81" s="542"/>
       <c r="Q81" s="164"/>
       <c r="R81" s="158"/>
       <c r="S81" s="180"/>
@@ -29910,8 +29934,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O82" s="540"/>
-      <c r="P82" s="542"/>
+      <c r="O82" s="529"/>
+      <c r="P82" s="543"/>
       <c r="Q82" s="164"/>
       <c r="R82" s="158"/>
       <c r="S82" s="180"/>
@@ -30069,8 +30093,8 @@
         <v>0</v>
       </c>
       <c r="K87" s="100"/>
-      <c r="L87" s="543"/>
-      <c r="M87" s="544"/>
+      <c r="L87" s="544"/>
+      <c r="M87" s="545"/>
       <c r="N87" s="48">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -30102,8 +30126,8 @@
         <v>0</v>
       </c>
       <c r="K88" s="100"/>
-      <c r="L88" s="543"/>
-      <c r="M88" s="544"/>
+      <c r="L88" s="544"/>
+      <c r="M88" s="545"/>
       <c r="N88" s="48">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -30306,8 +30330,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O94" s="539"/>
-      <c r="P94" s="535"/>
+      <c r="O94" s="528"/>
+      <c r="P94" s="538"/>
       <c r="Q94" s="164"/>
       <c r="R94" s="129"/>
       <c r="S94" s="180"/>
@@ -30339,8 +30363,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O95" s="540"/>
-      <c r="P95" s="536"/>
+      <c r="O95" s="529"/>
+      <c r="P95" s="539"/>
       <c r="Q95" s="164"/>
       <c r="R95" s="129"/>
       <c r="S95" s="180"/>
@@ -35732,11 +35756,11 @@
         <f t="shared" si="10"/>
         <v>#VALUE!</v>
       </c>
-      <c r="F259" s="537" t="s">
+      <c r="F259" s="540" t="s">
         <v>26</v>
       </c>
-      <c r="G259" s="537"/>
-      <c r="H259" s="538"/>
+      <c r="G259" s="540"/>
+      <c r="H259" s="541"/>
       <c r="I259" s="317">
         <f>SUM(I4:I258)</f>
         <v>517031.52999999991</v>
@@ -36310,17 +36334,6 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="O58:O59"/>
-    <mergeCell ref="P58:P59"/>
-    <mergeCell ref="C58:C59"/>
-    <mergeCell ref="O94:O95"/>
-    <mergeCell ref="P94:P95"/>
-    <mergeCell ref="F259:H259"/>
-    <mergeCell ref="O79:O80"/>
-    <mergeCell ref="P79:P80"/>
-    <mergeCell ref="O81:O82"/>
-    <mergeCell ref="P81:P82"/>
     <mergeCell ref="A1:J2"/>
     <mergeCell ref="S1:T2"/>
     <mergeCell ref="W1:X1"/>
@@ -36337,6 +36350,17 @@
     <mergeCell ref="O62:O63"/>
     <mergeCell ref="P62:P63"/>
     <mergeCell ref="H58:H59"/>
+    <mergeCell ref="F259:H259"/>
+    <mergeCell ref="O79:O80"/>
+    <mergeCell ref="P79:P80"/>
+    <mergeCell ref="O81:O82"/>
+    <mergeCell ref="P81:P82"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="O58:O59"/>
+    <mergeCell ref="P58:P59"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="O94:O95"/>
+    <mergeCell ref="P94:P95"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -36344,7 +36368,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Hoja4">
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
@@ -36383,49 +36407,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="42.75" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A1" s="514" t="s">
+      <c r="A1" s="546" t="s">
         <v>288</v>
       </c>
-      <c r="B1" s="514"/>
-      <c r="C1" s="514"/>
-      <c r="D1" s="514"/>
-      <c r="E1" s="514"/>
-      <c r="F1" s="514"/>
-      <c r="G1" s="514"/>
-      <c r="H1" s="514"/>
-      <c r="I1" s="514"/>
-      <c r="J1" s="514"/>
+      <c r="B1" s="546"/>
+      <c r="C1" s="546"/>
+      <c r="D1" s="546"/>
+      <c r="E1" s="546"/>
+      <c r="F1" s="546"/>
+      <c r="G1" s="546"/>
+      <c r="H1" s="546"/>
+      <c r="I1" s="546"/>
+      <c r="J1" s="546"/>
       <c r="K1" s="375"/>
       <c r="L1" s="375"/>
       <c r="M1" s="375"/>
       <c r="N1" s="375"/>
       <c r="O1" s="376"/>
-      <c r="S1" s="557" t="s">
+      <c r="S1" s="565" t="s">
         <v>142</v>
       </c>
-      <c r="T1" s="557"/>
+      <c r="T1" s="565"/>
       <c r="U1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="V1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="W1" s="515" t="s">
+      <c r="W1" s="547" t="s">
         <v>2</v>
       </c>
-      <c r="X1" s="516"/>
+      <c r="X1" s="548"/>
     </row>
     <row r="2" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="514"/>
-      <c r="B2" s="514"/>
-      <c r="C2" s="514"/>
-      <c r="D2" s="514"/>
-      <c r="E2" s="514"/>
-      <c r="F2" s="514"/>
-      <c r="G2" s="514"/>
-      <c r="H2" s="514"/>
-      <c r="I2" s="514"/>
-      <c r="J2" s="514"/>
+      <c r="A2" s="546"/>
+      <c r="B2" s="546"/>
+      <c r="C2" s="546"/>
+      <c r="D2" s="546"/>
+      <c r="E2" s="546"/>
+      <c r="F2" s="546"/>
+      <c r="G2" s="546"/>
+      <c r="H2" s="546"/>
+      <c r="I2" s="546"/>
+      <c r="J2" s="546"/>
       <c r="K2" s="377"/>
       <c r="L2" s="377"/>
       <c r="M2" s="377"/>
@@ -36433,8 +36457,8 @@
       <c r="O2" s="379"/>
       <c r="Q2" s="10"/>
       <c r="R2" s="11"/>
-      <c r="S2" s="558"/>
-      <c r="T2" s="558"/>
+      <c r="S2" s="566"/>
+      <c r="T2" s="566"/>
       <c r="U2" s="14"/>
       <c r="V2" s="15"/>
       <c r="W2" s="16"/>
@@ -36479,10 +36503,10 @@
       <c r="N3" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="517" t="s">
+      <c r="O3" s="549" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="518"/>
+      <c r="P3" s="550"/>
       <c r="Q3" s="30" t="s">
         <v>16</v>
       </c>
@@ -39864,13 +39888,13 @@
       <c r="V63" s="54"/>
     </row>
     <row r="64" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="559" t="s">
+      <c r="A64" s="567" t="s">
         <v>111</v>
       </c>
       <c r="B64" s="178" t="s">
         <v>464</v>
       </c>
-      <c r="C64" s="566" t="s">
+      <c r="C64" s="576" t="s">
         <v>465</v>
       </c>
       <c r="D64" s="171"/>
@@ -39881,7 +39905,7 @@
       <c r="G64" s="504">
         <v>44681</v>
       </c>
-      <c r="H64" s="574">
+      <c r="H64" s="582">
         <v>132899</v>
       </c>
       <c r="I64" s="505">
@@ -39900,10 +39924,10 @@
         <f t="shared" si="1"/>
         <v>19360</v>
       </c>
-      <c r="O64" s="576" t="s">
+      <c r="O64" s="584" t="s">
         <v>59</v>
       </c>
-      <c r="P64" s="578">
+      <c r="P64" s="586">
         <v>44708</v>
       </c>
       <c r="Q64" s="167"/>
@@ -39914,11 +39938,11 @@
       <c r="V64" s="54"/>
     </row>
     <row r="65" spans="1:22" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="561"/>
+      <c r="A65" s="571"/>
       <c r="B65" s="178" t="s">
         <v>240</v>
       </c>
-      <c r="C65" s="567"/>
+      <c r="C65" s="577"/>
       <c r="D65" s="171"/>
       <c r="E65" s="60"/>
       <c r="F65" s="151">
@@ -39927,7 +39951,7 @@
       <c r="G65" s="504">
         <v>44681</v>
       </c>
-      <c r="H65" s="575"/>
+      <c r="H65" s="583"/>
       <c r="I65" s="505">
         <v>508</v>
       </c>
@@ -39944,8 +39968,8 @@
         <f t="shared" si="1"/>
         <v>32512</v>
       </c>
-      <c r="O65" s="577"/>
-      <c r="P65" s="579"/>
+      <c r="O65" s="585"/>
+      <c r="P65" s="587"/>
       <c r="Q65" s="167"/>
       <c r="R65" s="129"/>
       <c r="S65" s="180"/>
@@ -40364,8 +40388,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O79" s="539"/>
-      <c r="P79" s="541"/>
+      <c r="O79" s="528"/>
+      <c r="P79" s="542"/>
       <c r="Q79" s="164"/>
       <c r="R79" s="129"/>
       <c r="S79" s="180"/>
@@ -40394,8 +40418,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O80" s="540"/>
-      <c r="P80" s="542"/>
+      <c r="O80" s="529"/>
+      <c r="P80" s="543"/>
       <c r="Q80" s="164"/>
       <c r="R80" s="129"/>
       <c r="S80" s="180"/>
@@ -40424,8 +40448,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O81" s="539"/>
-      <c r="P81" s="541"/>
+      <c r="O81" s="528"/>
+      <c r="P81" s="542"/>
       <c r="Q81" s="164"/>
       <c r="R81" s="158"/>
       <c r="S81" s="180"/>
@@ -40457,8 +40481,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O82" s="540"/>
-      <c r="P82" s="542"/>
+      <c r="O82" s="529"/>
+      <c r="P82" s="543"/>
       <c r="Q82" s="164"/>
       <c r="R82" s="158"/>
       <c r="S82" s="180"/>
@@ -40616,8 +40640,8 @@
         <v>0</v>
       </c>
       <c r="K87" s="100"/>
-      <c r="L87" s="543"/>
-      <c r="M87" s="544"/>
+      <c r="L87" s="544"/>
+      <c r="M87" s="545"/>
       <c r="N87" s="48">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -40649,8 +40673,8 @@
         <v>0</v>
       </c>
       <c r="K88" s="100"/>
-      <c r="L88" s="543"/>
-      <c r="M88" s="544"/>
+      <c r="L88" s="544"/>
+      <c r="M88" s="545"/>
       <c r="N88" s="48">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -40853,8 +40877,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O94" s="539"/>
-      <c r="P94" s="535"/>
+      <c r="O94" s="528"/>
+      <c r="P94" s="538"/>
       <c r="Q94" s="164"/>
       <c r="R94" s="129"/>
       <c r="S94" s="180"/>
@@ -40886,8 +40910,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O95" s="540"/>
-      <c r="P95" s="536"/>
+      <c r="O95" s="529"/>
+      <c r="P95" s="539"/>
       <c r="Q95" s="164"/>
       <c r="R95" s="129"/>
       <c r="S95" s="180"/>
@@ -46279,11 +46303,11 @@
         <f t="shared" si="11"/>
         <v>#VALUE!</v>
       </c>
-      <c r="F259" s="537" t="s">
+      <c r="F259" s="540" t="s">
         <v>26</v>
       </c>
-      <c r="G259" s="537"/>
-      <c r="H259" s="538"/>
+      <c r="G259" s="540"/>
+      <c r="H259" s="541"/>
       <c r="I259" s="317">
         <f>SUM(I4:I258)</f>
         <v>491966.85000000003</v>
@@ -46857,6 +46881,12 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="F259:H259"/>
+    <mergeCell ref="O81:O82"/>
+    <mergeCell ref="P81:P82"/>
+    <mergeCell ref="L87:M88"/>
+    <mergeCell ref="O94:O95"/>
+    <mergeCell ref="P94:P95"/>
     <mergeCell ref="W1:X1"/>
     <mergeCell ref="O3:P3"/>
     <mergeCell ref="O79:O80"/>
@@ -46868,12 +46898,6 @@
     <mergeCell ref="H64:H65"/>
     <mergeCell ref="O64:O65"/>
     <mergeCell ref="P64:P65"/>
-    <mergeCell ref="F259:H259"/>
-    <mergeCell ref="O81:O82"/>
-    <mergeCell ref="P81:P82"/>
-    <mergeCell ref="L87:M88"/>
-    <mergeCell ref="O94:O95"/>
-    <mergeCell ref="P94:P95"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -46881,17 +46905,17 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Hoja5">
     <tabColor theme="0" tint="-0.499984740745262"/>
   </sheetPr>
   <dimension ref="A1:X292"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="8" ySplit="3" topLeftCell="R19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="8" ySplit="3" topLeftCell="R31" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="U17" sqref="U17"/>
+      <selection pane="bottomRight" activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -46920,49 +46944,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="42.75" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A1" s="514" t="s">
+      <c r="A1" s="546" t="s">
         <v>402</v>
       </c>
-      <c r="B1" s="514"/>
-      <c r="C1" s="514"/>
-      <c r="D1" s="514"/>
-      <c r="E1" s="514"/>
-      <c r="F1" s="514"/>
-      <c r="G1" s="514"/>
-      <c r="H1" s="514"/>
-      <c r="I1" s="514"/>
-      <c r="J1" s="514"/>
+      <c r="B1" s="546"/>
+      <c r="C1" s="546"/>
+      <c r="D1" s="546"/>
+      <c r="E1" s="546"/>
+      <c r="F1" s="546"/>
+      <c r="G1" s="546"/>
+      <c r="H1" s="546"/>
+      <c r="I1" s="546"/>
+      <c r="J1" s="546"/>
       <c r="K1" s="375"/>
       <c r="L1" s="375"/>
       <c r="M1" s="375"/>
       <c r="N1" s="375"/>
       <c r="O1" s="376"/>
-      <c r="S1" s="557" t="s">
+      <c r="S1" s="565" t="s">
         <v>142</v>
       </c>
-      <c r="T1" s="557"/>
+      <c r="T1" s="565"/>
       <c r="U1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="V1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="W1" s="515" t="s">
+      <c r="W1" s="547" t="s">
         <v>2</v>
       </c>
-      <c r="X1" s="516"/>
+      <c r="X1" s="548"/>
     </row>
     <row r="2" spans="1:24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="514"/>
-      <c r="B2" s="514"/>
-      <c r="C2" s="514"/>
-      <c r="D2" s="514"/>
-      <c r="E2" s="514"/>
-      <c r="F2" s="514"/>
-      <c r="G2" s="514"/>
-      <c r="H2" s="514"/>
-      <c r="I2" s="514"/>
-      <c r="J2" s="514"/>
+      <c r="A2" s="546"/>
+      <c r="B2" s="546"/>
+      <c r="C2" s="546"/>
+      <c r="D2" s="546"/>
+      <c r="E2" s="546"/>
+      <c r="F2" s="546"/>
+      <c r="G2" s="546"/>
+      <c r="H2" s="546"/>
+      <c r="I2" s="546"/>
+      <c r="J2" s="546"/>
       <c r="K2" s="377"/>
       <c r="L2" s="377"/>
       <c r="M2" s="377"/>
@@ -46970,8 +46994,8 @@
       <c r="O2" s="379"/>
       <c r="Q2" s="10"/>
       <c r="R2" s="11"/>
-      <c r="S2" s="558"/>
-      <c r="T2" s="558"/>
+      <c r="S2" s="566"/>
+      <c r="T2" s="566"/>
       <c r="U2" s="14"/>
       <c r="V2" s="15"/>
       <c r="W2" s="16"/>
@@ -47016,10 +47040,10 @@
       <c r="N3" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="517" t="s">
+      <c r="O3" s="549" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="518"/>
+      <c r="P3" s="550"/>
       <c r="Q3" s="30" t="s">
         <v>16</v>
       </c>
@@ -47098,13 +47122,13 @@
       <c r="S4" s="51">
         <v>11200</v>
       </c>
-      <c r="T4" s="589" t="s">
+      <c r="T4" s="519" t="s">
         <v>415</v>
       </c>
-      <c r="U4" s="590" t="s">
+      <c r="U4" s="520" t="s">
         <v>560</v>
       </c>
-      <c r="V4" s="591">
+      <c r="V4" s="521">
         <v>4640</v>
       </c>
       <c r="W4" s="55" t="s">
@@ -47171,13 +47195,13 @@
       <c r="S5" s="51">
         <v>11200</v>
       </c>
-      <c r="T5" s="589" t="s">
+      <c r="T5" s="519" t="s">
         <v>404</v>
       </c>
-      <c r="U5" s="590" t="s">
+      <c r="U5" s="520" t="s">
         <v>560</v>
       </c>
-      <c r="V5" s="591">
+      <c r="V5" s="521">
         <v>4640</v>
       </c>
       <c r="W5" s="68" t="s">
@@ -47244,13 +47268,13 @@
       <c r="S6" s="51">
         <v>11200</v>
       </c>
-      <c r="T6" s="589" t="s">
+      <c r="T6" s="519" t="s">
         <v>405</v>
       </c>
-      <c r="U6" s="590" t="s">
+      <c r="U6" s="520" t="s">
         <v>560</v>
       </c>
-      <c r="V6" s="591">
+      <c r="V6" s="521">
         <v>4640</v>
       </c>
       <c r="W6" s="53" t="s">
@@ -47317,13 +47341,13 @@
       <c r="S7" s="51">
         <v>0</v>
       </c>
-      <c r="T7" s="589" t="s">
+      <c r="T7" s="519" t="s">
         <v>405</v>
       </c>
-      <c r="U7" s="590" t="s">
+      <c r="U7" s="520" t="s">
         <v>560</v>
       </c>
-      <c r="V7" s="591">
+      <c r="V7" s="521">
         <v>0</v>
       </c>
       <c r="W7" s="53" t="s">
@@ -47390,13 +47414,13 @@
       <c r="S8" s="51">
         <v>11200</v>
       </c>
-      <c r="T8" s="589" t="s">
+      <c r="T8" s="519" t="s">
         <v>406</v>
       </c>
-      <c r="U8" s="590" t="s">
+      <c r="U8" s="520" t="s">
         <v>560</v>
       </c>
-      <c r="V8" s="591">
+      <c r="V8" s="521">
         <v>4640</v>
       </c>
       <c r="W8" s="53" t="s">
@@ -47463,13 +47487,13 @@
       <c r="S9" s="51">
         <v>11200</v>
       </c>
-      <c r="T9" s="589" t="s">
+      <c r="T9" s="519" t="s">
         <v>425</v>
       </c>
-      <c r="U9" s="590" t="s">
+      <c r="U9" s="520" t="s">
         <v>560</v>
       </c>
-      <c r="V9" s="591">
+      <c r="V9" s="521">
         <v>4640</v>
       </c>
       <c r="W9" s="53" t="s">
@@ -47536,13 +47560,13 @@
       <c r="S10" s="51">
         <v>0</v>
       </c>
-      <c r="T10" s="589" t="s">
+      <c r="T10" s="519" t="s">
         <v>425</v>
       </c>
-      <c r="U10" s="590" t="s">
+      <c r="U10" s="520" t="s">
         <v>560</v>
       </c>
-      <c r="V10" s="591">
+      <c r="V10" s="521">
         <v>0</v>
       </c>
       <c r="W10" s="53" t="s">
@@ -47609,13 +47633,13 @@
       <c r="S11" s="51">
         <v>11200</v>
       </c>
-      <c r="T11" s="589" t="s">
+      <c r="T11" s="519" t="s">
         <v>417</v>
       </c>
-      <c r="U11" s="590" t="s">
+      <c r="U11" s="520" t="s">
         <v>560</v>
       </c>
-      <c r="V11" s="591">
+      <c r="V11" s="521">
         <v>4640</v>
       </c>
       <c r="W11" s="53" t="s">
@@ -47682,13 +47706,13 @@
       <c r="S12" s="51">
         <v>0</v>
       </c>
-      <c r="T12" s="589" t="s">
+      <c r="T12" s="519" t="s">
         <v>417</v>
       </c>
-      <c r="U12" s="590" t="s">
+      <c r="U12" s="520" t="s">
         <v>560</v>
       </c>
-      <c r="V12" s="591">
+      <c r="V12" s="521">
         <v>0</v>
       </c>
       <c r="W12" s="53" t="s">
@@ -47755,13 +47779,13 @@
       <c r="S13" s="51">
         <v>11200</v>
       </c>
-      <c r="T13" s="589" t="s">
+      <c r="T13" s="519" t="s">
         <v>418</v>
       </c>
-      <c r="U13" s="590" t="s">
+      <c r="U13" s="520" t="s">
         <v>560</v>
       </c>
-      <c r="V13" s="591">
+      <c r="V13" s="521">
         <v>4640</v>
       </c>
       <c r="W13" s="53" t="s">
@@ -47828,13 +47852,13 @@
       <c r="S14" s="51">
         <v>0</v>
       </c>
-      <c r="T14" s="589" t="s">
+      <c r="T14" s="519" t="s">
         <v>418</v>
       </c>
-      <c r="U14" s="590" t="s">
+      <c r="U14" s="520" t="s">
         <v>560</v>
       </c>
-      <c r="V14" s="591">
+      <c r="V14" s="521">
         <v>0</v>
       </c>
       <c r="W14" s="53" t="s">
@@ -47904,10 +47928,10 @@
       <c r="T15" s="92" t="s">
         <v>419</v>
       </c>
-      <c r="U15" s="590" t="s">
+      <c r="U15" s="520" t="s">
         <v>560</v>
       </c>
-      <c r="V15" s="591">
+      <c r="V15" s="521">
         <v>4640</v>
       </c>
       <c r="W15" s="53" t="s">
@@ -47977,10 +48001,10 @@
       <c r="T16" s="92" t="s">
         <v>419</v>
       </c>
-      <c r="U16" s="590" t="s">
+      <c r="U16" s="520" t="s">
         <v>560</v>
       </c>
-      <c r="V16" s="591">
+      <c r="V16" s="521">
         <v>0</v>
       </c>
       <c r="W16" s="53" t="s">
@@ -48050,10 +48074,10 @@
       <c r="T17" s="92" t="s">
         <v>438</v>
       </c>
-      <c r="U17" s="590" t="s">
+      <c r="U17" s="520" t="s">
         <v>560</v>
       </c>
-      <c r="V17" s="591">
+      <c r="V17" s="521">
         <v>4640</v>
       </c>
       <c r="W17" s="53" t="s">
@@ -48123,10 +48147,10 @@
       <c r="T18" s="92" t="s">
         <v>438</v>
       </c>
-      <c r="U18" s="590" t="s">
+      <c r="U18" s="520" t="s">
         <v>560</v>
       </c>
-      <c r="V18" s="591">
+      <c r="V18" s="521">
         <v>0</v>
       </c>
       <c r="W18" s="53" t="s">
@@ -49168,11 +49192,15 @@
       <c r="B33" s="93" t="s">
         <v>290</v>
       </c>
-      <c r="C33" s="59"/>
-      <c r="D33" s="60"/>
+      <c r="C33" s="59" t="s">
+        <v>561</v>
+      </c>
+      <c r="D33" s="60">
+        <v>54</v>
+      </c>
       <c r="E33" s="40">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1134054</v>
       </c>
       <c r="F33" s="61">
         <v>21001</v>
@@ -49238,8 +49266,12 @@
       <c r="B34" s="93" t="s">
         <v>32</v>
       </c>
-      <c r="C34" s="59"/>
-      <c r="D34" s="60"/>
+      <c r="C34" s="59" t="s">
+        <v>561</v>
+      </c>
+      <c r="D34" s="60">
+        <v>0</v>
+      </c>
       <c r="E34" s="40">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -49307,11 +49339,15 @@
       <c r="B35" s="93" t="s">
         <v>476</v>
       </c>
-      <c r="C35" s="59"/>
-      <c r="D35" s="60"/>
+      <c r="C35" s="59" t="s">
+        <v>562</v>
+      </c>
+      <c r="D35" s="60">
+        <v>54</v>
+      </c>
       <c r="E35" s="40">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1243728</v>
       </c>
       <c r="F35" s="61">
         <v>23032</v>
@@ -51052,8 +51088,8 @@
         <v>0</v>
       </c>
       <c r="K87" s="100"/>
-      <c r="L87" s="543"/>
-      <c r="M87" s="544"/>
+      <c r="L87" s="544"/>
+      <c r="M87" s="545"/>
       <c r="N87" s="48">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -51085,8 +51121,8 @@
         <v>0</v>
       </c>
       <c r="K88" s="100"/>
-      <c r="L88" s="543"/>
-      <c r="M88" s="544"/>
+      <c r="L88" s="544"/>
+      <c r="M88" s="545"/>
       <c r="N88" s="48">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -51289,8 +51325,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O94" s="539"/>
-      <c r="P94" s="535"/>
+      <c r="O94" s="528"/>
+      <c r="P94" s="538"/>
       <c r="Q94" s="164"/>
       <c r="R94" s="129"/>
       <c r="S94" s="180"/>
@@ -51322,8 +51358,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O95" s="540"/>
-      <c r="P95" s="536"/>
+      <c r="O95" s="529"/>
+      <c r="P95" s="539"/>
       <c r="Q95" s="164"/>
       <c r="R95" s="129"/>
       <c r="S95" s="180"/>
@@ -56715,11 +56751,11 @@
         <f t="shared" si="12"/>
         <v>#VALUE!</v>
       </c>
-      <c r="F259" s="537" t="s">
+      <c r="F259" s="540" t="s">
         <v>26</v>
       </c>
-      <c r="G259" s="537"/>
-      <c r="H259" s="538"/>
+      <c r="G259" s="540"/>
+      <c r="H259" s="541"/>
       <c r="I259" s="317">
         <f>SUM(I4:I258)</f>
         <v>476067.89999999997</v>
@@ -57303,22 +57339,22 @@
     <mergeCell ref="P94:P95"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr codeName="Hoja6">
     <tabColor rgb="FFCCFF33"/>
   </sheetPr>
   <dimension ref="A1:X292"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="10" ySplit="3" topLeftCell="V17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="10" ySplit="3" topLeftCell="V4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C27" sqref="C26:C27"/>
+      <selection pane="bottomRight" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -57326,8 +57362,8 @@
     <col min="1" max="1" width="49.28515625" customWidth="1"/>
     <col min="2" max="2" width="28.5703125" style="310" customWidth="1"/>
     <col min="3" max="3" width="13.85546875" style="310" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" style="310" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" style="331" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" style="310" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" style="331" customWidth="1"/>
     <col min="6" max="6" width="14.140625" style="311" customWidth="1"/>
     <col min="7" max="7" width="14.140625" style="312" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.28515625" style="315" customWidth="1"/>
@@ -57347,49 +57383,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="42.75" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A1" s="514" t="s">
+      <c r="A1" s="546" t="s">
         <v>482</v>
       </c>
-      <c r="B1" s="514"/>
-      <c r="C1" s="514"/>
-      <c r="D1" s="514"/>
-      <c r="E1" s="514"/>
-      <c r="F1" s="514"/>
-      <c r="G1" s="514"/>
-      <c r="H1" s="514"/>
-      <c r="I1" s="514"/>
-      <c r="J1" s="514"/>
+      <c r="B1" s="546"/>
+      <c r="C1" s="546"/>
+      <c r="D1" s="546"/>
+      <c r="E1" s="546"/>
+      <c r="F1" s="546"/>
+      <c r="G1" s="546"/>
+      <c r="H1" s="546"/>
+      <c r="I1" s="546"/>
+      <c r="J1" s="546"/>
       <c r="K1" s="375"/>
       <c r="L1" s="375"/>
       <c r="M1" s="375"/>
       <c r="N1" s="375"/>
       <c r="O1" s="376"/>
-      <c r="S1" s="557" t="s">
+      <c r="S1" s="565" t="s">
         <v>142</v>
       </c>
-      <c r="T1" s="557"/>
+      <c r="T1" s="565"/>
       <c r="U1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="V1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="W1" s="515" t="s">
+      <c r="W1" s="547" t="s">
         <v>2</v>
       </c>
-      <c r="X1" s="516"/>
+      <c r="X1" s="548"/>
     </row>
     <row r="2" spans="1:24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="514"/>
-      <c r="B2" s="514"/>
-      <c r="C2" s="514"/>
-      <c r="D2" s="514"/>
-      <c r="E2" s="514"/>
-      <c r="F2" s="514"/>
-      <c r="G2" s="514"/>
-      <c r="H2" s="514"/>
-      <c r="I2" s="514"/>
-      <c r="J2" s="514"/>
+      <c r="A2" s="546"/>
+      <c r="B2" s="546"/>
+      <c r="C2" s="546"/>
+      <c r="D2" s="546"/>
+      <c r="E2" s="546"/>
+      <c r="F2" s="546"/>
+      <c r="G2" s="546"/>
+      <c r="H2" s="546"/>
+      <c r="I2" s="546"/>
+      <c r="J2" s="546"/>
       <c r="K2" s="377"/>
       <c r="L2" s="377"/>
       <c r="M2" s="377"/>
@@ -57397,8 +57433,8 @@
       <c r="O2" s="379"/>
       <c r="Q2" s="10"/>
       <c r="R2" s="11"/>
-      <c r="S2" s="558"/>
-      <c r="T2" s="558"/>
+      <c r="S2" s="566"/>
+      <c r="T2" s="566"/>
       <c r="U2" s="14"/>
       <c r="V2" s="15"/>
       <c r="W2" s="16"/>
@@ -57443,10 +57479,10 @@
       <c r="N3" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="517" t="s">
+      <c r="O3" s="549" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="518"/>
+      <c r="P3" s="550"/>
       <c r="Q3" s="30" t="s">
         <v>16</v>
       </c>
@@ -57475,11 +57511,15 @@
       <c r="B4" s="37" t="s">
         <v>290</v>
       </c>
-      <c r="C4" s="38"/>
-      <c r="D4" s="39"/>
+      <c r="C4" s="38" t="s">
+        <v>563</v>
+      </c>
+      <c r="D4" s="39">
+        <v>54</v>
+      </c>
       <c r="E4" s="40">
         <f>D4*F4</f>
-        <v>0</v>
+        <v>1104570</v>
       </c>
       <c r="F4" s="41">
         <v>20455</v>
@@ -57536,8 +57576,12 @@
       <c r="B5" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="59"/>
-      <c r="D5" s="60"/>
+      <c r="C5" s="59" t="s">
+        <v>563</v>
+      </c>
+      <c r="D5" s="60">
+        <v>0</v>
+      </c>
       <c r="E5" s="40">
         <f t="shared" ref="E5:E40" si="2">D5*F5</f>
         <v>0</v>
@@ -57597,11 +57641,15 @@
       <c r="B6" s="58" t="s">
         <v>483</v>
       </c>
-      <c r="C6" s="59"/>
-      <c r="D6" s="60"/>
+      <c r="C6" s="59" t="s">
+        <v>564</v>
+      </c>
+      <c r="D6" s="60">
+        <v>55</v>
+      </c>
       <c r="E6" s="40">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1291400</v>
       </c>
       <c r="F6" s="61">
         <v>23480</v>
@@ -57662,8 +57710,12 @@
       <c r="B7" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="59"/>
-      <c r="D7" s="60"/>
+      <c r="C7" s="59" t="s">
+        <v>564</v>
+      </c>
+      <c r="D7" s="60">
+        <v>0</v>
+      </c>
       <c r="E7" s="40">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -57727,11 +57779,15 @@
       <c r="B8" s="58" t="s">
         <v>485</v>
       </c>
-      <c r="C8" s="59"/>
-      <c r="D8" s="60"/>
+      <c r="C8" s="59" t="s">
+        <v>565</v>
+      </c>
+      <c r="D8" s="60">
+        <v>57</v>
+      </c>
       <c r="E8" s="40">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1261980</v>
       </c>
       <c r="F8" s="61">
         <v>22140</v>
@@ -57792,8 +57848,12 @@
       <c r="B9" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="59"/>
-      <c r="D9" s="60"/>
+      <c r="C9" s="59" t="s">
+        <v>565</v>
+      </c>
+      <c r="D9" s="60">
+        <v>0</v>
+      </c>
       <c r="E9" s="40">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -59030,7 +59090,7 @@
       </c>
     </row>
     <row r="30" spans="1:24" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="588" t="s">
+      <c r="A30" s="518" t="s">
         <v>556</v>
       </c>
       <c r="B30" s="93" t="s">
@@ -60199,7 +60259,7 @@
         <f t="shared" si="1"/>
         <v>13114.4</v>
       </c>
-      <c r="O62" s="586" t="s">
+      <c r="O62" s="516" t="s">
         <v>159</v>
       </c>
       <c r="P62" s="507">
@@ -60249,10 +60309,10 @@
         <f>K63*I63</f>
         <v>9778</v>
       </c>
-      <c r="O63" s="584" t="s">
+      <c r="O63" s="588" t="s">
         <v>59</v>
       </c>
-      <c r="P63" s="580">
+      <c r="P63" s="590">
         <v>44742</v>
       </c>
       <c r="Q63" s="167"/>
@@ -60299,8 +60359,8 @@
         <f>K64*I64</f>
         <v>9454</v>
       </c>
-      <c r="O64" s="585"/>
-      <c r="P64" s="581"/>
+      <c r="O64" s="589"/>
+      <c r="P64" s="591"/>
       <c r="Q64" s="167"/>
       <c r="R64" s="129"/>
       <c r="S64" s="180"/>
@@ -60309,7 +60369,7 @@
       <c r="V64" s="54"/>
     </row>
     <row r="65" spans="1:22" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="583" t="s">
+      <c r="A65" s="515" t="s">
         <v>527</v>
       </c>
       <c r="B65" s="178" t="s">
@@ -60345,10 +60405,10 @@
         <f>K65*I65</f>
         <v>3964.9999199999997</v>
       </c>
-      <c r="O65" s="587" t="s">
+      <c r="O65" s="517" t="s">
         <v>546</v>
       </c>
-      <c r="P65" s="582">
+      <c r="P65" s="514">
         <v>44742</v>
       </c>
       <c r="Q65" s="167"/>
@@ -61021,8 +61081,8 @@
         <v>0</v>
       </c>
       <c r="K87" s="100"/>
-      <c r="L87" s="543"/>
-      <c r="M87" s="544"/>
+      <c r="L87" s="544"/>
+      <c r="M87" s="545"/>
       <c r="N87" s="48">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -61054,8 +61114,8 @@
         <v>0</v>
       </c>
       <c r="K88" s="100"/>
-      <c r="L88" s="543"/>
-      <c r="M88" s="544"/>
+      <c r="L88" s="544"/>
+      <c r="M88" s="545"/>
       <c r="N88" s="48">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -61258,8 +61318,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O94" s="539"/>
-      <c r="P94" s="535"/>
+      <c r="O94" s="528"/>
+      <c r="P94" s="538"/>
       <c r="Q94" s="164"/>
       <c r="R94" s="129"/>
       <c r="S94" s="180"/>
@@ -61291,8 +61351,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O95" s="540"/>
-      <c r="P95" s="536"/>
+      <c r="O95" s="529"/>
+      <c r="P95" s="539"/>
       <c r="Q95" s="164"/>
       <c r="R95" s="129"/>
       <c r="S95" s="180"/>
@@ -66684,11 +66744,11 @@
         <f t="shared" si="11"/>
         <v>#VALUE!</v>
       </c>
-      <c r="F259" s="537" t="s">
+      <c r="F259" s="540" t="s">
         <v>26</v>
       </c>
-      <c r="G259" s="537"/>
-      <c r="H259" s="538"/>
+      <c r="G259" s="540"/>
+      <c r="H259" s="541"/>
       <c r="I259" s="317">
         <f>SUM(I4:I258)</f>
         <v>390058.12237999996</v>
@@ -67261,7 +67321,7 @@
       <c r="V292"/>
     </row>
   </sheetData>
-  <sortState ref="A63:P65">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A63:P65">
     <sortCondition ref="C63:C65"/>
   </sortState>
   <mergeCells count="10">
@@ -67282,7 +67342,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr codeName="Hoja7"/>
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
CIERRE 12 jULIO 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #06  JUNIO 2022/ENTRADAS OBRADOR     J U N I O         2022.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #06  JUNIO 2022/ENTRADAS OBRADOR     J U N I O         2022.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1698" uniqueCount="575">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1700" uniqueCount="576">
   <si>
     <t>FECHA DE PAGO</t>
   </si>
@@ -1777,6 +1777,9 @@
   <si>
     <t>0350 A1</t>
   </si>
+  <si>
+    <t>0265 A1</t>
+  </si>
 </sst>
 </file>
 
@@ -3199,7 +3202,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="595">
+  <cellXfs count="592">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4610,6 +4613,78 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="54" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="31" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="31" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="11" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="11" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="26" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="26" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4643,83 +4718,11 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="11" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="11" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="22" fillId="11" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="22" fillId="11" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="26" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="26" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="31" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="31" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -4749,6 +4752,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="32" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="32" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4784,12 +4793,6 @@
     <xf numFmtId="1" fontId="18" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="32" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="32" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="11" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4819,15 +4822,6 @@
     </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="68" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="19" fillId="14" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="19" fillId="14" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -5158,18 +5152,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="42.75" thickBot="1" x14ac:dyDescent="0.7">
-      <c r="A1" s="522" t="s">
+      <c r="A1" s="546" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="522"/>
-      <c r="C1" s="522"/>
-      <c r="D1" s="522"/>
-      <c r="E1" s="522"/>
-      <c r="F1" s="522"/>
-      <c r="G1" s="522"/>
-      <c r="H1" s="522"/>
-      <c r="I1" s="522"/>
-      <c r="J1" s="522"/>
+      <c r="B1" s="546"/>
+      <c r="C1" s="546"/>
+      <c r="D1" s="546"/>
+      <c r="E1" s="546"/>
+      <c r="F1" s="546"/>
+      <c r="G1" s="546"/>
+      <c r="H1" s="546"/>
+      <c r="I1" s="546"/>
+      <c r="J1" s="546"/>
       <c r="K1" s="375"/>
       <c r="L1" s="375"/>
       <c r="M1" s="375"/>
@@ -5183,22 +5177,22 @@
       <c r="V1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="W1" s="523" t="s">
+      <c r="W1" s="547" t="s">
         <v>2</v>
       </c>
-      <c r="X1" s="524"/>
+      <c r="X1" s="548"/>
     </row>
     <row r="2" spans="1:24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="522"/>
-      <c r="B2" s="522"/>
-      <c r="C2" s="522"/>
-      <c r="D2" s="522"/>
-      <c r="E2" s="522"/>
-      <c r="F2" s="522"/>
-      <c r="G2" s="522"/>
-      <c r="H2" s="522"/>
-      <c r="I2" s="522"/>
-      <c r="J2" s="522"/>
+      <c r="A2" s="546"/>
+      <c r="B2" s="546"/>
+      <c r="C2" s="546"/>
+      <c r="D2" s="546"/>
+      <c r="E2" s="546"/>
+      <c r="F2" s="546"/>
+      <c r="G2" s="546"/>
+      <c r="H2" s="546"/>
+      <c r="I2" s="546"/>
+      <c r="J2" s="546"/>
       <c r="K2" s="377"/>
       <c r="L2" s="377"/>
       <c r="M2" s="377"/>
@@ -5252,10 +5246,10 @@
       <c r="N3" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="525" t="s">
+      <c r="O3" s="549" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="526"/>
+      <c r="P3" s="550"/>
       <c r="Q3" s="30" t="s">
         <v>16</v>
       </c>
@@ -5799,7 +5793,7 @@
       <c r="B12" s="58" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="527" t="s">
+      <c r="C12" s="551" t="s">
         <v>103</v>
       </c>
       <c r="D12" s="400"/>
@@ -5863,7 +5857,7 @@
       <c r="B13" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="528"/>
+      <c r="C13" s="552"/>
       <c r="D13" s="400"/>
       <c r="E13" s="401"/>
       <c r="F13" s="402">
@@ -7865,13 +7859,13 @@
       <c r="V55" s="160"/>
     </row>
     <row r="56" spans="1:24" s="161" customFormat="1" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="539" t="s">
+      <c r="A56" s="530" t="s">
         <v>41</v>
       </c>
       <c r="B56" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="C56" s="541" t="s">
+      <c r="C56" s="532" t="s">
         <v>110</v>
       </c>
       <c r="D56" s="150"/>
@@ -7882,7 +7876,7 @@
       <c r="G56" s="152">
         <v>44571</v>
       </c>
-      <c r="H56" s="533">
+      <c r="H56" s="534">
         <v>782</v>
       </c>
       <c r="I56" s="151">
@@ -7911,11 +7905,11 @@
       <c r="V56" s="160"/>
     </row>
     <row r="57" spans="1:24" s="161" customFormat="1" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="540"/>
+      <c r="A57" s="531"/>
       <c r="B57" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="C57" s="542"/>
+      <c r="C57" s="533"/>
       <c r="D57" s="150"/>
       <c r="E57" s="40"/>
       <c r="F57" s="151">
@@ -7924,7 +7918,7 @@
       <c r="G57" s="152">
         <v>44571</v>
       </c>
-      <c r="H57" s="534"/>
+      <c r="H57" s="535"/>
       <c r="I57" s="151">
         <v>319</v>
       </c>
@@ -7951,13 +7945,13 @@
       <c r="V57" s="160"/>
     </row>
     <row r="58" spans="1:24" s="161" customFormat="1" ht="29.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="539" t="s">
+      <c r="A58" s="530" t="s">
         <v>41</v>
       </c>
       <c r="B58" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="C58" s="541" t="s">
+      <c r="C58" s="532" t="s">
         <v>129</v>
       </c>
       <c r="D58" s="150"/>
@@ -7968,7 +7962,7 @@
       <c r="G58" s="152">
         <v>44578</v>
       </c>
-      <c r="H58" s="533">
+      <c r="H58" s="534">
         <v>810</v>
       </c>
       <c r="I58" s="151">
@@ -7987,10 +7981,10 @@
         <f t="shared" si="1"/>
         <v>75875.8</v>
       </c>
-      <c r="O58" s="535" t="s">
+      <c r="O58" s="536" t="s">
         <v>59</v>
       </c>
-      <c r="P58" s="537">
+      <c r="P58" s="557">
         <v>44606</v>
       </c>
       <c r="Q58" s="128"/>
@@ -8001,11 +7995,11 @@
       <c r="V58" s="160"/>
     </row>
     <row r="59" spans="1:24" s="161" customFormat="1" ht="29.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="540"/>
+      <c r="A59" s="531"/>
       <c r="B59" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="C59" s="542"/>
+      <c r="C59" s="533"/>
       <c r="D59" s="150"/>
       <c r="E59" s="40"/>
       <c r="F59" s="151">
@@ -8014,7 +8008,7 @@
       <c r="G59" s="152">
         <v>44578</v>
       </c>
-      <c r="H59" s="534"/>
+      <c r="H59" s="535"/>
       <c r="I59" s="151">
         <v>220</v>
       </c>
@@ -8031,8 +8025,8 @@
         <f t="shared" si="1"/>
         <v>22440</v>
       </c>
-      <c r="O59" s="536"/>
-      <c r="P59" s="538"/>
+      <c r="O59" s="537"/>
+      <c r="P59" s="558"/>
       <c r="Q59" s="128"/>
       <c r="R59" s="158"/>
       <c r="S59" s="92"/>
@@ -8041,13 +8035,13 @@
       <c r="V59" s="160"/>
     </row>
     <row r="60" spans="1:24" s="161" customFormat="1" ht="48.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="531" t="s">
+      <c r="A60" s="555" t="s">
         <v>41</v>
       </c>
       <c r="B60" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="C60" s="529" t="s">
+      <c r="C60" s="553" t="s">
         <v>109</v>
       </c>
       <c r="D60" s="163"/>
@@ -8061,7 +8055,7 @@
       <c r="G60" s="152">
         <v>44585</v>
       </c>
-      <c r="H60" s="533">
+      <c r="H60" s="534">
         <v>800</v>
       </c>
       <c r="I60" s="151">
@@ -8080,10 +8074,10 @@
         <f t="shared" si="1"/>
         <v>151187.4</v>
       </c>
-      <c r="O60" s="535" t="s">
+      <c r="O60" s="536" t="s">
         <v>59</v>
       </c>
-      <c r="P60" s="537">
+      <c r="P60" s="557">
         <v>44594</v>
       </c>
       <c r="Q60" s="164"/>
@@ -8096,11 +8090,11 @@
       <c r="X60"/>
     </row>
     <row r="61" spans="1:24" ht="26.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="532"/>
+      <c r="A61" s="556"/>
       <c r="B61" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="C61" s="530"/>
+      <c r="C61" s="554"/>
       <c r="D61" s="165"/>
       <c r="E61" s="40">
         <f t="shared" si="2"/>
@@ -8112,7 +8106,7 @@
       <c r="G61" s="152">
         <v>44585</v>
       </c>
-      <c r="H61" s="534"/>
+      <c r="H61" s="535"/>
       <c r="I61" s="151">
         <v>231.6</v>
       </c>
@@ -8129,8 +8123,8 @@
         <f t="shared" si="1"/>
         <v>23623.200000000001</v>
       </c>
-      <c r="O61" s="536"/>
-      <c r="P61" s="538"/>
+      <c r="O61" s="537"/>
+      <c r="P61" s="558"/>
       <c r="Q61" s="164"/>
       <c r="R61" s="129"/>
       <c r="S61" s="92"/>
@@ -8196,7 +8190,7 @@
       <c r="B63" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="C63" s="555"/>
+      <c r="C63" s="524"/>
       <c r="D63" s="163"/>
       <c r="E63" s="40">
         <f t="shared" si="2"/>
@@ -8204,7 +8198,7 @@
       </c>
       <c r="F63" s="151"/>
       <c r="G63" s="152"/>
-      <c r="H63" s="557"/>
+      <c r="H63" s="526"/>
       <c r="I63" s="151"/>
       <c r="J63" s="45">
         <f t="shared" si="0"/>
@@ -8233,7 +8227,7 @@
       <c r="B64" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="C64" s="556"/>
+      <c r="C64" s="525"/>
       <c r="D64" s="168"/>
       <c r="E64" s="40">
         <f t="shared" si="2"/>
@@ -8241,7 +8235,7 @@
       </c>
       <c r="F64" s="151"/>
       <c r="G64" s="152"/>
-      <c r="H64" s="558"/>
+      <c r="H64" s="527"/>
       <c r="I64" s="151"/>
       <c r="J64" s="45">
         <f t="shared" si="0"/>
@@ -8419,8 +8413,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O68" s="547"/>
-      <c r="P68" s="553"/>
+      <c r="O68" s="528"/>
+      <c r="P68" s="522"/>
       <c r="Q68" s="164"/>
       <c r="R68" s="129"/>
       <c r="S68" s="180"/>
@@ -8454,8 +8448,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O69" s="548"/>
-      <c r="P69" s="554"/>
+      <c r="O69" s="529"/>
+      <c r="P69" s="523"/>
       <c r="Q69" s="164"/>
       <c r="R69" s="129"/>
       <c r="S69" s="180"/>
@@ -8945,8 +8939,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O82" s="547"/>
-      <c r="P82" s="549"/>
+      <c r="O82" s="528"/>
+      <c r="P82" s="542"/>
       <c r="Q82" s="164"/>
       <c r="R82" s="129"/>
       <c r="S82" s="180"/>
@@ -8978,8 +8972,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O83" s="548"/>
-      <c r="P83" s="550"/>
+      <c r="O83" s="529"/>
+      <c r="P83" s="543"/>
       <c r="Q83" s="164"/>
       <c r="R83" s="129"/>
       <c r="S83" s="180"/>
@@ -9011,8 +9005,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O84" s="547"/>
-      <c r="P84" s="549"/>
+      <c r="O84" s="528"/>
+      <c r="P84" s="542"/>
       <c r="Q84" s="164"/>
       <c r="R84" s="158"/>
       <c r="S84" s="180"/>
@@ -9044,8 +9038,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O85" s="548"/>
-      <c r="P85" s="550"/>
+      <c r="O85" s="529"/>
+      <c r="P85" s="543"/>
       <c r="Q85" s="164"/>
       <c r="R85" s="158"/>
       <c r="S85" s="180"/>
@@ -9203,8 +9197,8 @@
         <v>0</v>
       </c>
       <c r="K90" s="100"/>
-      <c r="L90" s="551"/>
-      <c r="M90" s="552"/>
+      <c r="L90" s="544"/>
+      <c r="M90" s="545"/>
       <c r="N90" s="77">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -9236,8 +9230,8 @@
         <v>0</v>
       </c>
       <c r="K91" s="100"/>
-      <c r="L91" s="551"/>
-      <c r="M91" s="552"/>
+      <c r="L91" s="544"/>
+      <c r="M91" s="545"/>
       <c r="N91" s="77">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -9440,8 +9434,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O97" s="547"/>
-      <c r="P97" s="543"/>
+      <c r="O97" s="528"/>
+      <c r="P97" s="538"/>
       <c r="Q97" s="164"/>
       <c r="R97" s="129"/>
       <c r="S97" s="180"/>
@@ -9473,8 +9467,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O98" s="548"/>
-      <c r="P98" s="544"/>
+      <c r="O98" s="529"/>
+      <c r="P98" s="539"/>
       <c r="Q98" s="164"/>
       <c r="R98" s="129"/>
       <c r="S98" s="180"/>
@@ -14866,11 +14860,11 @@
         <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
-      <c r="F262" s="545" t="s">
+      <c r="F262" s="540" t="s">
         <v>26</v>
       </c>
-      <c r="G262" s="545"/>
-      <c r="H262" s="546"/>
+      <c r="G262" s="540"/>
+      <c r="H262" s="541"/>
       <c r="I262" s="317">
         <f>SUM(I4:I261)</f>
         <v>426245.47000000003</v>
@@ -15444,22 +15438,6 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="P68:P69"/>
-    <mergeCell ref="C63:C64"/>
-    <mergeCell ref="H63:H64"/>
-    <mergeCell ref="O68:O69"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="C58:C59"/>
-    <mergeCell ref="H58:H59"/>
-    <mergeCell ref="O58:O59"/>
-    <mergeCell ref="P97:P98"/>
-    <mergeCell ref="F262:H262"/>
-    <mergeCell ref="O82:O83"/>
-    <mergeCell ref="P82:P83"/>
-    <mergeCell ref="O84:O85"/>
-    <mergeCell ref="P84:P85"/>
-    <mergeCell ref="L90:M91"/>
-    <mergeCell ref="O97:O98"/>
     <mergeCell ref="A1:J2"/>
     <mergeCell ref="W1:X1"/>
     <mergeCell ref="O3:P3"/>
@@ -15473,6 +15451,22 @@
     <mergeCell ref="C56:C57"/>
     <mergeCell ref="H56:H57"/>
     <mergeCell ref="P58:P59"/>
+    <mergeCell ref="P97:P98"/>
+    <mergeCell ref="F262:H262"/>
+    <mergeCell ref="O82:O83"/>
+    <mergeCell ref="P82:P83"/>
+    <mergeCell ref="O84:O85"/>
+    <mergeCell ref="P84:P85"/>
+    <mergeCell ref="L90:M91"/>
+    <mergeCell ref="O97:O98"/>
+    <mergeCell ref="P68:P69"/>
+    <mergeCell ref="C63:C64"/>
+    <mergeCell ref="H63:H64"/>
+    <mergeCell ref="O68:O69"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="H58:H59"/>
+    <mergeCell ref="O58:O59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -15516,18 +15510,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="42.75" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A1" s="522" t="s">
+      <c r="A1" s="546" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="522"/>
-      <c r="C1" s="522"/>
-      <c r="D1" s="522"/>
-      <c r="E1" s="522"/>
-      <c r="F1" s="522"/>
-      <c r="G1" s="522"/>
-      <c r="H1" s="522"/>
-      <c r="I1" s="522"/>
-      <c r="J1" s="522"/>
+      <c r="B1" s="546"/>
+      <c r="C1" s="546"/>
+      <c r="D1" s="546"/>
+      <c r="E1" s="546"/>
+      <c r="F1" s="546"/>
+      <c r="G1" s="546"/>
+      <c r="H1" s="546"/>
+      <c r="I1" s="546"/>
+      <c r="J1" s="546"/>
       <c r="K1" s="375"/>
       <c r="L1" s="375"/>
       <c r="M1" s="375"/>
@@ -15543,22 +15537,22 @@
       <c r="V1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="W1" s="523" t="s">
+      <c r="W1" s="547" t="s">
         <v>2</v>
       </c>
-      <c r="X1" s="524"/>
+      <c r="X1" s="548"/>
     </row>
     <row r="2" spans="1:24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="522"/>
-      <c r="B2" s="522"/>
-      <c r="C2" s="522"/>
-      <c r="D2" s="522"/>
-      <c r="E2" s="522"/>
-      <c r="F2" s="522"/>
-      <c r="G2" s="522"/>
-      <c r="H2" s="522"/>
-      <c r="I2" s="522"/>
-      <c r="J2" s="522"/>
+      <c r="A2" s="546"/>
+      <c r="B2" s="546"/>
+      <c r="C2" s="546"/>
+      <c r="D2" s="546"/>
+      <c r="E2" s="546"/>
+      <c r="F2" s="546"/>
+      <c r="G2" s="546"/>
+      <c r="H2" s="546"/>
+      <c r="I2" s="546"/>
+      <c r="J2" s="546"/>
       <c r="K2" s="377"/>
       <c r="L2" s="377"/>
       <c r="M2" s="377"/>
@@ -15612,10 +15606,10 @@
       <c r="N3" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="525" t="s">
+      <c r="O3" s="549" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="526"/>
+      <c r="P3" s="550"/>
       <c r="Q3" s="30" t="s">
         <v>16</v>
       </c>
@@ -18257,7 +18251,7 @@
       <c r="B55" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="C55" s="541" t="s">
+      <c r="C55" s="532" t="s">
         <v>160</v>
       </c>
       <c r="D55" s="150"/>
@@ -18268,7 +18262,7 @@
       <c r="G55" s="152">
         <v>44599</v>
       </c>
-      <c r="H55" s="557" t="s">
+      <c r="H55" s="526" t="s">
         <v>161</v>
       </c>
       <c r="I55" s="151">
@@ -18301,7 +18295,7 @@
       <c r="B56" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="C56" s="542"/>
+      <c r="C56" s="533"/>
       <c r="D56" s="163"/>
       <c r="E56" s="40"/>
       <c r="F56" s="151">
@@ -18310,7 +18304,7 @@
       <c r="G56" s="152">
         <v>44599</v>
       </c>
-      <c r="H56" s="558"/>
+      <c r="H56" s="527"/>
       <c r="I56" s="151">
         <v>194.4</v>
       </c>
@@ -18356,7 +18350,7 @@
       <c r="G57" s="152">
         <v>44606</v>
       </c>
-      <c r="H57" s="557" t="s">
+      <c r="H57" s="526" t="s">
         <v>163</v>
       </c>
       <c r="I57" s="151">
@@ -18375,10 +18369,10 @@
         <f t="shared" si="1"/>
         <v>35776</v>
       </c>
-      <c r="O57" s="547" t="s">
+      <c r="O57" s="528" t="s">
         <v>59</v>
       </c>
-      <c r="P57" s="553">
+      <c r="P57" s="522">
         <v>44620</v>
       </c>
       <c r="Q57" s="164"/>
@@ -18402,7 +18396,7 @@
       <c r="G58" s="152">
         <v>44606</v>
       </c>
-      <c r="H58" s="558"/>
+      <c r="H58" s="527"/>
       <c r="I58" s="151">
         <v>627.60209999999995</v>
       </c>
@@ -18446,7 +18440,7 @@
       <c r="G59" s="152">
         <v>44613</v>
       </c>
-      <c r="H59" s="557" t="s">
+      <c r="H59" s="526" t="s">
         <v>225</v>
       </c>
       <c r="I59" s="151">
@@ -18490,7 +18484,7 @@
       <c r="E60" s="40"/>
       <c r="F60" s="151"/>
       <c r="G60" s="152"/>
-      <c r="H60" s="558"/>
+      <c r="H60" s="527"/>
       <c r="I60" s="151"/>
       <c r="J60" s="45">
         <f t="shared" si="0"/>
@@ -19153,8 +19147,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O79" s="547"/>
-      <c r="P79" s="549"/>
+      <c r="O79" s="528"/>
+      <c r="P79" s="542"/>
       <c r="Q79" s="164"/>
       <c r="R79" s="129"/>
       <c r="S79" s="180"/>
@@ -19183,8 +19177,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O80" s="548"/>
-      <c r="P80" s="550"/>
+      <c r="O80" s="529"/>
+      <c r="P80" s="543"/>
       <c r="Q80" s="164"/>
       <c r="R80" s="129"/>
       <c r="S80" s="180"/>
@@ -19213,8 +19207,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O81" s="547"/>
-      <c r="P81" s="549"/>
+      <c r="O81" s="528"/>
+      <c r="P81" s="542"/>
       <c r="Q81" s="164"/>
       <c r="R81" s="158"/>
       <c r="S81" s="180"/>
@@ -19246,8 +19240,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O82" s="548"/>
-      <c r="P82" s="550"/>
+      <c r="O82" s="529"/>
+      <c r="P82" s="543"/>
       <c r="Q82" s="164"/>
       <c r="R82" s="158"/>
       <c r="S82" s="180"/>
@@ -19405,8 +19399,8 @@
         <v>0</v>
       </c>
       <c r="K87" s="100"/>
-      <c r="L87" s="551"/>
-      <c r="M87" s="552"/>
+      <c r="L87" s="544"/>
+      <c r="M87" s="545"/>
       <c r="N87" s="77">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -19438,8 +19432,8 @@
         <v>0</v>
       </c>
       <c r="K88" s="100"/>
-      <c r="L88" s="551"/>
-      <c r="M88" s="552"/>
+      <c r="L88" s="544"/>
+      <c r="M88" s="545"/>
       <c r="N88" s="77">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -19642,8 +19636,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O94" s="547"/>
-      <c r="P94" s="543"/>
+      <c r="O94" s="528"/>
+      <c r="P94" s="538"/>
       <c r="Q94" s="164"/>
       <c r="R94" s="129"/>
       <c r="S94" s="180"/>
@@ -19675,8 +19669,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O95" s="548"/>
-      <c r="P95" s="544"/>
+      <c r="O95" s="529"/>
+      <c r="P95" s="539"/>
       <c r="Q95" s="164"/>
       <c r="R95" s="129"/>
       <c r="S95" s="180"/>
@@ -25068,11 +25062,11 @@
         <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
-      <c r="F259" s="545" t="s">
+      <c r="F259" s="540" t="s">
         <v>26</v>
       </c>
-      <c r="G259" s="545"/>
-      <c r="H259" s="546"/>
+      <c r="G259" s="540"/>
+      <c r="H259" s="541"/>
       <c r="I259" s="317">
         <f>SUM(I4:I258)</f>
         <v>387207.97210000001</v>
@@ -25646,6 +25640,12 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="F259:H259"/>
+    <mergeCell ref="O81:O82"/>
+    <mergeCell ref="P81:P82"/>
+    <mergeCell ref="L87:M88"/>
+    <mergeCell ref="O94:O95"/>
+    <mergeCell ref="P94:P95"/>
     <mergeCell ref="O79:O80"/>
     <mergeCell ref="P79:P80"/>
     <mergeCell ref="A1:J2"/>
@@ -25661,12 +25661,6 @@
     <mergeCell ref="C55:C56"/>
     <mergeCell ref="A55:A56"/>
     <mergeCell ref="H55:H56"/>
-    <mergeCell ref="F259:H259"/>
-    <mergeCell ref="O81:O82"/>
-    <mergeCell ref="P81:P82"/>
-    <mergeCell ref="L87:M88"/>
-    <mergeCell ref="O94:O95"/>
-    <mergeCell ref="P94:P95"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -25713,18 +25707,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="42.75" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A1" s="522" t="s">
+      <c r="A1" s="546" t="s">
         <v>189</v>
       </c>
-      <c r="B1" s="522"/>
-      <c r="C1" s="522"/>
-      <c r="D1" s="522"/>
-      <c r="E1" s="522"/>
-      <c r="F1" s="522"/>
-      <c r="G1" s="522"/>
-      <c r="H1" s="522"/>
-      <c r="I1" s="522"/>
-      <c r="J1" s="522"/>
+      <c r="B1" s="546"/>
+      <c r="C1" s="546"/>
+      <c r="D1" s="546"/>
+      <c r="E1" s="546"/>
+      <c r="F1" s="546"/>
+      <c r="G1" s="546"/>
+      <c r="H1" s="546"/>
+      <c r="I1" s="546"/>
+      <c r="J1" s="546"/>
       <c r="K1" s="375"/>
       <c r="L1" s="375"/>
       <c r="M1" s="375"/>
@@ -25740,22 +25734,22 @@
       <c r="V1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="W1" s="523" t="s">
+      <c r="W1" s="547" t="s">
         <v>2</v>
       </c>
-      <c r="X1" s="524"/>
+      <c r="X1" s="548"/>
     </row>
     <row r="2" spans="1:24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="522"/>
-      <c r="B2" s="522"/>
-      <c r="C2" s="522"/>
-      <c r="D2" s="522"/>
-      <c r="E2" s="522"/>
-      <c r="F2" s="522"/>
-      <c r="G2" s="522"/>
-      <c r="H2" s="522"/>
-      <c r="I2" s="522"/>
-      <c r="J2" s="522"/>
+      <c r="A2" s="546"/>
+      <c r="B2" s="546"/>
+      <c r="C2" s="546"/>
+      <c r="D2" s="546"/>
+      <c r="E2" s="546"/>
+      <c r="F2" s="546"/>
+      <c r="G2" s="546"/>
+      <c r="H2" s="546"/>
+      <c r="I2" s="546"/>
+      <c r="J2" s="546"/>
       <c r="K2" s="377"/>
       <c r="L2" s="377"/>
       <c r="M2" s="377"/>
@@ -25809,10 +25803,10 @@
       <c r="N3" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="525" t="s">
+      <c r="O3" s="549" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="526"/>
+      <c r="P3" s="550"/>
       <c r="Q3" s="30" t="s">
         <v>16</v>
       </c>
@@ -29026,7 +29020,7 @@
       <c r="B55" s="438" t="s">
         <v>24</v>
       </c>
-      <c r="C55" s="541" t="s">
+      <c r="C55" s="532" t="s">
         <v>229</v>
       </c>
       <c r="D55" s="439"/>
@@ -29037,7 +29031,7 @@
       <c r="G55" s="152">
         <v>44627</v>
       </c>
-      <c r="H55" s="570" t="s">
+      <c r="H55" s="572" t="s">
         <v>230</v>
       </c>
       <c r="I55" s="151">
@@ -29056,10 +29050,10 @@
         <f t="shared" si="1"/>
         <v>18886.399999999998</v>
       </c>
-      <c r="O55" s="547" t="s">
+      <c r="O55" s="528" t="s">
         <v>59</v>
       </c>
-      <c r="P55" s="553">
+      <c r="P55" s="522">
         <v>44645</v>
       </c>
       <c r="Q55" s="128"/>
@@ -29070,11 +29064,11 @@
       <c r="V55" s="160"/>
     </row>
     <row r="56" spans="1:24" s="161" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="569"/>
+      <c r="A56" s="571"/>
       <c r="B56" s="438" t="s">
         <v>24</v>
       </c>
-      <c r="C56" s="542"/>
+      <c r="C56" s="533"/>
       <c r="D56" s="440"/>
       <c r="E56" s="60"/>
       <c r="F56" s="151">
@@ -29083,7 +29077,7 @@
       <c r="G56" s="152">
         <v>44627</v>
       </c>
-      <c r="H56" s="571"/>
+      <c r="H56" s="573"/>
       <c r="I56" s="151">
         <v>967</v>
       </c>
@@ -29100,8 +29094,8 @@
         <f t="shared" si="1"/>
         <v>92832</v>
       </c>
-      <c r="O56" s="548"/>
-      <c r="P56" s="554"/>
+      <c r="O56" s="529"/>
+      <c r="P56" s="523"/>
       <c r="Q56" s="164"/>
       <c r="R56" s="158"/>
       <c r="S56" s="92"/>
@@ -29162,13 +29156,13 @@
       <c r="V57" s="54"/>
     </row>
     <row r="58" spans="1:24" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="531" t="s">
+      <c r="A58" s="555" t="s">
         <v>41</v>
       </c>
       <c r="B58" s="170" t="s">
         <v>24</v>
       </c>
-      <c r="C58" s="580" t="s">
+      <c r="C58" s="569" t="s">
         <v>319</v>
       </c>
       <c r="D58" s="165"/>
@@ -29179,7 +29173,7 @@
       <c r="G58" s="152">
         <v>44648</v>
       </c>
-      <c r="H58" s="578" t="s">
+      <c r="H58" s="580" t="s">
         <v>315</v>
       </c>
       <c r="I58" s="151">
@@ -29198,10 +29192,10 @@
         <f t="shared" si="1"/>
         <v>35255.600000000006</v>
       </c>
-      <c r="O58" s="535" t="s">
+      <c r="O58" s="536" t="s">
         <v>59</v>
       </c>
-      <c r="P58" s="537">
+      <c r="P58" s="557">
         <v>44662</v>
       </c>
       <c r="Q58" s="164"/>
@@ -29212,11 +29206,11 @@
       <c r="V58" s="54"/>
     </row>
     <row r="59" spans="1:24" s="161" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="532"/>
+      <c r="A59" s="556"/>
       <c r="B59" s="170" t="s">
         <v>23</v>
       </c>
-      <c r="C59" s="581"/>
+      <c r="C59" s="570"/>
       <c r="D59" s="163"/>
       <c r="E59" s="60"/>
       <c r="F59" s="151">
@@ -29225,7 +29219,7 @@
       <c r="G59" s="152">
         <v>44648</v>
       </c>
-      <c r="H59" s="579"/>
+      <c r="H59" s="581"/>
       <c r="I59" s="151">
         <v>719</v>
       </c>
@@ -29242,8 +29236,8 @@
         <f t="shared" si="1"/>
         <v>69024</v>
       </c>
-      <c r="O59" s="536"/>
-      <c r="P59" s="538"/>
+      <c r="O59" s="537"/>
+      <c r="P59" s="558"/>
       <c r="Q59" s="164"/>
       <c r="R59" s="158"/>
       <c r="S59" s="92"/>
@@ -29316,13 +29310,13 @@
       <c r="V61" s="54"/>
     </row>
     <row r="62" spans="1:24" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A62" s="572" t="s">
+      <c r="A62" s="574" t="s">
         <v>106</v>
       </c>
       <c r="B62" s="178" t="s">
         <v>237</v>
       </c>
-      <c r="C62" s="574" t="s">
+      <c r="C62" s="576" t="s">
         <v>238</v>
       </c>
       <c r="D62" s="168"/>
@@ -29333,7 +29327,7 @@
       <c r="G62" s="152">
         <v>44622</v>
       </c>
-      <c r="H62" s="576">
+      <c r="H62" s="578">
         <v>37162</v>
       </c>
       <c r="I62" s="151">
@@ -29352,10 +29346,10 @@
         <f t="shared" si="1"/>
         <v>7782.5999999999995</v>
       </c>
-      <c r="O62" s="547" t="s">
+      <c r="O62" s="528" t="s">
         <v>61</v>
       </c>
-      <c r="P62" s="553">
+      <c r="P62" s="522">
         <v>44643</v>
       </c>
       <c r="Q62" s="164"/>
@@ -29366,11 +29360,11 @@
       <c r="V62" s="54"/>
     </row>
     <row r="63" spans="1:24" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A63" s="573"/>
+      <c r="A63" s="575"/>
       <c r="B63" s="178" t="s">
         <v>239</v>
       </c>
-      <c r="C63" s="575"/>
+      <c r="C63" s="577"/>
       <c r="D63" s="168"/>
       <c r="E63" s="60"/>
       <c r="F63" s="151">
@@ -29379,7 +29373,7 @@
       <c r="G63" s="152">
         <v>44622</v>
       </c>
-      <c r="H63" s="577"/>
+      <c r="H63" s="579"/>
       <c r="I63" s="151">
         <v>204.8</v>
       </c>
@@ -29396,8 +29390,8 @@
         <f t="shared" si="1"/>
         <v>16998.400000000001</v>
       </c>
-      <c r="O63" s="548"/>
-      <c r="P63" s="554"/>
+      <c r="O63" s="529"/>
+      <c r="P63" s="523"/>
       <c r="Q63" s="164"/>
       <c r="R63" s="129"/>
       <c r="S63" s="92"/>
@@ -29876,8 +29870,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O79" s="547"/>
-      <c r="P79" s="549"/>
+      <c r="O79" s="528"/>
+      <c r="P79" s="542"/>
       <c r="Q79" s="164"/>
       <c r="R79" s="129"/>
       <c r="S79" s="180"/>
@@ -29906,8 +29900,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O80" s="548"/>
-      <c r="P80" s="550"/>
+      <c r="O80" s="529"/>
+      <c r="P80" s="543"/>
       <c r="Q80" s="164"/>
       <c r="R80" s="129"/>
       <c r="S80" s="180"/>
@@ -29936,8 +29930,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O81" s="547"/>
-      <c r="P81" s="549"/>
+      <c r="O81" s="528"/>
+      <c r="P81" s="542"/>
       <c r="Q81" s="164"/>
       <c r="R81" s="158"/>
       <c r="S81" s="180"/>
@@ -29969,8 +29963,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O82" s="548"/>
-      <c r="P82" s="550"/>
+      <c r="O82" s="529"/>
+      <c r="P82" s="543"/>
       <c r="Q82" s="164"/>
       <c r="R82" s="158"/>
       <c r="S82" s="180"/>
@@ -30128,8 +30122,8 @@
         <v>0</v>
       </c>
       <c r="K87" s="100"/>
-      <c r="L87" s="551"/>
-      <c r="M87" s="552"/>
+      <c r="L87" s="544"/>
+      <c r="M87" s="545"/>
       <c r="N87" s="48">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -30161,8 +30155,8 @@
         <v>0</v>
       </c>
       <c r="K88" s="100"/>
-      <c r="L88" s="551"/>
-      <c r="M88" s="552"/>
+      <c r="L88" s="544"/>
+      <c r="M88" s="545"/>
       <c r="N88" s="48">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -30365,8 +30359,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O94" s="547"/>
-      <c r="P94" s="543"/>
+      <c r="O94" s="528"/>
+      <c r="P94" s="538"/>
       <c r="Q94" s="164"/>
       <c r="R94" s="129"/>
       <c r="S94" s="180"/>
@@ -30398,8 +30392,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O95" s="548"/>
-      <c r="P95" s="544"/>
+      <c r="O95" s="529"/>
+      <c r="P95" s="539"/>
       <c r="Q95" s="164"/>
       <c r="R95" s="129"/>
       <c r="S95" s="180"/>
@@ -35791,11 +35785,11 @@
         <f t="shared" si="10"/>
         <v>#VALUE!</v>
       </c>
-      <c r="F259" s="545" t="s">
+      <c r="F259" s="540" t="s">
         <v>26</v>
       </c>
-      <c r="G259" s="545"/>
-      <c r="H259" s="546"/>
+      <c r="G259" s="540"/>
+      <c r="H259" s="541"/>
       <c r="I259" s="317">
         <f>SUM(I4:I258)</f>
         <v>517031.52999999991</v>
@@ -36369,17 +36363,6 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="O58:O59"/>
-    <mergeCell ref="P58:P59"/>
-    <mergeCell ref="C58:C59"/>
-    <mergeCell ref="O94:O95"/>
-    <mergeCell ref="P94:P95"/>
-    <mergeCell ref="F259:H259"/>
-    <mergeCell ref="O79:O80"/>
-    <mergeCell ref="P79:P80"/>
-    <mergeCell ref="O81:O82"/>
-    <mergeCell ref="P81:P82"/>
     <mergeCell ref="A1:J2"/>
     <mergeCell ref="S1:T2"/>
     <mergeCell ref="W1:X1"/>
@@ -36396,6 +36379,17 @@
     <mergeCell ref="O62:O63"/>
     <mergeCell ref="P62:P63"/>
     <mergeCell ref="H58:H59"/>
+    <mergeCell ref="F259:H259"/>
+    <mergeCell ref="O79:O80"/>
+    <mergeCell ref="P79:P80"/>
+    <mergeCell ref="O81:O82"/>
+    <mergeCell ref="P81:P82"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="O58:O59"/>
+    <mergeCell ref="P58:P59"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="O94:O95"/>
+    <mergeCell ref="P94:P95"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -36442,18 +36436,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="42.75" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A1" s="522" t="s">
+      <c r="A1" s="546" t="s">
         <v>288</v>
       </c>
-      <c r="B1" s="522"/>
-      <c r="C1" s="522"/>
-      <c r="D1" s="522"/>
-      <c r="E1" s="522"/>
-      <c r="F1" s="522"/>
-      <c r="G1" s="522"/>
-      <c r="H1" s="522"/>
-      <c r="I1" s="522"/>
-      <c r="J1" s="522"/>
+      <c r="B1" s="546"/>
+      <c r="C1" s="546"/>
+      <c r="D1" s="546"/>
+      <c r="E1" s="546"/>
+      <c r="F1" s="546"/>
+      <c r="G1" s="546"/>
+      <c r="H1" s="546"/>
+      <c r="I1" s="546"/>
+      <c r="J1" s="546"/>
       <c r="K1" s="375"/>
       <c r="L1" s="375"/>
       <c r="M1" s="375"/>
@@ -36469,22 +36463,22 @@
       <c r="V1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="W1" s="523" t="s">
+      <c r="W1" s="547" t="s">
         <v>2</v>
       </c>
-      <c r="X1" s="524"/>
+      <c r="X1" s="548"/>
     </row>
     <row r="2" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="522"/>
-      <c r="B2" s="522"/>
-      <c r="C2" s="522"/>
-      <c r="D2" s="522"/>
-      <c r="E2" s="522"/>
-      <c r="F2" s="522"/>
-      <c r="G2" s="522"/>
-      <c r="H2" s="522"/>
-      <c r="I2" s="522"/>
-      <c r="J2" s="522"/>
+      <c r="A2" s="546"/>
+      <c r="B2" s="546"/>
+      <c r="C2" s="546"/>
+      <c r="D2" s="546"/>
+      <c r="E2" s="546"/>
+      <c r="F2" s="546"/>
+      <c r="G2" s="546"/>
+      <c r="H2" s="546"/>
+      <c r="I2" s="546"/>
+      <c r="J2" s="546"/>
       <c r="K2" s="377"/>
       <c r="L2" s="377"/>
       <c r="M2" s="377"/>
@@ -36538,10 +36532,10 @@
       <c r="N3" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="525" t="s">
+      <c r="O3" s="549" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="526"/>
+      <c r="P3" s="550"/>
       <c r="Q3" s="30" t="s">
         <v>16</v>
       </c>
@@ -39929,7 +39923,7 @@
       <c r="B64" s="178" t="s">
         <v>464</v>
       </c>
-      <c r="C64" s="574" t="s">
+      <c r="C64" s="576" t="s">
         <v>465</v>
       </c>
       <c r="D64" s="171"/>
@@ -39973,11 +39967,11 @@
       <c r="V64" s="54"/>
     </row>
     <row r="65" spans="1:22" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="569"/>
+      <c r="A65" s="571"/>
       <c r="B65" s="178" t="s">
         <v>240</v>
       </c>
-      <c r="C65" s="575"/>
+      <c r="C65" s="577"/>
       <c r="D65" s="171"/>
       <c r="E65" s="60"/>
       <c r="F65" s="151">
@@ -40423,8 +40417,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O79" s="547"/>
-      <c r="P79" s="549"/>
+      <c r="O79" s="528"/>
+      <c r="P79" s="542"/>
       <c r="Q79" s="164"/>
       <c r="R79" s="129"/>
       <c r="S79" s="180"/>
@@ -40453,8 +40447,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O80" s="548"/>
-      <c r="P80" s="550"/>
+      <c r="O80" s="529"/>
+      <c r="P80" s="543"/>
       <c r="Q80" s="164"/>
       <c r="R80" s="129"/>
       <c r="S80" s="180"/>
@@ -40483,8 +40477,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O81" s="547"/>
-      <c r="P81" s="549"/>
+      <c r="O81" s="528"/>
+      <c r="P81" s="542"/>
       <c r="Q81" s="164"/>
       <c r="R81" s="158"/>
       <c r="S81" s="180"/>
@@ -40516,8 +40510,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O82" s="548"/>
-      <c r="P82" s="550"/>
+      <c r="O82" s="529"/>
+      <c r="P82" s="543"/>
       <c r="Q82" s="164"/>
       <c r="R82" s="158"/>
       <c r="S82" s="180"/>
@@ -40675,8 +40669,8 @@
         <v>0</v>
       </c>
       <c r="K87" s="100"/>
-      <c r="L87" s="551"/>
-      <c r="M87" s="552"/>
+      <c r="L87" s="544"/>
+      <c r="M87" s="545"/>
       <c r="N87" s="48">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -40708,8 +40702,8 @@
         <v>0</v>
       </c>
       <c r="K88" s="100"/>
-      <c r="L88" s="551"/>
-      <c r="M88" s="552"/>
+      <c r="L88" s="544"/>
+      <c r="M88" s="545"/>
       <c r="N88" s="48">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -40912,8 +40906,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O94" s="547"/>
-      <c r="P94" s="543"/>
+      <c r="O94" s="528"/>
+      <c r="P94" s="538"/>
       <c r="Q94" s="164"/>
       <c r="R94" s="129"/>
       <c r="S94" s="180"/>
@@ -40945,8 +40939,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O95" s="548"/>
-      <c r="P95" s="544"/>
+      <c r="O95" s="529"/>
+      <c r="P95" s="539"/>
       <c r="Q95" s="164"/>
       <c r="R95" s="129"/>
       <c r="S95" s="180"/>
@@ -46338,11 +46332,11 @@
         <f t="shared" si="11"/>
         <v>#VALUE!</v>
       </c>
-      <c r="F259" s="545" t="s">
+      <c r="F259" s="540" t="s">
         <v>26</v>
       </c>
-      <c r="G259" s="545"/>
-      <c r="H259" s="546"/>
+      <c r="G259" s="540"/>
+      <c r="H259" s="541"/>
       <c r="I259" s="317">
         <f>SUM(I4:I258)</f>
         <v>491966.85000000003</v>
@@ -46916,6 +46910,12 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="F259:H259"/>
+    <mergeCell ref="O81:O82"/>
+    <mergeCell ref="P81:P82"/>
+    <mergeCell ref="L87:M88"/>
+    <mergeCell ref="O94:O95"/>
+    <mergeCell ref="P94:P95"/>
     <mergeCell ref="W1:X1"/>
     <mergeCell ref="O3:P3"/>
     <mergeCell ref="O79:O80"/>
@@ -46927,12 +46927,6 @@
     <mergeCell ref="H64:H65"/>
     <mergeCell ref="O64:O65"/>
     <mergeCell ref="P64:P65"/>
-    <mergeCell ref="F259:H259"/>
-    <mergeCell ref="O81:O82"/>
-    <mergeCell ref="P81:P82"/>
-    <mergeCell ref="L87:M88"/>
-    <mergeCell ref="O94:O95"/>
-    <mergeCell ref="P94:P95"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -46979,18 +46973,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="42.75" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A1" s="522" t="s">
+      <c r="A1" s="546" t="s">
         <v>402</v>
       </c>
-      <c r="B1" s="522"/>
-      <c r="C1" s="522"/>
-      <c r="D1" s="522"/>
-      <c r="E1" s="522"/>
-      <c r="F1" s="522"/>
-      <c r="G1" s="522"/>
-      <c r="H1" s="522"/>
-      <c r="I1" s="522"/>
-      <c r="J1" s="522"/>
+      <c r="B1" s="546"/>
+      <c r="C1" s="546"/>
+      <c r="D1" s="546"/>
+      <c r="E1" s="546"/>
+      <c r="F1" s="546"/>
+      <c r="G1" s="546"/>
+      <c r="H1" s="546"/>
+      <c r="I1" s="546"/>
+      <c r="J1" s="546"/>
       <c r="K1" s="375"/>
       <c r="L1" s="375"/>
       <c r="M1" s="375"/>
@@ -47006,22 +47000,22 @@
       <c r="V1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="W1" s="523" t="s">
+      <c r="W1" s="547" t="s">
         <v>2</v>
       </c>
-      <c r="X1" s="524"/>
+      <c r="X1" s="548"/>
     </row>
     <row r="2" spans="1:24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="522"/>
-      <c r="B2" s="522"/>
-      <c r="C2" s="522"/>
-      <c r="D2" s="522"/>
-      <c r="E2" s="522"/>
-      <c r="F2" s="522"/>
-      <c r="G2" s="522"/>
-      <c r="H2" s="522"/>
-      <c r="I2" s="522"/>
-      <c r="J2" s="522"/>
+      <c r="A2" s="546"/>
+      <c r="B2" s="546"/>
+      <c r="C2" s="546"/>
+      <c r="D2" s="546"/>
+      <c r="E2" s="546"/>
+      <c r="F2" s="546"/>
+      <c r="G2" s="546"/>
+      <c r="H2" s="546"/>
+      <c r="I2" s="546"/>
+      <c r="J2" s="546"/>
       <c r="K2" s="377"/>
       <c r="L2" s="377"/>
       <c r="M2" s="377"/>
@@ -47075,10 +47069,10 @@
       <c r="N3" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="525" t="s">
+      <c r="O3" s="549" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="526"/>
+      <c r="P3" s="550"/>
       <c r="Q3" s="30" t="s">
         <v>16</v>
       </c>
@@ -51123,8 +51117,8 @@
         <v>0</v>
       </c>
       <c r="K87" s="100"/>
-      <c r="L87" s="551"/>
-      <c r="M87" s="552"/>
+      <c r="L87" s="544"/>
+      <c r="M87" s="545"/>
       <c r="N87" s="48">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -51156,8 +51150,8 @@
         <v>0</v>
       </c>
       <c r="K88" s="100"/>
-      <c r="L88" s="551"/>
-      <c r="M88" s="552"/>
+      <c r="L88" s="544"/>
+      <c r="M88" s="545"/>
       <c r="N88" s="48">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -51360,8 +51354,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O94" s="547"/>
-      <c r="P94" s="543"/>
+      <c r="O94" s="528"/>
+      <c r="P94" s="538"/>
       <c r="Q94" s="164"/>
       <c r="R94" s="129"/>
       <c r="S94" s="180"/>
@@ -51393,8 +51387,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O95" s="548"/>
-      <c r="P95" s="544"/>
+      <c r="O95" s="529"/>
+      <c r="P95" s="539"/>
       <c r="Q95" s="164"/>
       <c r="R95" s="129"/>
       <c r="S95" s="180"/>
@@ -56786,11 +56780,11 @@
         <f t="shared" si="12"/>
         <v>#VALUE!</v>
       </c>
-      <c r="F259" s="545" t="s">
+      <c r="F259" s="540" t="s">
         <v>26</v>
       </c>
-      <c r="G259" s="545"/>
-      <c r="H259" s="546"/>
+      <c r="G259" s="540"/>
+      <c r="H259" s="541"/>
       <c r="I259" s="317">
         <f>SUM(I4:I258)</f>
         <v>476067.89999999997</v>
@@ -57389,7 +57383,7 @@
       <pane xSplit="10" ySplit="3" topLeftCell="K13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D28" sqref="D28"/>
+      <selection pane="bottomRight" activeCell="C18" sqref="C18:E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -57418,18 +57412,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="42.75" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A1" s="522" t="s">
+      <c r="A1" s="546" t="s">
         <v>482</v>
       </c>
-      <c r="B1" s="522"/>
-      <c r="C1" s="522"/>
-      <c r="D1" s="522"/>
-      <c r="E1" s="522"/>
-      <c r="F1" s="522"/>
-      <c r="G1" s="522"/>
-      <c r="H1" s="522"/>
-      <c r="I1" s="522"/>
-      <c r="J1" s="522"/>
+      <c r="B1" s="546"/>
+      <c r="C1" s="546"/>
+      <c r="D1" s="546"/>
+      <c r="E1" s="546"/>
+      <c r="F1" s="546"/>
+      <c r="G1" s="546"/>
+      <c r="H1" s="546"/>
+      <c r="I1" s="546"/>
+      <c r="J1" s="546"/>
       <c r="K1" s="375"/>
       <c r="L1" s="375"/>
       <c r="M1" s="375"/>
@@ -57445,22 +57439,22 @@
       <c r="V1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="W1" s="523" t="s">
+      <c r="W1" s="547" t="s">
         <v>2</v>
       </c>
-      <c r="X1" s="524"/>
+      <c r="X1" s="548"/>
     </row>
     <row r="2" spans="1:24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="522"/>
-      <c r="B2" s="522"/>
-      <c r="C2" s="522"/>
-      <c r="D2" s="522"/>
-      <c r="E2" s="522"/>
-      <c r="F2" s="522"/>
-      <c r="G2" s="522"/>
-      <c r="H2" s="522"/>
-      <c r="I2" s="522"/>
-      <c r="J2" s="522"/>
+      <c r="A2" s="546"/>
+      <c r="B2" s="546"/>
+      <c r="C2" s="546"/>
+      <c r="D2" s="546"/>
+      <c r="E2" s="546"/>
+      <c r="F2" s="546"/>
+      <c r="G2" s="546"/>
+      <c r="H2" s="546"/>
+      <c r="I2" s="546"/>
+      <c r="J2" s="546"/>
       <c r="K2" s="377"/>
       <c r="L2" s="377"/>
       <c r="M2" s="377"/>
@@ -57514,10 +57508,10 @@
       <c r="N3" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="525" t="s">
+      <c r="O3" s="549" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="526"/>
+      <c r="P3" s="550"/>
       <c r="Q3" s="30" t="s">
         <v>16</v>
       </c>
@@ -58499,11 +58493,15 @@
       <c r="B18" s="58" t="s">
         <v>72</v>
       </c>
-      <c r="C18" s="592"/>
-      <c r="D18" s="593"/>
-      <c r="E18" s="594">
+      <c r="C18" s="59" t="s">
+        <v>575</v>
+      </c>
+      <c r="D18" s="60">
+        <v>59</v>
+      </c>
+      <c r="E18" s="40">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1384140</v>
       </c>
       <c r="F18" s="61">
         <v>23460</v>
@@ -58560,9 +58558,13 @@
       <c r="B19" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="592"/>
-      <c r="D19" s="593"/>
-      <c r="E19" s="594">
+      <c r="C19" s="59" t="s">
+        <v>575</v>
+      </c>
+      <c r="D19" s="60">
+        <v>0</v>
+      </c>
+      <c r="E19" s="40">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -61176,8 +61178,8 @@
         <v>0</v>
       </c>
       <c r="K87" s="100"/>
-      <c r="L87" s="551"/>
-      <c r="M87" s="552"/>
+      <c r="L87" s="544"/>
+      <c r="M87" s="545"/>
       <c r="N87" s="48">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -61209,8 +61211,8 @@
         <v>0</v>
       </c>
       <c r="K88" s="100"/>
-      <c r="L88" s="551"/>
-      <c r="M88" s="552"/>
+      <c r="L88" s="544"/>
+      <c r="M88" s="545"/>
       <c r="N88" s="48">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -61413,8 +61415,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O94" s="547"/>
-      <c r="P94" s="543"/>
+      <c r="O94" s="528"/>
+      <c r="P94" s="538"/>
       <c r="Q94" s="164"/>
       <c r="R94" s="129"/>
       <c r="S94" s="180"/>
@@ -61446,8 +61448,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O95" s="548"/>
-      <c r="P95" s="544"/>
+      <c r="O95" s="529"/>
+      <c r="P95" s="539"/>
       <c r="Q95" s="164"/>
       <c r="R95" s="129"/>
       <c r="S95" s="180"/>
@@ -66839,11 +66841,11 @@
         <f t="shared" si="11"/>
         <v>#VALUE!</v>
       </c>
-      <c r="F259" s="545" t="s">
+      <c r="F259" s="540" t="s">
         <v>26</v>
       </c>
-      <c r="G259" s="545"/>
-      <c r="H259" s="546"/>
+      <c r="G259" s="540"/>
+      <c r="H259" s="541"/>
       <c r="I259" s="317">
         <f>SUM(I4:I258)</f>
         <v>390058.12237999996</v>

</xml_diff>